<commit_message>
Parâmetros de entrada pelo Excel
</commit_message>
<xml_diff>
--- a/ExoCTK_results.xlsx
+++ b/ExoCTK_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vikto\PycharmProjects\StarsAndExoplanets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D60CEB8-46AE-4D9A-864D-EC054705D836}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75E88085-A631-48CD-942B-86B0E1ADD4E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{3BF26EB7-DF66-4B75-A14D-202BA100B451}"/>
+    <workbookView xWindow="17175" yWindow="1005" windowWidth="19965" windowHeight="12990" xr2:uid="{3BF26EB7-DF66-4B75-A14D-202BA100B451}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="24">
   <si>
     <t>Teff</t>
   </si>
@@ -467,116 +467,116 @@
   <dimension ref="A1:R16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:P4"/>
+      <selection sqref="A1:P12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="N2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O2" s="1" t="s">
+      <c r="O2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="P2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>5385</v>
       </c>
@@ -593,42 +593,42 @@
         <v>16</v>
       </c>
       <c r="F3" s="2">
-        <v>0.42</v>
+        <v>0.42199999999999999</v>
       </c>
       <c r="G3" s="2">
-        <v>0.46800000000000003</v>
+        <v>0.4456</v>
       </c>
       <c r="H3" s="2">
-        <v>0.51600000000000001</v>
+        <v>0.46899999999999997</v>
       </c>
       <c r="I3" s="2">
-        <v>-0.153</v>
+        <v>-0.12</v>
       </c>
       <c r="J3" s="2">
-        <v>3.5000000000000003E-2</v>
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="K3" s="2">
-        <v>1.3069999999999999</v>
+        <v>1.159</v>
       </c>
       <c r="L3" s="2">
-        <v>8.2000000000000003E-2</v>
+        <v>7.8E-2</v>
       </c>
       <c r="M3" s="2">
-        <v>-0.379</v>
+        <v>-0.189</v>
       </c>
       <c r="N3" s="2">
-        <v>8.3000000000000004E-2</v>
+        <v>7.8E-2</v>
       </c>
       <c r="O3" s="2">
-        <v>0.01</v>
+        <v>-4.3999999999999997E-2</v>
       </c>
       <c r="P3" s="2">
-        <v>0.03</v>
+        <v>2.9000000000000001E-2</v>
       </c>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>5385</v>
       </c>
@@ -645,225 +645,481 @@
         <v>16</v>
       </c>
       <c r="F4" s="2">
+        <v>0.47</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0.49340000000000001</v>
+      </c>
+      <c r="H4" s="2">
         <v>0.51700000000000002</v>
       </c>
-      <c r="G4" s="2">
-        <v>0.56499999999999995</v>
-      </c>
-      <c r="H4" s="2">
-        <v>0.61299999999999999</v>
-      </c>
       <c r="I4" s="2">
-        <v>-6.3E-2</v>
+        <v>-0.16800000000000001</v>
       </c>
       <c r="J4" s="2">
-        <v>3.7999999999999999E-2</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="K4" s="2">
-        <v>1.262</v>
+        <v>1.381</v>
       </c>
       <c r="L4" s="2">
-        <v>8.8999999999999996E-2</v>
+        <v>8.5999999999999993E-2</v>
       </c>
       <c r="M4" s="2">
-        <v>-0.54600000000000004</v>
+        <v>-0.48</v>
       </c>
       <c r="N4" s="2">
-        <v>0.09</v>
+        <v>8.6999999999999994E-2</v>
       </c>
       <c r="O4" s="2">
-        <v>7.6999999999999999E-2</v>
+        <v>3.9E-2</v>
       </c>
       <c r="P4" s="2">
-        <v>3.3000000000000002E-2</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>5385</v>
+      </c>
+      <c r="B5" s="2">
+        <v>4.49</v>
+      </c>
+      <c r="C5" s="2">
+        <v>-0.05</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.51800000000000002</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0.54149999999999998</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0.56499999999999995</v>
+      </c>
+      <c r="I5" s="2">
+        <v>-5.5E-2</v>
+      </c>
+      <c r="J5" s="2">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="K5" s="2">
+        <v>1.202</v>
+      </c>
+      <c r="L5" s="2">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="M5" s="2">
+        <v>-0.44600000000000001</v>
+      </c>
+      <c r="N5" s="2">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="O5" s="2">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="P5" s="2">
+        <v>3.2000000000000001E-2</v>
+      </c>
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5385</v>
+      </c>
+      <c r="B6" s="2">
+        <v>4.49</v>
+      </c>
+      <c r="C6" s="2">
+        <v>-0.05</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.56599999999999995</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0.58940000000000003</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="I6" s="2">
+        <v>-7.4999999999999997E-2</v>
+      </c>
+      <c r="J6" s="2">
+        <v>3.9E-2</v>
+      </c>
+      <c r="K6" s="2">
+        <v>1.331</v>
+      </c>
+      <c r="L6" s="2">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="M6" s="2">
+        <v>-0.65600000000000003</v>
+      </c>
+      <c r="N6" s="2">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="O6" s="2">
+        <v>0.115</v>
+      </c>
+      <c r="P6" s="2">
+        <v>3.4000000000000002E-2</v>
+      </c>
       <c r="Q6" s="1"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>5385</v>
+      </c>
+      <c r="B7" s="2">
+        <v>4.49</v>
+      </c>
+      <c r="C7" s="2">
+        <v>-0.05</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.61399999999999999</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0.63770000000000004</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0.66100000000000003</v>
+      </c>
+      <c r="I7" s="2">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="J7" s="2">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="K7" s="2">
+        <v>1.1259999999999999</v>
+      </c>
+      <c r="L7" s="2">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="M7" s="2">
+        <v>-0.52800000000000002</v>
+      </c>
+      <c r="N7" s="2">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="O7" s="2">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="P7" s="2">
+        <v>3.3000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>5385</v>
+      </c>
+      <c r="B8" s="2">
+        <v>4.49</v>
+      </c>
+      <c r="C8" s="2">
+        <v>-0.05</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0.66200000000000003</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0.6855</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0.70899999999999996</v>
+      </c>
+      <c r="I8" s="2">
+        <v>6.3E-2</v>
+      </c>
+      <c r="J8" s="2">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="K8" s="2">
+        <v>1.016</v>
+      </c>
+      <c r="L8" s="2">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="M8" s="2">
+        <v>-0.48</v>
+      </c>
+      <c r="N8" s="2">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="O8" s="2">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="P8" s="2">
+        <v>3.6999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>5385</v>
+      </c>
+      <c r="B9" s="2">
+        <v>4.49</v>
+      </c>
+      <c r="C9" s="2">
+        <v>-0.05</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.71</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0.73340000000000005</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0.75700000000000001</v>
+      </c>
+      <c r="I9" s="2">
+        <v>0.111</v>
+      </c>
+      <c r="J9" s="2">
+        <v>0.04</v>
+      </c>
+      <c r="K9" s="2">
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="L9" s="2">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="M9" s="2">
+        <v>-0.41299999999999998</v>
+      </c>
+      <c r="N9" s="2">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="O9" s="2">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="P9" s="2">
+        <v>3.5000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>5385</v>
+      </c>
+      <c r="B10" s="2">
+        <v>4.49</v>
+      </c>
+      <c r="C10" s="2">
+        <v>-0.05</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0.75800000000000001</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0.78169999999999995</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0.80500000000000005</v>
+      </c>
+      <c r="I10" s="2">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="J10" s="2">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="K10" s="2">
+        <v>0.83499999999999996</v>
+      </c>
+      <c r="L10" s="2">
+        <v>0.107</v>
+      </c>
+      <c r="M10" s="2">
+        <v>-0.40600000000000003</v>
+      </c>
+      <c r="N10" s="2">
+        <v>0.108</v>
+      </c>
+      <c r="O10" s="2">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="P10" s="2">
+        <v>3.9E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>5385</v>
+      </c>
+      <c r="B11" s="2">
+        <v>4.49</v>
+      </c>
+      <c r="C11" s="2">
+        <v>-0.05</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0.80600000000000005</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0.8296</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0.85299999999999998</v>
+      </c>
+      <c r="I11" s="2">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="J11" s="2">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="K11" s="2">
+        <v>0.71299999999999997</v>
+      </c>
+      <c r="L11" s="2">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="M11" s="2">
+        <v>-0.311</v>
+      </c>
+      <c r="N11" s="2">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="O11" s="2">
+        <v>2.7E-2</v>
+      </c>
+      <c r="P11" s="2">
+        <v>3.2000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>5385</v>
+      </c>
+      <c r="B12" s="2">
+        <v>4.49</v>
+      </c>
+      <c r="C12" s="2">
+        <v>-0.05</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0.85399999999999998</v>
+      </c>
+      <c r="G12" s="2">
+        <v>0.87739999999999996</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0.90100000000000002</v>
+      </c>
+      <c r="I12" s="2">
+        <v>0.18</v>
+      </c>
+      <c r="J12" s="2">
+        <v>3.9E-2</v>
+      </c>
+      <c r="K12" s="2">
+        <v>0.71199999999999997</v>
+      </c>
+      <c r="L12" s="2">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="M12" s="2">
+        <v>-0.35299999999999998</v>
+      </c>
+      <c r="N12" s="2">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="O12" s="2">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="P12" s="2">
+        <v>3.4000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -881,7 +1137,7 @@
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>

</xml_diff>

<commit_message>
Testes GJ 1132 b
</commit_message>
<xml_diff>
--- a/ExoCTK_results.xlsx
+++ b/ExoCTK_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vikto\PycharmProjects\StarsAndExoplanets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FBB39B3-A535-4FEA-B2D6-7CB91ADDE6A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D5D975E-D72E-4FE2-94B4-BEEAA3FCA3A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{3BF26EB7-DF66-4B75-A14D-202BA100B451}"/>
+    <workbookView xWindow="3630" yWindow="1860" windowWidth="32805" windowHeight="11385" xr2:uid="{3BF26EB7-DF66-4B75-A14D-202BA100B451}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="24">
   <si>
     <t>Teff</t>
   </si>
@@ -101,13 +101,10 @@
     <t>4-parameter</t>
   </si>
   <si>
-    <t>---</t>
-  </si>
-  <si>
-    <t>----------</t>
-  </si>
-  <si>
-    <t>STIS.G430L</t>
+    <t>----------------</t>
+  </si>
+  <si>
+    <t>HST/WFC3_IR.G141</t>
   </si>
 </sst>
 </file>
@@ -148,9 +145,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -469,400 +467,866 @@
   <dimension ref="A1:R22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="N2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="P2" s="1" t="s">
+      <c r="P2" s="2" t="s">
         <v>18</v>
       </c>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>6380</v>
-      </c>
-      <c r="B3" s="1">
-        <v>4.3099999999999996</v>
-      </c>
-      <c r="C3" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="A3" s="2">
+        <v>3500</v>
+      </c>
+      <c r="B3" s="2">
+        <v>4.88</v>
+      </c>
+      <c r="C3" s="2">
+        <v>-0.12</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="1">
-        <v>0.4995</v>
-      </c>
-      <c r="G3" s="1">
-        <v>0.50539999999999996</v>
-      </c>
-      <c r="H3" s="1">
-        <v>0.51170000000000004</v>
-      </c>
-      <c r="I3" s="1">
-        <v>0.20899999999999999</v>
-      </c>
-      <c r="J3" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="K3" s="1">
-        <v>1.1759999999999999</v>
-      </c>
-      <c r="L3" s="1">
-        <v>0.11799999999999999</v>
-      </c>
-      <c r="M3" s="1">
-        <v>-0.86499999999999999</v>
-      </c>
-      <c r="N3" s="1">
-        <v>0.11899999999999999</v>
-      </c>
-      <c r="O3" s="1">
-        <v>0.26700000000000002</v>
-      </c>
-      <c r="P3" s="1">
-        <v>4.2999999999999997E-2</v>
+      <c r="E3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1.0409999999999999</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1.06</v>
+      </c>
+      <c r="H3" s="2">
+        <v>1.0780000000000001</v>
+      </c>
+      <c r="I3" s="2">
+        <v>1.397</v>
+      </c>
+      <c r="J3" s="2">
+        <v>1.6E-2</v>
+      </c>
+      <c r="K3" s="2">
+        <v>-1.292</v>
+      </c>
+      <c r="L3" s="2">
+        <v>3.9E-2</v>
+      </c>
+      <c r="M3" s="2">
+        <v>0.81899999999999995</v>
+      </c>
+      <c r="N3" s="2">
+        <v>3.9E-2</v>
+      </c>
+      <c r="O3" s="2">
+        <v>-0.22</v>
+      </c>
+      <c r="P3" s="2">
+        <v>1.4E-2</v>
       </c>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
+      <c r="A4" s="2">
+        <v>3500</v>
+      </c>
+      <c r="B4" s="2">
+        <v>4.88</v>
+      </c>
+      <c r="C4" s="2">
+        <v>-0.12</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1.0780000000000001</v>
+      </c>
+      <c r="G4" s="2">
+        <v>1.0980000000000001</v>
+      </c>
+      <c r="H4" s="2">
+        <v>1.117</v>
+      </c>
+      <c r="I4" s="2">
+        <v>1.337</v>
+      </c>
+      <c r="J4" s="2">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="K4" s="2">
+        <v>-1.222</v>
+      </c>
+      <c r="L4" s="2">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="M4" s="2">
+        <v>0.754</v>
+      </c>
+      <c r="N4" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="O4" s="2">
+        <v>-0.19500000000000001</v>
+      </c>
+      <c r="P4" s="2">
+        <v>2.1999999999999999E-2</v>
+      </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
+      <c r="A5" s="2">
+        <v>3500</v>
+      </c>
+      <c r="B5" s="2">
+        <v>4.88</v>
+      </c>
+      <c r="C5" s="2">
+        <v>-0.12</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1.117</v>
+      </c>
+      <c r="G5" s="2">
+        <v>1.1379999999999999</v>
+      </c>
+      <c r="H5" s="2">
+        <v>1.1579999999999999</v>
+      </c>
+      <c r="I5" s="2">
+        <v>1.2889999999999999</v>
+      </c>
+      <c r="J5" s="2">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="K5" s="2">
+        <v>-1.155</v>
+      </c>
+      <c r="L5" s="2">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="M5" s="2">
+        <v>0.69099999999999995</v>
+      </c>
+      <c r="N5" s="2">
+        <v>7.8E-2</v>
+      </c>
+      <c r="O5" s="2">
+        <v>-0.17100000000000001</v>
+      </c>
+      <c r="P5" s="2">
+        <v>2.8000000000000001E-2</v>
+      </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
+      <c r="A6" s="2">
+        <v>3500</v>
+      </c>
+      <c r="B6" s="2">
+        <v>4.88</v>
+      </c>
+      <c r="C6" s="2">
+        <v>-0.12</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1.1579999999999999</v>
+      </c>
+      <c r="G6" s="2">
+        <v>1.179</v>
+      </c>
+      <c r="H6" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="I6" s="2">
+        <v>1.23</v>
+      </c>
+      <c r="J6" s="2">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="K6" s="2">
+        <v>-1.056</v>
+      </c>
+      <c r="L6" s="2">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="M6" s="2">
+        <v>0.59099999999999997</v>
+      </c>
+      <c r="N6" s="2">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="O6" s="2">
+        <v>-0.13300000000000001</v>
+      </c>
+      <c r="P6" s="2">
+        <v>3.6999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>3500</v>
+      </c>
+      <c r="B7" s="2">
+        <v>4.88</v>
+      </c>
+      <c r="C7" s="2">
+        <v>-0.12</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="G7" s="2">
+        <v>1.222</v>
+      </c>
+      <c r="H7" s="2">
+        <v>1.2430000000000001</v>
+      </c>
+      <c r="I7" s="2">
+        <v>1.1339999999999999</v>
+      </c>
+      <c r="J7" s="2">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="K7" s="2">
+        <v>-0.86799999999999999</v>
+      </c>
+      <c r="L7" s="2">
+        <v>0.157</v>
+      </c>
+      <c r="M7" s="2">
+        <v>0.39700000000000002</v>
+      </c>
+      <c r="N7" s="2">
+        <v>0.158</v>
+      </c>
+      <c r="O7" s="2">
+        <v>-5.8000000000000003E-2</v>
+      </c>
+      <c r="P7" s="2">
+        <v>5.8000000000000003E-2</v>
+      </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
+      <c r="A8" s="2">
+        <v>3500</v>
+      </c>
+      <c r="B8" s="2">
+        <v>4.88</v>
+      </c>
+      <c r="C8" s="2">
+        <v>-0.12</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1.2430000000000001</v>
+      </c>
+      <c r="G8" s="2">
+        <v>1.266</v>
+      </c>
+      <c r="H8" s="2">
+        <v>1.288</v>
+      </c>
+      <c r="I8" s="2">
+        <v>1.139</v>
+      </c>
+      <c r="J8" s="2">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="K8" s="2">
+        <v>-0.92300000000000004</v>
+      </c>
+      <c r="L8" s="2">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="M8" s="2">
+        <v>0.46899999999999997</v>
+      </c>
+      <c r="N8" s="2">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="O8" s="2">
+        <v>-8.7999999999999995E-2</v>
+      </c>
+      <c r="P8" s="2">
+        <v>4.8000000000000001E-2</v>
+      </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
+      <c r="A9" s="2">
+        <v>3500</v>
+      </c>
+      <c r="B9" s="2">
+        <v>4.88</v>
+      </c>
+      <c r="C9" s="2">
+        <v>-0.12</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1.288</v>
+      </c>
+      <c r="G9" s="2">
+        <v>1.3120000000000001</v>
+      </c>
+      <c r="H9" s="2">
+        <v>1.335</v>
+      </c>
+      <c r="I9" s="2">
+        <v>1.121</v>
+      </c>
+      <c r="J9" s="2">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="K9" s="2">
+        <v>-0.92600000000000005</v>
+      </c>
+      <c r="L9" s="2">
+        <v>0.126</v>
+      </c>
+      <c r="M9" s="2">
+        <v>0.47899999999999998</v>
+      </c>
+      <c r="N9" s="2">
+        <v>0.127</v>
+      </c>
+      <c r="O9" s="2">
+        <v>-9.2999999999999999E-2</v>
+      </c>
+      <c r="P9" s="2">
+        <v>4.5999999999999999E-2</v>
+      </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
+      <c r="A10" s="2">
+        <v>3500</v>
+      </c>
+      <c r="B10" s="2">
+        <v>4.88</v>
+      </c>
+      <c r="C10" s="2">
+        <v>-0.12</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1.335</v>
+      </c>
+      <c r="G10" s="2">
+        <v>1.3580000000000001</v>
+      </c>
+      <c r="H10" s="2">
+        <v>1.383</v>
+      </c>
+      <c r="I10" s="2">
+        <v>1.0960000000000001</v>
+      </c>
+      <c r="J10" s="2">
+        <v>5.5E-2</v>
+      </c>
+      <c r="K10" s="2">
+        <v>-0.90200000000000002</v>
+      </c>
+      <c r="L10" s="2">
+        <v>0.129</v>
+      </c>
+      <c r="M10" s="2">
+        <v>0.46</v>
+      </c>
+      <c r="N10" s="2">
+        <v>0.13</v>
+      </c>
+      <c r="O10" s="2">
+        <v>-8.7999999999999995E-2</v>
+      </c>
+      <c r="P10" s="2">
+        <v>4.7E-2</v>
+      </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
+      <c r="A11" s="2">
+        <v>3500</v>
+      </c>
+      <c r="B11" s="2">
+        <v>4.88</v>
+      </c>
+      <c r="C11" s="2">
+        <v>-0.12</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="2">
+        <v>1.383</v>
+      </c>
+      <c r="G11" s="2">
+        <v>1.4079999999999999</v>
+      </c>
+      <c r="H11" s="2">
+        <v>1.4339999999999999</v>
+      </c>
+      <c r="I11" s="2">
+        <v>1.0609999999999999</v>
+      </c>
+      <c r="J11" s="2">
+        <v>5.5E-2</v>
+      </c>
+      <c r="K11" s="2">
+        <v>-0.86199999999999999</v>
+      </c>
+      <c r="L11" s="2">
+        <v>0.129</v>
+      </c>
+      <c r="M11" s="2">
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="N11" s="2">
+        <v>0.13</v>
+      </c>
+      <c r="O11" s="2">
+        <v>-7.8E-2</v>
+      </c>
+      <c r="P11" s="2">
+        <v>4.7E-2</v>
+      </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
+      <c r="A12" s="2">
+        <v>3500</v>
+      </c>
+      <c r="B12" s="2">
+        <v>4.88</v>
+      </c>
+      <c r="C12" s="2">
+        <v>-0.12</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1.4339999999999999</v>
+      </c>
+      <c r="G12" s="2">
+        <v>1.4590000000000001</v>
+      </c>
+      <c r="H12" s="2">
+        <v>1.4850000000000001</v>
+      </c>
+      <c r="I12" s="2">
+        <v>1.0389999999999999</v>
+      </c>
+      <c r="J12" s="2">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="K12" s="2">
+        <v>-0.83599999999999997</v>
+      </c>
+      <c r="L12" s="2">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="M12" s="2">
+        <v>0.40200000000000002</v>
+      </c>
+      <c r="N12" s="2">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="O12" s="2">
+        <v>-6.8000000000000005E-2</v>
+      </c>
+      <c r="P12" s="2">
+        <v>5.0999999999999997E-2</v>
+      </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
+      <c r="A13" s="2">
+        <v>3500</v>
+      </c>
+      <c r="B13" s="2">
+        <v>4.88</v>
+      </c>
+      <c r="C13" s="2">
+        <v>-0.12</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="2">
+        <v>1.4850000000000001</v>
+      </c>
+      <c r="G13" s="2">
+        <v>1.512</v>
+      </c>
+      <c r="H13" s="2">
+        <v>1.5389999999999999</v>
+      </c>
+      <c r="I13" s="2">
+        <v>1.028</v>
+      </c>
+      <c r="J13" s="2">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="K13" s="2">
+        <v>-0.85699999999999998</v>
+      </c>
+      <c r="L13" s="2">
+        <v>0.125</v>
+      </c>
+      <c r="M13" s="2">
+        <v>0.434</v>
+      </c>
+      <c r="N13" s="2">
+        <v>0.126</v>
+      </c>
+      <c r="O13" s="2">
+        <v>-8.2000000000000003E-2</v>
+      </c>
+      <c r="P13" s="2">
+        <v>4.5999999999999999E-2</v>
+      </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
+      <c r="A14" s="2">
+        <v>3500</v>
+      </c>
+      <c r="B14" s="2">
+        <v>4.88</v>
+      </c>
+      <c r="C14" s="2">
+        <v>-0.12</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="2">
+        <v>1.5389999999999999</v>
+      </c>
+      <c r="G14" s="2">
+        <v>1.5660000000000001</v>
+      </c>
+      <c r="H14" s="2">
+        <v>1.595</v>
+      </c>
+      <c r="I14" s="2">
+        <v>1.038</v>
+      </c>
+      <c r="J14" s="2">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="K14" s="2">
+        <v>-0.93</v>
+      </c>
+      <c r="L14" s="2">
+        <v>0.121</v>
+      </c>
+      <c r="M14" s="2">
+        <v>0.50900000000000001</v>
+      </c>
+      <c r="N14" s="2">
+        <v>0.122</v>
+      </c>
+      <c r="O14" s="2">
+        <v>-0.109</v>
+      </c>
+      <c r="P14" s="2">
+        <v>4.3999999999999997E-2</v>
+      </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
+      <c r="A15" s="2">
+        <v>3500</v>
+      </c>
+      <c r="B15" s="2">
+        <v>4.88</v>
+      </c>
+      <c r="C15" s="2">
+        <v>-0.12</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="2">
+        <v>1.595</v>
+      </c>
+      <c r="G15" s="2">
+        <v>1.623</v>
+      </c>
+      <c r="H15" s="2">
+        <v>1.6519999999999999</v>
+      </c>
+      <c r="I15" s="2">
+        <v>0.95499999999999996</v>
+      </c>
+      <c r="J15" s="2">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="K15" s="2">
+        <v>-0.84099999999999997</v>
+      </c>
+      <c r="L15" s="2">
+        <v>0.106</v>
+      </c>
+      <c r="M15" s="2">
+        <v>0.438</v>
+      </c>
+      <c r="N15" s="2">
+        <v>0.107</v>
+      </c>
+      <c r="O15" s="2">
+        <v>-8.5000000000000006E-2</v>
+      </c>
+      <c r="P15" s="2">
+        <v>3.9E-2</v>
+      </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
+      <c r="A16" s="2">
+        <v>3500</v>
+      </c>
+      <c r="B16" s="2">
+        <v>4.88</v>
+      </c>
+      <c r="C16" s="2">
+        <v>-0.12</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" s="2">
+        <v>1.6519999999999999</v>
+      </c>
+      <c r="G16" s="2">
+        <v>1.6819999999999999</v>
+      </c>
+      <c r="H16" s="2">
+        <v>1.712</v>
+      </c>
+      <c r="I16" s="2">
+        <v>0.86299999999999999</v>
+      </c>
+      <c r="J16" s="2">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="K16" s="2">
+        <v>-0.68300000000000005</v>
+      </c>
+      <c r="L16" s="2">
+        <v>0.113</v>
+      </c>
+      <c r="M16" s="2">
+        <v>0.29399999999999998</v>
+      </c>
+      <c r="N16" s="2">
+        <v>0.114</v>
+      </c>
+      <c r="O16" s="2">
+        <v>-3.5999999999999997E-2</v>
+      </c>
+      <c r="P16" s="2">
+        <v>4.2000000000000003E-2</v>
+      </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
-      <c r="O17" s="1"/>
-      <c r="P17" s="1"/>
+      <c r="A17" s="2">
+        <v>3500</v>
+      </c>
+      <c r="B17" s="2">
+        <v>4.88</v>
+      </c>
+      <c r="C17" s="2">
+        <v>-0.12</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" s="2">
+        <v>1.712</v>
+      </c>
+      <c r="G17" s="2">
+        <v>1.7430000000000001</v>
+      </c>
+      <c r="H17" s="2">
+        <v>1.7729999999999999</v>
+      </c>
+      <c r="I17" s="2">
+        <v>0.90100000000000002</v>
+      </c>
+      <c r="J17" s="2">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="K17" s="2">
+        <v>-0.79800000000000004</v>
+      </c>
+      <c r="L17" s="2">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="M17" s="2">
+        <v>0.41399999999999998</v>
+      </c>
+      <c r="N17" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="O17" s="2">
+        <v>-7.9000000000000001E-2</v>
+      </c>
+      <c r="P17" s="2">
+        <v>3.3000000000000002E-2</v>
+      </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>

</xml_diff>

<commit_message>
Testes com a implementação em C
As curvas no espectro de transmissão deram valores abaixo daqueles calculados anteriormente, sem a implementação em C.
</commit_message>
<xml_diff>
--- a/ExoCTK_results.xlsx
+++ b/ExoCTK_results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vikto\PycharmProjects\StarsAndExoplanets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48DFBA52-EB45-4F88-8593-4FCC320A9325}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4FFEEB0-D133-4741-A12A-B1C6364C8869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{3BF26EB7-DF66-4B75-A14D-202BA100B451}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="26">
   <si>
     <t>Teff</t>
   </si>
@@ -104,13 +104,10 @@
     <t>----------</t>
   </si>
   <si>
-    <t>---</t>
+    <t>STIS.G750L</t>
   </si>
   <si>
     <t>STIS.G430L</t>
-  </si>
-  <si>
-    <t>STIS.G750L</t>
   </si>
   <si>
     <t>HST/WFC3_IR.G141</t>
@@ -465,7 +462,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -476,7 +473,7 @@
   <dimension ref="A1:AH27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="AB22" sqref="AB22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,7 +538,7 @@
         <v>17</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>19</v>
@@ -587,13 +584,13 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>5172</v>
+        <v>6380</v>
       </c>
       <c r="B3" s="1">
-        <v>4.43</v>
+        <v>4.3099999999999996</v>
       </c>
       <c r="C3" s="1">
-        <v>0.35</v>
+        <v>0.2</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>21</v>
@@ -611,325 +608,581 @@
         <v>0.51170000000000004</v>
       </c>
       <c r="I3" s="1">
-        <v>0.247</v>
+        <v>0.22900000000000001</v>
       </c>
       <c r="J3" s="1">
-        <v>4.2000000000000003E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="K3" s="1">
-        <v>0.184</v>
+        <v>1.1180000000000001</v>
       </c>
       <c r="L3" s="1">
-        <v>0.1</v>
+        <v>0.121</v>
       </c>
       <c r="M3" s="1">
-        <v>0.79600000000000004</v>
+        <v>-0.755</v>
       </c>
       <c r="N3" s="1">
-        <v>0.10100000000000001</v>
+        <v>0.122</v>
       </c>
       <c r="O3" s="1">
-        <v>-0.36499999999999999</v>
+        <v>0.221</v>
       </c>
       <c r="P3" s="1">
-        <v>3.6999999999999998E-2</v>
+        <v>4.3999999999999997E-2</v>
       </c>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>5172</v>
+        <v>6380</v>
       </c>
       <c r="B4" s="1">
-        <v>4.43</v>
+        <v>4.3099999999999996</v>
       </c>
       <c r="C4" s="1">
-        <v>0.35</v>
+        <v>0.2</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F4" s="1">
-        <v>0.626</v>
+        <v>0.51200000000000001</v>
       </c>
       <c r="G4" s="1">
-        <v>0.67700000000000005</v>
+        <v>0.54249999999999998</v>
       </c>
       <c r="H4" s="1">
-        <v>0.72699999999999998</v>
+        <v>0.57299999999999995</v>
       </c>
       <c r="I4" s="1">
-        <v>0.378</v>
+        <v>0.157</v>
       </c>
       <c r="J4" s="1">
-        <v>3.1E-2</v>
+        <v>4.2999999999999997E-2</v>
       </c>
       <c r="K4" s="1">
-        <v>0.222</v>
+        <v>1.2869999999999999</v>
       </c>
       <c r="L4" s="1">
-        <v>7.3999999999999996E-2</v>
+        <v>0.10199999999999999</v>
       </c>
       <c r="M4" s="1">
-        <v>0.36099999999999999</v>
+        <v>-1.0229999999999999</v>
       </c>
       <c r="N4" s="1">
-        <v>7.3999999999999996E-2</v>
+        <v>0.10299999999999999</v>
       </c>
       <c r="O4" s="1">
-        <v>-0.21099999999999999</v>
+        <v>0.32400000000000001</v>
       </c>
       <c r="P4" s="1">
-        <v>2.7E-2</v>
+        <v>3.6999999999999998E-2</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>5172</v>
+        <v>6380</v>
       </c>
       <c r="B5" s="1">
-        <v>4.43</v>
+        <v>4.3099999999999996</v>
       </c>
       <c r="C5" s="1">
-        <v>0.35</v>
+        <v>0.2</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F5" s="1">
-        <v>1.04</v>
+        <v>0.52500000000000002</v>
       </c>
       <c r="G5" s="1">
-        <v>1.0980000000000001</v>
+        <v>0.57499999999999996</v>
       </c>
       <c r="H5" s="1">
-        <v>1.157</v>
+        <v>0.626</v>
       </c>
       <c r="I5" s="1">
-        <v>0.33800000000000002</v>
+        <v>0.125</v>
       </c>
       <c r="J5" s="1">
-        <v>3.2000000000000001E-2</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="K5" s="1">
-        <v>0.39900000000000002</v>
+        <v>1.395</v>
       </c>
       <c r="L5" s="1">
-        <v>7.5999999999999998E-2</v>
+        <v>0.09</v>
       </c>
       <c r="M5" s="1">
-        <v>-0.158</v>
+        <v>-1.196</v>
       </c>
       <c r="N5" s="1">
-        <v>7.6999999999999999E-2</v>
+        <v>9.0999999999999998E-2</v>
       </c>
       <c r="O5" s="1">
-        <v>2E-3</v>
+        <v>0.39</v>
       </c>
       <c r="P5" s="1">
-        <v>2.8000000000000001E-2</v>
+        <v>3.3000000000000002E-2</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>5172</v>
+        <v>6380</v>
       </c>
       <c r="B6" s="1">
-        <v>4.43</v>
+        <v>4.3099999999999996</v>
       </c>
       <c r="C6" s="1">
-        <v>0.35</v>
+        <v>0.2</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F6" s="1">
+        <v>0.626</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0.67700000000000005</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0.72699999999999998</v>
+      </c>
+      <c r="I6" s="1">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="J6" s="1">
+        <v>2.7E-2</v>
+      </c>
+      <c r="K6" s="1">
+        <v>1.4690000000000001</v>
+      </c>
+      <c r="L6" s="1">
+        <v>6.3E-2</v>
+      </c>
+      <c r="M6" s="1">
+        <v>-1.35</v>
+      </c>
+      <c r="N6" s="1">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="O6" s="1">
+        <v>0.44400000000000001</v>
+      </c>
+      <c r="P6" s="1">
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6380</v>
+      </c>
+      <c r="B7" s="1">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.72799999999999998</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0.77829999999999999</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0.82899999999999996</v>
+      </c>
+      <c r="I7" s="1">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="J7" s="1">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="K7" s="1">
+        <v>1.4139999999999999</v>
+      </c>
+      <c r="L7" s="1">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="M7" s="1">
+        <v>-1.3380000000000001</v>
+      </c>
+      <c r="N7" s="1">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="O7" s="1">
+        <v>0.44500000000000001</v>
+      </c>
+      <c r="P7" s="1">
+        <v>1.6E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>6380</v>
+      </c>
+      <c r="B8" s="1">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0.82899999999999996</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0.93</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="J8" s="1">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="K8" s="1">
+        <v>1.1180000000000001</v>
+      </c>
+      <c r="L8" s="1">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="M8" s="1">
+        <v>-1.069</v>
+      </c>
+      <c r="N8" s="1">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="O8" s="1">
+        <v>0.34499999999999997</v>
+      </c>
+      <c r="P8" s="1">
+        <v>1.9E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>6380</v>
+      </c>
+      <c r="B9" s="1">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0.93100000000000005</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0.98140000000000005</v>
+      </c>
+      <c r="H9" s="1">
+        <v>1.032</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="J9" s="1">
+        <v>1.6E-2</v>
+      </c>
+      <c r="K9" s="1">
+        <v>1.085</v>
+      </c>
+      <c r="L9" s="1">
+        <v>3.9E-2</v>
+      </c>
+      <c r="M9" s="1">
+        <v>-1.0760000000000001</v>
+      </c>
+      <c r="N9" s="1">
+        <v>3.9E-2</v>
+      </c>
+      <c r="O9" s="1">
+        <v>0.36299999999999999</v>
+      </c>
+      <c r="P9" s="1">
+        <v>1.4E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>6380</v>
+      </c>
+      <c r="B10" s="1">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1.04</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1.0980000000000001</v>
+      </c>
+      <c r="H10" s="1">
+        <v>1.157</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="K10" s="1">
+        <v>0.878</v>
+      </c>
+      <c r="L10" s="1">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="M10" s="1">
+        <v>-0.94899999999999995</v>
+      </c>
+      <c r="N10" s="1">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="O10" s="1">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="P10" s="1">
+        <v>1.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>6380</v>
+      </c>
+      <c r="B11" s="1">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1.1579999999999999</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1.222</v>
+      </c>
+      <c r="H11" s="1">
+        <v>1.288</v>
+      </c>
+      <c r="I11" s="1">
+        <v>0.35699999999999998</v>
+      </c>
+      <c r="J11" s="1">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="K11" s="1">
+        <v>0.66300000000000003</v>
+      </c>
+      <c r="L11" s="1">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="M11" s="1">
+        <v>-0.81299999999999994</v>
+      </c>
+      <c r="N11" s="1">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="O11" s="1">
+        <v>0.30099999999999999</v>
+      </c>
+      <c r="P11" s="1">
+        <v>2.1000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>6380</v>
+      </c>
+      <c r="B12" s="1">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1.288</v>
+      </c>
+      <c r="G12" s="1">
+        <v>1.359</v>
+      </c>
+      <c r="H12" s="1">
+        <v>1.4339999999999999</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0.57299999999999995</v>
+      </c>
+      <c r="J12" s="1">
+        <v>2.3E-2</v>
+      </c>
+      <c r="K12" s="1">
+        <v>0.224</v>
+      </c>
+      <c r="L12" s="1">
+        <v>5.5E-2</v>
+      </c>
+      <c r="M12" s="1">
+        <v>-0.47799999999999998</v>
+      </c>
+      <c r="N12" s="1">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="O12" s="1">
+        <v>0.20399999999999999</v>
+      </c>
+      <c r="P12" s="1">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>6380</v>
+      </c>
+      <c r="B13" s="1">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="1">
+        <v>1.4339999999999999</v>
+      </c>
+      <c r="G13" s="1">
+        <v>1.5129999999999999</v>
+      </c>
+      <c r="H13" s="1">
         <v>1.595</v>
       </c>
-      <c r="G6" s="1">
+      <c r="I13" s="1">
+        <v>0.89900000000000002</v>
+      </c>
+      <c r="J13" s="1">
+        <v>1.4E-2</v>
+      </c>
+      <c r="K13" s="1">
+        <v>-0.53600000000000003</v>
+      </c>
+      <c r="L13" s="1">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="M13" s="1">
+        <v>0.19600000000000001</v>
+      </c>
+      <c r="N13" s="1">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="O13" s="1">
+        <v>-1.9E-2</v>
+      </c>
+      <c r="P13" s="1">
+        <v>1.2E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>6380</v>
+      </c>
+      <c r="B14" s="1">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" s="1">
+        <v>1.595</v>
+      </c>
+      <c r="G14" s="1">
         <v>1.6830000000000001</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H14" s="1">
         <v>1.774</v>
       </c>
-      <c r="I6" s="1">
-        <v>0.80100000000000005</v>
-      </c>
-      <c r="J6" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="K6" s="1">
-        <v>-0.105</v>
-      </c>
-      <c r="L6" s="1">
-        <v>2.3E-2</v>
-      </c>
-      <c r="M6" s="1">
-        <v>-0.192</v>
-      </c>
-      <c r="N6" s="1">
-        <v>2.3E-2</v>
-      </c>
-      <c r="O6" s="1">
-        <v>9.5000000000000001E-2</v>
-      </c>
-      <c r="P6" s="1">
-        <v>8.0000000000000002E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
+      <c r="I14" s="1">
+        <v>1.0129999999999999</v>
+      </c>
+      <c r="J14" s="1">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="K14" s="1">
+        <v>-0.85</v>
+      </c>
+      <c r="L14" s="1">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="M14" s="1">
+        <v>0.46899999999999997</v>
+      </c>
+      <c r="N14" s="1">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="O14" s="1">
+        <v>-0.108</v>
+      </c>
+      <c r="P14" s="1">
+        <v>6.0000000000000001E-3</v>
+      </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>

</xml_diff>

<commit_message>
Erro de arredondamento int
No arquivo "eclipse_nv1", linha 260, a variável raioPlanetaPixel não pode ser inteiro, isso resulta em uma diferença muito grande na profundidade do trânsito.
</commit_message>
<xml_diff>
--- a/ExoCTK_results.xlsx
+++ b/ExoCTK_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vikto\PycharmProjects\StarsAndExoplanets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4FFEEB0-D133-4741-A12A-B1C6364C8869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9ADE4E5-B688-4590-B6E5-FC7EE117E0F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{3BF26EB7-DF66-4B75-A14D-202BA100B451}"/>
+    <workbookView xWindow="3015" yWindow="2055" windowWidth="22155" windowHeight="13545" xr2:uid="{3BF26EB7-DF66-4B75-A14D-202BA100B451}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -473,7 +473,7 @@
   <dimension ref="A1:AH27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB22" sqref="AB22"/>
+      <selection activeCell="Q15" sqref="A4:Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
raioPlanetaPixel com valores reais
A variável raioPlanetaPixel não é mais inteira. Foi corrigido o problema e esta, agora, é float.
</commit_message>
<xml_diff>
--- a/ExoCTK_results.xlsx
+++ b/ExoCTK_results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Meu Drive\StarsAndExoplanets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2402A68-4E3C-44E5-BBFF-4AC10BC16CC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E8FF005-7D23-418C-BC4C-AC404A0BB740}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{3BF26EB7-DF66-4B75-A14D-202BA100B451}"/>
+    <workbookView xWindow="12855" yWindow="1140" windowWidth="22155" windowHeight="13545" xr2:uid="{3BF26EB7-DF66-4B75-A14D-202BA100B451}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -465,7 +465,7 @@
   <dimension ref="A1:AH27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Valores da anomalia excêntrica
A função eccanom = solve(m, ecc) pode ser utilizado também eccanom = keplerfunc(m, ecc). Eles diferem nos valores em radiano, p.ex., -4.47 e 1.81, mas ao calcular o sen e cos destes ângulos, os valores de xs e ys acabam sendo iguais.
</commit_message>
<xml_diff>
--- a/ExoCTK_results.xlsx
+++ b/ExoCTK_results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Meu Drive\StarsAndExoplanets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meu Drive\StarsAndExoplanets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E8FF005-7D23-418C-BC4C-AC404A0BB740}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C6A8BE9-BFE7-451E-B663-A4D5682C3939}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12855" yWindow="1140" windowWidth="22155" windowHeight="13545" xr2:uid="{3BF26EB7-DF66-4B75-A14D-202BA100B451}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{3BF26EB7-DF66-4B75-A14D-202BA100B451}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -166,7 +166,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -465,12 +465,12 @@
   <dimension ref="A1:AH27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -522,7 +522,7 @@
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
@@ -574,7 +574,7 @@
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>6380</v>
       </c>
@@ -626,7 +626,7 @@
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>6380</v>
       </c>
@@ -676,7 +676,7 @@
         <v>3.6999999999999998E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>6380</v>
       </c>
@@ -726,7 +726,7 @@
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>6380</v>
       </c>
@@ -776,7 +776,7 @@
         <v>2.3E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>6380</v>
       </c>
@@ -826,7 +826,7 @@
         <v>1.6E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>6380</v>
       </c>
@@ -876,7 +876,7 @@
         <v>1.9E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>6380</v>
       </c>
@@ -926,7 +926,7 @@
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>6380</v>
       </c>
@@ -976,7 +976,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>6380</v>
       </c>
@@ -1026,7 +1026,7 @@
         <v>2.1000000000000001E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>6380</v>
       </c>
@@ -1076,7 +1076,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>6380</v>
       </c>
@@ -1126,7 +1126,7 @@
         <v>1.2E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>6380</v>
       </c>
@@ -1176,7 +1176,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1194,7 +1194,7 @@
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1212,7 +1212,7 @@
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1230,7 +1230,7 @@
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1248,7 +1248,7 @@
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1282,7 +1282,7 @@
       <c r="AG19" s="1"/>
       <c r="AH19" s="1"/>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1316,7 +1316,7 @@
       <c r="AG20" s="1"/>
       <c r="AH20" s="1"/>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.35">
       <c r="S21" s="1"/>
       <c r="T21" s="1"/>
       <c r="U21" s="1"/>
@@ -1334,7 +1334,7 @@
       <c r="AG21" s="1"/>
       <c r="AH21" s="1"/>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.35">
       <c r="S22" s="1"/>
       <c r="T22" s="1"/>
       <c r="U22" s="1"/>
@@ -1352,7 +1352,7 @@
       <c r="AG22" s="1"/>
       <c r="AH22" s="1"/>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.35">
       <c r="S23" s="1"/>
       <c r="T23" s="1"/>
       <c r="U23" s="1"/>
@@ -1370,7 +1370,7 @@
       <c r="AG23" s="1"/>
       <c r="AH23" s="1"/>
     </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.35">
       <c r="S24" s="1"/>
       <c r="T24" s="1"/>
       <c r="U24" s="1"/>
@@ -1388,7 +1388,7 @@
       <c r="AG24" s="1"/>
       <c r="AH24" s="1"/>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.35">
       <c r="S25" s="1"/>
       <c r="T25" s="1"/>
       <c r="U25" s="1"/>
@@ -1406,7 +1406,7 @@
       <c r="AG25" s="1"/>
       <c r="AH25" s="1"/>
     </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.35">
       <c r="S26" s="1"/>
       <c r="T26" s="1"/>
       <c r="U26" s="1"/>
@@ -1424,7 +1424,7 @@
       <c r="AG26" s="1"/>
       <c r="AH26" s="1"/>
     </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.35">
       <c r="S27" s="1"/>
       <c r="T27" s="1"/>
       <c r="U27" s="1"/>

</xml_diff>

<commit_message>
Inserção de paleta de cores
Paleta de cores para o print das curvas de luz.
</commit_message>
<xml_diff>
--- a/ExoCTK_results.xlsx
+++ b/ExoCTK_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Meu Drive\StarsAndExoplanets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F357D2EE-12D0-4979-9EF0-44F0397EAD99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E471F5-5F1C-4CD4-BB40-14D22A3E6AC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13890" yWindow="2055" windowWidth="22155" windowHeight="13545" xr2:uid="{3BF26EB7-DF66-4B75-A14D-202BA100B451}"/>
   </bookViews>
@@ -465,7 +465,7 @@
   <dimension ref="A1:AH27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R17" sqref="A6:R17"/>
+      <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Modificações para os gráficos do paper
</commit_message>
<xml_diff>
--- a/ExoCTK_results.xlsx
+++ b/ExoCTK_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Meu Drive\StarsAndExoplanets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0214421-7F1C-4EFC-9C47-04491F1C87C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94599E15-A90D-40C8-8E09-DFF46A317BFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{FD485E45-5400-4809-8075-6517CC8BF8A4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="27">
   <si>
     <t>Teff</t>
   </si>
@@ -146,9 +146,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -464,13 +465,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E7459B0-01F0-423D-9E42-EFF86DA61453}">
-  <dimension ref="A1:P51"/>
+  <dimension ref="A1:P60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q4" sqref="A4:Q51"/>
+      <selection activeCell="T44" sqref="T44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="20.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -589,34 +593,34 @@
         <v>24</v>
       </c>
       <c r="F3" s="1">
-        <v>0.29199999999999998</v>
+        <v>0.29399999999999998</v>
       </c>
       <c r="G3" s="1">
-        <v>0.30599999999999999</v>
+        <v>0.30049999999999999</v>
       </c>
       <c r="H3" s="1">
-        <v>0.31979999999999997</v>
+        <v>0.30709999999999998</v>
       </c>
       <c r="I3" s="1">
-        <v>-0.26600000000000001</v>
+        <v>-0.32500000000000001</v>
       </c>
       <c r="J3" s="1">
         <v>1.4E-2</v>
       </c>
       <c r="K3" s="1">
-        <v>1.833</v>
+        <v>1.8939999999999999</v>
       </c>
       <c r="L3" s="1">
-        <v>3.2000000000000001E-2</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="M3" s="1">
-        <v>-1.01</v>
+        <v>-1.008</v>
       </c>
       <c r="N3" s="1">
-        <v>3.3000000000000002E-2</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="O3" s="1">
-        <v>0.28999999999999998</v>
+        <v>0.28799999999999998</v>
       </c>
       <c r="P3" s="1">
         <v>1.2E-2</v>
@@ -639,37 +643,37 @@
         <v>24</v>
       </c>
       <c r="F4" s="1">
-        <v>0.32</v>
+        <v>0.30790000000000001</v>
       </c>
       <c r="G4" s="1">
-        <v>0.33400000000000002</v>
+        <v>0.3145</v>
       </c>
       <c r="H4" s="1">
-        <v>0.34799999999999998</v>
+        <v>0.32100000000000001</v>
       </c>
       <c r="I4" s="1">
-        <v>-0.29299999999999998</v>
+        <v>-0.23499999999999999</v>
       </c>
       <c r="J4" s="1">
-        <v>2.1000000000000001E-2</v>
+        <v>1.4E-2</v>
       </c>
       <c r="K4" s="1">
-        <v>2.0830000000000002</v>
+        <v>1.8109999999999999</v>
       </c>
       <c r="L4" s="1">
-        <v>0.05</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="M4" s="1">
-        <v>-1.369</v>
+        <v>-1.0269999999999999</v>
       </c>
       <c r="N4" s="1">
-        <v>0.05</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="O4" s="1">
-        <v>0.39500000000000002</v>
+        <v>0.29499999999999998</v>
       </c>
       <c r="P4" s="1">
-        <v>1.7999999999999999E-2</v>
+        <v>1.2E-2</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -689,37 +693,37 @@
         <v>24</v>
       </c>
       <c r="F5" s="1">
-        <v>0.34799999999999998</v>
+        <v>0.32150000000000001</v>
       </c>
       <c r="G5" s="1">
-        <v>0.36180000000000001</v>
+        <v>0.32840000000000003</v>
       </c>
       <c r="H5" s="1">
-        <v>0.376</v>
+        <v>0.33500000000000002</v>
       </c>
       <c r="I5" s="1">
-        <v>-0.20100000000000001</v>
+        <v>-0.27300000000000002</v>
       </c>
       <c r="J5" s="1">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="K5" s="1">
-        <v>2.1280000000000001</v>
+        <v>2.0550000000000002</v>
       </c>
       <c r="L5" s="1">
-        <v>0.06</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="M5" s="1">
-        <v>-1.6080000000000001</v>
+        <v>-1.347</v>
       </c>
       <c r="N5" s="1">
-        <v>0.06</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="O5" s="1">
-        <v>0.47899999999999998</v>
+        <v>0.39300000000000002</v>
       </c>
       <c r="P5" s="1">
-        <v>2.1999999999999999E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -739,34 +743,34 @@
         <v>24</v>
       </c>
       <c r="F6" s="1">
-        <v>0.376</v>
+        <v>0.3352</v>
       </c>
       <c r="G6" s="1">
-        <v>0.39</v>
+        <v>0.34200000000000003</v>
       </c>
       <c r="H6" s="1">
-        <v>0.40400000000000003</v>
+        <v>0.34889999999999999</v>
       </c>
       <c r="I6" s="1">
-        <v>6.3E-2</v>
+        <v>-0.308</v>
       </c>
       <c r="J6" s="1">
         <v>0.02</v>
       </c>
       <c r="K6" s="1">
-        <v>1.026</v>
+        <v>2.1230000000000002</v>
       </c>
       <c r="L6" s="1">
         <v>4.7E-2</v>
       </c>
       <c r="M6" s="1">
-        <v>-0.252</v>
+        <v>-1.421</v>
       </c>
       <c r="N6" s="1">
         <v>4.7E-2</v>
       </c>
       <c r="O6" s="1">
-        <v>3.0000000000000001E-3</v>
+        <v>0.40799999999999997</v>
       </c>
       <c r="P6" s="1">
         <v>1.7000000000000001E-2</v>
@@ -789,37 +793,37 @@
         <v>24</v>
       </c>
       <c r="F7" s="1">
-        <v>0.40400000000000003</v>
+        <v>0.34899999999999998</v>
       </c>
       <c r="G7" s="1">
-        <v>0.41799999999999998</v>
+        <v>0.35599999999999998</v>
       </c>
       <c r="H7" s="1">
-        <v>0.432</v>
+        <v>0.36280000000000001</v>
       </c>
       <c r="I7" s="1">
-        <v>0.186</v>
+        <v>-0.22800000000000001</v>
       </c>
       <c r="J7" s="1">
-        <v>3.9E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="K7" s="1">
-        <v>0.93700000000000006</v>
+        <v>2.1190000000000002</v>
       </c>
       <c r="L7" s="1">
-        <v>9.1999999999999998E-2</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="M7" s="1">
-        <v>-0.31</v>
+        <v>-1.548</v>
       </c>
       <c r="N7" s="1">
-        <v>9.2999999999999999E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
       <c r="O7" s="1">
-        <v>0.04</v>
+        <v>0.45900000000000002</v>
       </c>
       <c r="P7" s="1">
-        <v>3.4000000000000002E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -839,37 +843,37 @@
         <v>24</v>
       </c>
       <c r="F8" s="1">
-        <v>0.432</v>
+        <v>0.36299999999999999</v>
       </c>
       <c r="G8" s="1">
-        <v>0.44600000000000001</v>
+        <v>0.36959999999999998</v>
       </c>
       <c r="H8" s="1">
-        <v>0.46</v>
+        <v>0.3765</v>
       </c>
       <c r="I8" s="1">
-        <v>0.19400000000000001</v>
+        <v>-0.17799999999999999</v>
       </c>
       <c r="J8" s="1">
-        <v>4.3999999999999997E-2</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="K8" s="1">
-        <v>1.071</v>
+        <v>2.1440000000000001</v>
       </c>
       <c r="L8" s="1">
-        <v>0.104</v>
+        <v>6.2E-2</v>
       </c>
       <c r="M8" s="1">
-        <v>-0.57599999999999996</v>
+        <v>-1.6679999999999999</v>
       </c>
       <c r="N8" s="1">
-        <v>0.104</v>
+        <v>6.2E-2</v>
       </c>
       <c r="O8" s="1">
-        <v>0.14299999999999999</v>
+        <v>0.496</v>
       </c>
       <c r="P8" s="1">
-        <v>3.7999999999999999E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -889,37 +893,37 @@
         <v>24</v>
       </c>
       <c r="F9" s="1">
-        <v>0.46</v>
+        <v>0.377</v>
       </c>
       <c r="G9" s="1">
-        <v>0.47399999999999998</v>
+        <v>0.38350000000000001</v>
       </c>
       <c r="H9" s="1">
-        <v>0.48799999999999999</v>
+        <v>0.3901</v>
       </c>
       <c r="I9" s="1">
-        <v>0.22700000000000001</v>
+        <v>-3.5000000000000003E-2</v>
       </c>
       <c r="J9" s="1">
-        <v>5.1999999999999998E-2</v>
+        <v>1.4E-2</v>
       </c>
       <c r="K9" s="1">
-        <v>1.133</v>
+        <v>1.2070000000000001</v>
       </c>
       <c r="L9" s="1">
-        <v>0.124</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="M9" s="1">
-        <v>-0.75900000000000001</v>
+        <v>-0.34499999999999997</v>
       </c>
       <c r="N9" s="1">
-        <v>0.125</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="O9" s="1">
-        <v>0.219</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="P9" s="1">
-        <v>4.5999999999999999E-2</v>
+        <v>1.2E-2</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -939,37 +943,37 @@
         <v>24</v>
       </c>
       <c r="F10" s="1">
-        <v>0.48799999999999999</v>
+        <v>0.39090000000000003</v>
       </c>
       <c r="G10" s="1">
-        <v>0.502</v>
+        <v>0.39750000000000002</v>
       </c>
       <c r="H10" s="1">
-        <v>0.51600000000000001</v>
+        <v>0.40400000000000003</v>
       </c>
       <c r="I10" s="1">
-        <v>0.2</v>
+        <v>0.159</v>
       </c>
       <c r="J10" s="1">
-        <v>4.8000000000000001E-2</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="K10" s="1">
-        <v>1.198</v>
+        <v>0.83099999999999996</v>
       </c>
       <c r="L10" s="1">
-        <v>0.114</v>
+        <v>6.2E-2</v>
       </c>
       <c r="M10" s="1">
-        <v>-0.88100000000000001</v>
+        <v>-0.124</v>
       </c>
       <c r="N10" s="1">
-        <v>0.115</v>
+        <v>6.3E-2</v>
       </c>
       <c r="O10" s="1">
-        <v>0.26900000000000002</v>
+        <v>-0.02</v>
       </c>
       <c r="P10" s="1">
-        <v>4.2000000000000003E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -989,34 +993,34 @@
         <v>24</v>
       </c>
       <c r="F11" s="1">
-        <v>0.51600000000000001</v>
+        <v>0.40450000000000003</v>
       </c>
       <c r="G11" s="1">
-        <v>0.53029999999999999</v>
+        <v>0.41110000000000002</v>
       </c>
       <c r="H11" s="1">
-        <v>0.54400000000000004</v>
+        <v>0.41799999999999998</v>
       </c>
       <c r="I11" s="1">
-        <v>0.16500000000000001</v>
+        <v>0.14599999999999999</v>
       </c>
       <c r="J11" s="1">
         <v>4.3999999999999997E-2</v>
       </c>
       <c r="K11" s="1">
-        <v>1.246</v>
+        <v>1.1659999999999999</v>
       </c>
       <c r="L11" s="1">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="M11" s="1">
+        <v>-0.59</v>
+      </c>
+      <c r="N11" s="1">
         <v>0.104</v>
       </c>
-      <c r="M11" s="1">
-        <v>-0.95799999999999996</v>
-      </c>
-      <c r="N11" s="1">
-        <v>0.105</v>
-      </c>
       <c r="O11" s="1">
-        <v>0.29899999999999999</v>
+        <v>0.13200000000000001</v>
       </c>
       <c r="P11" s="1">
         <v>3.7999999999999999E-2</v>
@@ -1039,37 +1043,37 @@
         <v>24</v>
       </c>
       <c r="F12" s="1">
-        <v>0.54400000000000004</v>
+        <v>0.41820000000000002</v>
       </c>
       <c r="G12" s="1">
-        <v>0.55800000000000005</v>
+        <v>0.42499999999999999</v>
       </c>
       <c r="H12" s="1">
-        <v>0.57199999999999995</v>
+        <v>0.432</v>
       </c>
       <c r="I12" s="1">
-        <v>0.14599999999999999</v>
+        <v>0.223</v>
       </c>
       <c r="J12" s="1">
-        <v>4.2000000000000003E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="K12" s="1">
-        <v>1.3420000000000001</v>
+        <v>0.72099999999999997</v>
       </c>
       <c r="L12" s="1">
-        <v>9.9000000000000005E-2</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="M12" s="1">
-        <v>-1.1140000000000001</v>
+        <v>-4.5999999999999999E-2</v>
       </c>
       <c r="N12" s="1">
-        <v>0.1</v>
+        <v>8.3000000000000004E-2</v>
       </c>
       <c r="O12" s="1">
-        <v>0.35899999999999999</v>
+        <v>-4.7E-2</v>
       </c>
       <c r="P12" s="1">
-        <v>3.5999999999999997E-2</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
@@ -1086,40 +1090,40 @@
         <v>23</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F13" s="1">
-        <v>0.55100000000000005</v>
+        <v>0.432</v>
       </c>
       <c r="G13" s="1">
-        <v>0.5635</v>
+        <v>0.439</v>
       </c>
       <c r="H13" s="1">
-        <v>0.57599999999999996</v>
+        <v>0.44579999999999997</v>
       </c>
       <c r="I13" s="1">
-        <v>0.13900000000000001</v>
+        <v>9.8000000000000004E-2</v>
       </c>
       <c r="J13" s="1">
-        <v>0.04</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="K13" s="1">
-        <v>1.361</v>
+        <v>1.2330000000000001</v>
       </c>
       <c r="L13" s="1">
-        <v>9.5000000000000001E-2</v>
+        <v>0.08</v>
       </c>
       <c r="M13" s="1">
-        <v>-1.143</v>
+        <v>-0.67900000000000005</v>
       </c>
       <c r="N13" s="1">
-        <v>9.6000000000000002E-2</v>
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="O13" s="1">
-        <v>0.37</v>
+        <v>0.16300000000000001</v>
       </c>
       <c r="P13" s="1">
-        <v>3.5000000000000003E-2</v>
+        <v>2.9000000000000001E-2</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
@@ -1136,40 +1140,40 @@
         <v>23</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F14" s="1">
-        <v>0.57599999999999996</v>
+        <v>0.44600000000000001</v>
       </c>
       <c r="G14" s="1">
-        <v>0.58840000000000003</v>
+        <v>0.4526</v>
       </c>
       <c r="H14" s="1">
-        <v>0.60099999999999998</v>
+        <v>0.45950000000000002</v>
       </c>
       <c r="I14" s="1">
-        <v>0.109</v>
+        <v>0.27700000000000002</v>
       </c>
       <c r="J14" s="1">
-        <v>3.6999999999999998E-2</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="K14" s="1">
-        <v>1.456</v>
+        <v>0.93100000000000005</v>
       </c>
       <c r="L14" s="1">
-        <v>8.5999999999999993E-2</v>
+        <v>0.125</v>
       </c>
       <c r="M14" s="1">
-        <v>-1.2809999999999999</v>
+        <v>-0.48699999999999999</v>
       </c>
       <c r="N14" s="1">
-        <v>8.6999999999999994E-2</v>
+        <v>0.126</v>
       </c>
       <c r="O14" s="1">
-        <v>0.42299999999999999</v>
+        <v>0.126</v>
       </c>
       <c r="P14" s="1">
-        <v>3.2000000000000001E-2</v>
+        <v>4.5999999999999999E-2</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
@@ -1186,40 +1190,40 @@
         <v>23</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F15" s="1">
-        <v>0.60160000000000002</v>
+        <v>0.46</v>
       </c>
       <c r="G15" s="1">
-        <v>0.61399999999999999</v>
+        <v>0.46660000000000001</v>
       </c>
       <c r="H15" s="1">
-        <v>0.626</v>
+        <v>0.47310000000000002</v>
       </c>
       <c r="I15" s="1">
-        <v>9.4E-2</v>
+        <v>0.25900000000000001</v>
       </c>
       <c r="J15" s="1">
-        <v>3.3000000000000002E-2</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="K15" s="1">
-        <v>1.462</v>
+        <v>1.014</v>
       </c>
       <c r="L15" s="1">
-        <v>7.8E-2</v>
+        <v>0.126</v>
       </c>
       <c r="M15" s="1">
-        <v>-1.302</v>
+        <v>-0.61399999999999999</v>
       </c>
       <c r="N15" s="1">
-        <v>7.9000000000000001E-2</v>
+        <v>0.127</v>
       </c>
       <c r="O15" s="1">
-        <v>0.42899999999999999</v>
+        <v>0.17199999999999999</v>
       </c>
       <c r="P15" s="1">
-        <v>2.9000000000000001E-2</v>
+        <v>4.5999999999999999E-2</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
@@ -1236,40 +1240,40 @@
         <v>23</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F16" s="1">
-        <v>0.627</v>
+        <v>0.47389999999999999</v>
       </c>
       <c r="G16" s="1">
-        <v>0.63900000000000001</v>
+        <v>0.48049999999999998</v>
       </c>
       <c r="H16" s="1">
-        <v>0.65139999999999998</v>
+        <v>0.48699999999999999</v>
       </c>
       <c r="I16" s="1">
-        <v>0.1</v>
+        <v>0.19900000000000001</v>
       </c>
       <c r="J16" s="1">
-        <v>3.4000000000000002E-2</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="K16" s="1">
-        <v>1.4339999999999999</v>
+        <v>1.2370000000000001</v>
       </c>
       <c r="L16" s="1">
-        <v>0.08</v>
+        <v>0.123</v>
       </c>
       <c r="M16" s="1">
-        <v>-1.292</v>
+        <v>-0.88600000000000001</v>
       </c>
       <c r="N16" s="1">
-        <v>8.1000000000000003E-2</v>
+        <v>0.124</v>
       </c>
       <c r="O16" s="1">
-        <v>0.42299999999999999</v>
+        <v>0.26</v>
       </c>
       <c r="P16" s="1">
-        <v>2.9000000000000001E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
@@ -1286,40 +1290,40 @@
         <v>23</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F17" s="1">
-        <v>0.65200000000000002</v>
+        <v>0.48749999999999999</v>
       </c>
       <c r="G17" s="1">
-        <v>0.66459999999999997</v>
+        <v>0.49409999999999998</v>
       </c>
       <c r="H17" s="1">
-        <v>0.67700000000000005</v>
+        <v>0.501</v>
       </c>
       <c r="I17" s="1">
-        <v>8.7999999999999995E-2</v>
+        <v>0.2</v>
       </c>
       <c r="J17" s="1">
-        <v>3.2000000000000001E-2</v>
+        <v>4.7E-2</v>
       </c>
       <c r="K17" s="1">
-        <v>1.4670000000000001</v>
+        <v>1.2130000000000001</v>
       </c>
       <c r="L17" s="1">
-        <v>7.6999999999999999E-2</v>
+        <v>0.112</v>
       </c>
       <c r="M17" s="1">
-        <v>-1.3540000000000001</v>
+        <v>-0.89</v>
       </c>
       <c r="N17" s="1">
-        <v>7.6999999999999999E-2</v>
+        <v>0.113</v>
       </c>
       <c r="O17" s="1">
-        <v>0.439</v>
+        <v>0.26800000000000002</v>
       </c>
       <c r="P17" s="1">
-        <v>2.8000000000000001E-2</v>
+        <v>4.1000000000000002E-2</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
@@ -1336,40 +1340,40 @@
         <v>23</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F18" s="1">
-        <v>0.67700000000000005</v>
+        <v>0.50149999999999995</v>
       </c>
       <c r="G18" s="1">
-        <v>0.6895</v>
+        <v>0.50829999999999997</v>
       </c>
       <c r="H18" s="1">
-        <v>0.70199999999999996</v>
+        <v>0.51500000000000001</v>
       </c>
       <c r="I18" s="1">
+        <v>0.20100000000000001</v>
+      </c>
+      <c r="J18" s="1">
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="J18" s="1">
-        <v>2.3E-2</v>
-      </c>
       <c r="K18" s="1">
-        <v>1.5109999999999999</v>
+        <v>1.1919999999999999</v>
       </c>
       <c r="L18" s="1">
-        <v>5.2999999999999999E-2</v>
+        <v>0.11700000000000001</v>
       </c>
       <c r="M18" s="1">
-        <v>-1.4</v>
+        <v>-0.88100000000000001</v>
       </c>
       <c r="N18" s="1">
-        <v>5.3999999999999999E-2</v>
+        <v>0.11799999999999999</v>
       </c>
       <c r="O18" s="1">
-        <v>0.46600000000000003</v>
+        <v>0.27200000000000002</v>
       </c>
       <c r="P18" s="1">
-        <v>0.02</v>
+        <v>4.2999999999999997E-2</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
@@ -1386,40 +1390,40 @@
         <v>23</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F19" s="1">
-        <v>0.7026</v>
+        <v>0.51500000000000001</v>
       </c>
       <c r="G19" s="1">
-        <v>0.71499999999999997</v>
+        <v>0.52200000000000002</v>
       </c>
       <c r="H19" s="1">
-        <v>0.72699999999999998</v>
+        <v>0.52900000000000003</v>
       </c>
       <c r="I19" s="1">
-        <v>5.0999999999999997E-2</v>
+        <v>0.153</v>
       </c>
       <c r="J19" s="1">
-        <v>2.1000000000000001E-2</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="K19" s="1">
-        <v>1.47</v>
+        <v>1.2430000000000001</v>
       </c>
       <c r="L19" s="1">
-        <v>4.9000000000000002E-2</v>
+        <v>9.8000000000000004E-2</v>
       </c>
       <c r="M19" s="1">
-        <v>-1.365</v>
+        <v>-0.92900000000000005</v>
       </c>
       <c r="N19" s="1">
-        <v>0.05</v>
+        <v>9.9000000000000005E-2</v>
       </c>
       <c r="O19" s="1">
-        <v>0.45300000000000001</v>
+        <v>0.28699999999999998</v>
       </c>
       <c r="P19" s="1">
-        <v>1.7999999999999999E-2</v>
+        <v>3.5999999999999997E-2</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
@@ -1436,40 +1440,40 @@
         <v>23</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F20" s="1">
-        <v>0.72799999999999998</v>
+        <v>0.52900000000000003</v>
       </c>
       <c r="G20" s="1">
-        <v>0.74</v>
+        <v>0.53559999999999997</v>
       </c>
       <c r="H20" s="1">
-        <v>0.75239999999999996</v>
+        <v>0.54249999999999998</v>
       </c>
       <c r="I20" s="1">
-        <v>5.5E-2</v>
+        <v>0.17499999999999999</v>
       </c>
       <c r="J20" s="1">
-        <v>1.9E-2</v>
+        <v>4.7E-2</v>
       </c>
       <c r="K20" s="1">
-        <v>1.4410000000000001</v>
+        <v>1.246</v>
       </c>
       <c r="L20" s="1">
-        <v>4.5999999999999999E-2</v>
+        <v>0.11</v>
       </c>
       <c r="M20" s="1">
-        <v>-1.35</v>
+        <v>-0.97699999999999998</v>
       </c>
       <c r="N20" s="1">
-        <v>4.5999999999999999E-2</v>
+        <v>0.111</v>
       </c>
       <c r="O20" s="1">
-        <v>0.44800000000000001</v>
+        <v>0.307</v>
       </c>
       <c r="P20" s="1">
-        <v>1.7000000000000001E-2</v>
+        <v>4.1000000000000002E-2</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
@@ -1486,40 +1490,40 @@
         <v>23</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F21" s="1">
-        <v>0.753</v>
+        <v>0.54300000000000004</v>
       </c>
       <c r="G21" s="1">
-        <v>0.76500000000000001</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="H21" s="1">
-        <v>0.77800000000000002</v>
+        <v>0.55600000000000005</v>
       </c>
       <c r="I21" s="1">
-        <v>5.1999999999999998E-2</v>
+        <v>0.157</v>
       </c>
       <c r="J21" s="1">
-        <v>1.7999999999999999E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="K21" s="1">
-        <v>1.4359999999999999</v>
+        <v>1.3109999999999999</v>
       </c>
       <c r="L21" s="1">
-        <v>4.2999999999999997E-2</v>
+        <v>0.105</v>
       </c>
       <c r="M21" s="1">
-        <v>-1.3620000000000001</v>
+        <v>-1.0660000000000001</v>
       </c>
       <c r="N21" s="1">
-        <v>4.3999999999999997E-2</v>
+        <v>0.106</v>
       </c>
       <c r="O21" s="1">
-        <v>0.45400000000000001</v>
+        <v>0.34</v>
       </c>
       <c r="P21" s="1">
-        <v>1.6E-2</v>
+        <v>3.9E-2</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
@@ -1536,1489 +1540,1939 @@
         <v>23</v>
       </c>
       <c r="E22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F22" s="1">
+        <v>0.55659999999999998</v>
+      </c>
+      <c r="G22" s="1">
+        <v>0.5635</v>
+      </c>
+      <c r="H22" s="1">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="I22" s="1">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="J22" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="K22" s="1">
+        <v>1.3660000000000001</v>
+      </c>
+      <c r="L22" s="1">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="M22" s="1">
+        <v>-1.1479999999999999</v>
+      </c>
+      <c r="N22" s="1">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="O22" s="1">
+        <v>0.372</v>
+      </c>
+      <c r="P22" s="1">
+        <v>3.5000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>6380</v>
+      </c>
+      <c r="B23" s="2">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F22" s="1">
+      <c r="F23" s="2">
+        <v>0.57599999999999996</v>
+      </c>
+      <c r="G23" s="2">
+        <v>0.58840000000000003</v>
+      </c>
+      <c r="H23" s="2">
+        <v>0.60099999999999998</v>
+      </c>
+      <c r="I23" s="2">
+        <v>0.109</v>
+      </c>
+      <c r="J23" s="2">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="K23" s="2">
+        <v>1.456</v>
+      </c>
+      <c r="L23" s="2">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="M23" s="2">
+        <v>-1.2809999999999999</v>
+      </c>
+      <c r="N23" s="2">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="O23" s="2">
+        <v>0.42299999999999999</v>
+      </c>
+      <c r="P23" s="2">
+        <v>3.2000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>6380</v>
+      </c>
+      <c r="B24" s="2">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F24" s="2">
+        <v>0.60160000000000002</v>
+      </c>
+      <c r="G24" s="2">
+        <v>0.61399999999999999</v>
+      </c>
+      <c r="H24" s="2">
+        <v>0.626</v>
+      </c>
+      <c r="I24" s="2">
+        <v>9.4E-2</v>
+      </c>
+      <c r="J24" s="2">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="K24" s="2">
+        <v>1.462</v>
+      </c>
+      <c r="L24" s="2">
+        <v>7.8E-2</v>
+      </c>
+      <c r="M24" s="2">
+        <v>-1.302</v>
+      </c>
+      <c r="N24" s="2">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="O24" s="2">
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="P24" s="2">
+        <v>2.9000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>6380</v>
+      </c>
+      <c r="B25" s="2">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F25" s="2">
+        <v>0.627</v>
+      </c>
+      <c r="G25" s="2">
+        <v>0.63900000000000001</v>
+      </c>
+      <c r="H25" s="2">
+        <v>0.65139999999999998</v>
+      </c>
+      <c r="I25" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="J25" s="2">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="K25" s="2">
+        <v>1.4339999999999999</v>
+      </c>
+      <c r="L25" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="M25" s="2">
+        <v>-1.292</v>
+      </c>
+      <c r="N25" s="2">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="O25" s="2">
+        <v>0.42299999999999999</v>
+      </c>
+      <c r="P25" s="2">
+        <v>2.9000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>6380</v>
+      </c>
+      <c r="B26" s="2">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F26" s="2">
+        <v>0.65200000000000002</v>
+      </c>
+      <c r="G26" s="2">
+        <v>0.66459999999999997</v>
+      </c>
+      <c r="H26" s="2">
+        <v>0.67700000000000005</v>
+      </c>
+      <c r="I26" s="2">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="J26" s="2">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="K26" s="2">
+        <v>1.4670000000000001</v>
+      </c>
+      <c r="L26" s="2">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="M26" s="2">
+        <v>-1.3540000000000001</v>
+      </c>
+      <c r="N26" s="2">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="O26" s="2">
+        <v>0.439</v>
+      </c>
+      <c r="P26" s="2">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>6380</v>
+      </c>
+      <c r="B27" s="2">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F27" s="2">
+        <v>0.67700000000000005</v>
+      </c>
+      <c r="G27" s="2">
+        <v>0.6895</v>
+      </c>
+      <c r="H27" s="2">
+        <v>0.70199999999999996</v>
+      </c>
+      <c r="I27" s="2">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="J27" s="2">
+        <v>2.3E-2</v>
+      </c>
+      <c r="K27" s="2">
+        <v>1.5109999999999999</v>
+      </c>
+      <c r="L27" s="2">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="M27" s="2">
+        <v>-1.4</v>
+      </c>
+      <c r="N27" s="2">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="O27" s="2">
+        <v>0.46600000000000003</v>
+      </c>
+      <c r="P27" s="2">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>6380</v>
+      </c>
+      <c r="B28" s="2">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="C28" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F28" s="2">
+        <v>0.7026</v>
+      </c>
+      <c r="G28" s="2">
+        <v>0.71499999999999997</v>
+      </c>
+      <c r="H28" s="2">
+        <v>0.72699999999999998</v>
+      </c>
+      <c r="I28" s="2">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="J28" s="2">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="K28" s="2">
+        <v>1.47</v>
+      </c>
+      <c r="L28" s="2">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="M28" s="2">
+        <v>-1.365</v>
+      </c>
+      <c r="N28" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="O28" s="2">
+        <v>0.45300000000000001</v>
+      </c>
+      <c r="P28" s="2">
+        <v>1.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>6380</v>
+      </c>
+      <c r="B29" s="2">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="C29" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F29" s="2">
+        <v>0.72799999999999998</v>
+      </c>
+      <c r="G29" s="2">
+        <v>0.74</v>
+      </c>
+      <c r="H29" s="2">
+        <v>0.75239999999999996</v>
+      </c>
+      <c r="I29" s="2">
+        <v>5.5E-2</v>
+      </c>
+      <c r="J29" s="2">
+        <v>1.9E-2</v>
+      </c>
+      <c r="K29" s="2">
+        <v>1.4410000000000001</v>
+      </c>
+      <c r="L29" s="2">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="M29" s="2">
+        <v>-1.35</v>
+      </c>
+      <c r="N29" s="2">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="O29" s="2">
+        <v>0.44800000000000001</v>
+      </c>
+      <c r="P29" s="2">
+        <v>1.7000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>6380</v>
+      </c>
+      <c r="B30" s="2">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="C30" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F30" s="2">
+        <v>0.753</v>
+      </c>
+      <c r="G30" s="2">
+        <v>0.76500000000000001</v>
+      </c>
+      <c r="H30" s="2">
         <v>0.77800000000000002</v>
       </c>
-      <c r="G22" s="1">
+      <c r="I30" s="2">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="J30" s="2">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="K30" s="2">
+        <v>1.4359999999999999</v>
+      </c>
+      <c r="L30" s="2">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="M30" s="2">
+        <v>-1.3620000000000001</v>
+      </c>
+      <c r="N30" s="2">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="O30" s="2">
+        <v>0.45400000000000001</v>
+      </c>
+      <c r="P30" s="2">
+        <v>1.6E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>6380</v>
+      </c>
+      <c r="B31" s="2">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="C31" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F31" s="2">
+        <v>0.77800000000000002</v>
+      </c>
+      <c r="G31" s="2">
         <v>0.79049999999999998</v>
       </c>
-      <c r="H22" s="1">
+      <c r="H31" s="2">
         <v>0.80300000000000005</v>
       </c>
-      <c r="I22" s="1">
+      <c r="I31" s="2">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="J22" s="1">
+      <c r="J31" s="2">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="K22" s="1">
+      <c r="K31" s="2">
         <v>1.4119999999999999</v>
       </c>
-      <c r="L22" s="1">
+      <c r="L31" s="2">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="M22" s="1">
+      <c r="M31" s="2">
         <v>-1.3440000000000001</v>
       </c>
-      <c r="N22" s="1">
+      <c r="N31" s="2">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="O22" s="1">
+      <c r="O31" s="2">
         <v>0.44700000000000001</v>
       </c>
-      <c r="P22" s="1">
+      <c r="P31" s="2">
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>6380</v>
-      </c>
-      <c r="B23" s="1">
-        <v>4.3099999999999996</v>
-      </c>
-      <c r="C23" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E23" s="1" t="s">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>6380</v>
+      </c>
+      <c r="B32" s="2">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="C32" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E32" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F23" s="1">
+      <c r="F32" s="2">
         <v>0.80369999999999997</v>
       </c>
-      <c r="G23" s="1">
+      <c r="G32" s="2">
         <v>0.81599999999999995</v>
       </c>
-      <c r="H23" s="1">
+      <c r="H32" s="2">
         <v>0.82799999999999996</v>
       </c>
-      <c r="I23" s="1">
+      <c r="I32" s="2">
         <v>7.8E-2</v>
       </c>
-      <c r="J23" s="1">
+      <c r="J32" s="2">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="K23" s="1">
+      <c r="K32" s="2">
         <v>1.331</v>
       </c>
-      <c r="L23" s="1">
+      <c r="L32" s="2">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="M23" s="1">
+      <c r="M32" s="2">
         <v>-1.2669999999999999</v>
       </c>
-      <c r="N23" s="1">
+      <c r="N32" s="2">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="O23" s="1">
+      <c r="O32" s="2">
         <v>0.41799999999999998</v>
       </c>
-      <c r="P23" s="1">
+      <c r="P32" s="2">
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>6380</v>
-      </c>
-      <c r="B24" s="1">
-        <v>4.3099999999999996</v>
-      </c>
-      <c r="C24" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E24" s="1" t="s">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>6380</v>
+      </c>
+      <c r="B33" s="2">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="C33" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E33" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F24" s="1">
+      <c r="F33" s="2">
         <v>0.82899999999999996</v>
       </c>
-      <c r="G24" s="1">
+      <c r="G33" s="2">
         <v>0.84130000000000005</v>
       </c>
-      <c r="H24" s="1">
+      <c r="H33" s="2">
         <v>0.85350000000000004</v>
       </c>
-      <c r="I24" s="1">
+      <c r="I33" s="2">
         <v>0.13400000000000001</v>
       </c>
-      <c r="J24" s="1">
+      <c r="J33" s="2">
         <v>2.4E-2</v>
       </c>
-      <c r="K24" s="1">
+      <c r="K33" s="2">
         <v>1.17</v>
       </c>
-      <c r="L24" s="1">
+      <c r="L33" s="2">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="M24" s="1">
+      <c r="M33" s="2">
         <v>-1.1100000000000001</v>
       </c>
-      <c r="N24" s="1">
+      <c r="N33" s="2">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="O24" s="1">
+      <c r="O33" s="2">
         <v>0.35899999999999999</v>
       </c>
-      <c r="P24" s="1">
+      <c r="P33" s="2">
         <v>2.1000000000000001E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>6380</v>
-      </c>
-      <c r="B25" s="1">
-        <v>4.3099999999999996</v>
-      </c>
-      <c r="C25" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E25" s="1" t="s">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>6380</v>
+      </c>
+      <c r="B34" s="2">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="C34" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E34" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F25" s="1">
+      <c r="F34" s="2">
         <v>0.85399999999999998</v>
       </c>
-      <c r="G25" s="1">
+      <c r="G34" s="2">
         <v>0.86599999999999999</v>
       </c>
-      <c r="H25" s="1">
+      <c r="H34" s="2">
         <v>0.879</v>
       </c>
-      <c r="I25" s="1">
+      <c r="I34" s="2">
         <v>0.13700000000000001</v>
       </c>
-      <c r="J25" s="1">
+      <c r="J34" s="2">
         <v>2.4E-2</v>
       </c>
-      <c r="K25" s="1">
+      <c r="K34" s="2">
         <v>1.149</v>
       </c>
-      <c r="L25" s="1">
+      <c r="L34" s="2">
         <v>5.6000000000000001E-2</v>
       </c>
-      <c r="M25" s="1">
+      <c r="M34" s="2">
         <v>-1.093</v>
       </c>
-      <c r="N25" s="1">
+      <c r="N34" s="2">
         <v>5.6000000000000001E-2</v>
       </c>
-      <c r="O25" s="1">
+      <c r="O34" s="2">
         <v>0.34899999999999998</v>
       </c>
-      <c r="P25" s="1">
+      <c r="P34" s="2">
         <v>0.02</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
-        <v>6380</v>
-      </c>
-      <c r="B26" s="1">
-        <v>4.3099999999999996</v>
-      </c>
-      <c r="C26" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E26" s="1" t="s">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>6380</v>
+      </c>
+      <c r="B35" s="2">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="C35" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E35" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F26" s="1">
+      <c r="F35" s="2">
         <v>0.879</v>
       </c>
-      <c r="G26" s="1">
+      <c r="G35" s="2">
         <v>0.89159999999999995</v>
       </c>
-      <c r="H26" s="1">
+      <c r="H35" s="2">
         <v>0.90400000000000003</v>
       </c>
-      <c r="I26" s="1">
+      <c r="I35" s="2">
         <v>0.16400000000000001</v>
       </c>
-      <c r="J26" s="1">
+      <c r="J35" s="2">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="K26" s="1">
+      <c r="K35" s="2">
         <v>1.0649999999999999</v>
       </c>
-      <c r="L26" s="1">
+      <c r="L35" s="2">
         <v>5.1999999999999998E-2</v>
       </c>
-      <c r="M26" s="1">
+      <c r="M35" s="2">
         <v>-1.024</v>
       </c>
-      <c r="N26" s="1">
+      <c r="N35" s="2">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="O26" s="1">
+      <c r="O35" s="2">
         <v>0.32900000000000001</v>
       </c>
-      <c r="P26" s="1">
+      <c r="P35" s="2">
         <v>1.9E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
-        <v>6380</v>
-      </c>
-      <c r="B27" s="1">
-        <v>4.3099999999999996</v>
-      </c>
-      <c r="C27" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E27" s="1" t="s">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>6380</v>
+      </c>
+      <c r="B36" s="2">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="C36" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F27" s="1">
+      <c r="F36" s="2">
         <v>0.90429999999999999</v>
       </c>
-      <c r="G27" s="1">
+      <c r="G36" s="2">
         <v>0.91700000000000004</v>
       </c>
-      <c r="H27" s="1">
+      <c r="H36" s="2">
         <v>0.92900000000000005</v>
       </c>
-      <c r="I27" s="1">
+      <c r="I36" s="2">
         <v>0.154</v>
       </c>
-      <c r="J27" s="1">
+      <c r="J36" s="2">
         <v>1.9E-2</v>
       </c>
-      <c r="K27" s="1">
+      <c r="K36" s="2">
         <v>1.077</v>
       </c>
-      <c r="L27" s="1">
+      <c r="L36" s="2">
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="M27" s="1">
+      <c r="M36" s="2">
         <v>-1.038</v>
       </c>
-      <c r="N27" s="1">
+      <c r="N36" s="2">
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="O27" s="1">
+      <c r="O36" s="2">
         <v>0.33800000000000002</v>
       </c>
-      <c r="P27" s="1">
+      <c r="P36" s="2">
         <v>1.6E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
-        <v>6380</v>
-      </c>
-      <c r="B28" s="1">
-        <v>4.3099999999999996</v>
-      </c>
-      <c r="C28" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E28" s="1" t="s">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>6380</v>
+      </c>
+      <c r="B37" s="2">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="C37" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E37" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F28" s="1">
+      <c r="F37" s="2">
         <v>0.93</v>
       </c>
-      <c r="G28" s="1">
+      <c r="G37" s="2">
         <v>0.94240000000000002</v>
       </c>
-      <c r="H28" s="1">
+      <c r="H37" s="2">
         <v>0.9546</v>
       </c>
-      <c r="I28" s="1">
+      <c r="I37" s="2">
         <v>0.13800000000000001</v>
       </c>
-      <c r="J28" s="1">
+      <c r="J37" s="2">
         <v>1.6E-2</v>
       </c>
-      <c r="K28" s="1">
+      <c r="K37" s="2">
         <v>1.109</v>
       </c>
-      <c r="L28" s="1">
+      <c r="L37" s="2">
         <v>3.6999999999999998E-2</v>
       </c>
-      <c r="M28" s="1">
+      <c r="M37" s="2">
         <v>-1.085</v>
       </c>
-      <c r="N28" s="1">
+      <c r="N37" s="2">
         <v>3.6999999999999998E-2</v>
       </c>
-      <c r="O28" s="1">
+      <c r="O37" s="2">
         <v>0.36399999999999999</v>
       </c>
-      <c r="P28" s="1">
+      <c r="P37" s="2">
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
-        <v>6380</v>
-      </c>
-      <c r="B29" s="1">
-        <v>4.3099999999999996</v>
-      </c>
-      <c r="C29" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E29" s="1" t="s">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>6380</v>
+      </c>
+      <c r="B38" s="2">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="C38" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E38" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F29" s="1">
+      <c r="F38" s="2">
         <v>0.95499999999999996</v>
       </c>
-      <c r="G29" s="1">
+      <c r="G38" s="2">
         <v>0.96730000000000005</v>
       </c>
-      <c r="H29" s="1">
+      <c r="H38" s="2">
         <v>0.98</v>
       </c>
-      <c r="I29" s="1">
+      <c r="I38" s="2">
         <v>0.153</v>
       </c>
-      <c r="J29" s="1">
+      <c r="J38" s="2">
         <v>1.6E-2</v>
       </c>
-      <c r="K29" s="1">
+      <c r="K38" s="2">
         <v>1.075</v>
       </c>
-      <c r="L29" s="1">
+      <c r="L38" s="2">
         <v>3.6999999999999998E-2</v>
       </c>
-      <c r="M29" s="1">
+      <c r="M38" s="2">
         <v>-1.0740000000000001</v>
       </c>
-      <c r="N29" s="1">
+      <c r="N38" s="2">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="O29" s="1">
+      <c r="O38" s="2">
         <v>0.36299999999999999</v>
       </c>
-      <c r="P29" s="1">
+      <c r="P38" s="2">
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
-        <v>6380</v>
-      </c>
-      <c r="B30" s="1">
-        <v>4.3099999999999996</v>
-      </c>
-      <c r="C30" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E30" s="1" t="s">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <v>6380</v>
+      </c>
+      <c r="B39" s="2">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="C39" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E39" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F30" s="1">
+      <c r="F39" s="2">
         <v>0.98</v>
       </c>
-      <c r="G30" s="1">
+      <c r="G39" s="2">
         <v>0.99270000000000003</v>
       </c>
-      <c r="H30" s="1">
+      <c r="H39" s="2">
         <v>1.0049999999999999</v>
       </c>
-      <c r="I30" s="1">
+      <c r="I39" s="2">
         <v>0.15</v>
       </c>
-      <c r="J30" s="1">
+      <c r="J39" s="2">
         <v>1.9E-2</v>
       </c>
-      <c r="K30" s="1">
+      <c r="K39" s="2">
         <v>1.083</v>
       </c>
-      <c r="L30" s="1">
+      <c r="L39" s="2">
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="M30" s="1">
+      <c r="M39" s="2">
         <v>-1.081</v>
       </c>
-      <c r="N30" s="1">
+      <c r="N39" s="2">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="O30" s="1">
+      <c r="O39" s="2">
         <v>0.36699999999999999</v>
       </c>
-      <c r="P30" s="1">
+      <c r="P39" s="2">
         <v>1.6E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <v>6380</v>
-      </c>
-      <c r="B31" s="1">
-        <v>4.3099999999999996</v>
-      </c>
-      <c r="C31" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E31" s="1" t="s">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <v>6380</v>
+      </c>
+      <c r="B40" s="2">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="C40" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E40" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F31" s="1">
+      <c r="F40" s="2">
         <v>1.006</v>
       </c>
-      <c r="G31" s="1">
+      <c r="G40" s="2">
         <v>1.018</v>
       </c>
-      <c r="H31" s="1">
+      <c r="H40" s="2">
         <v>1.03</v>
       </c>
-      <c r="I31" s="1">
+      <c r="I40" s="2">
         <v>0.17699999999999999</v>
       </c>
-      <c r="J31" s="1">
+      <c r="J40" s="2">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="K31" s="1">
+      <c r="K40" s="2">
         <v>1.0249999999999999</v>
       </c>
-      <c r="L31" s="1">
+      <c r="L40" s="2">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="M31" s="1">
+      <c r="M40" s="2">
         <v>-1.042</v>
       </c>
-      <c r="N31" s="1">
+      <c r="N40" s="2">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="O31" s="1">
+      <c r="O40" s="2">
         <v>0.35399999999999998</v>
       </c>
-      <c r="P31" s="1">
+      <c r="P40" s="2">
         <v>1.6E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
-        <v>6380</v>
-      </c>
-      <c r="B32" s="1">
-        <v>4.3099999999999996</v>
-      </c>
-      <c r="C32" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E32" s="1" t="s">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
+        <v>6380</v>
+      </c>
+      <c r="B41" s="2">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="C41" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E41" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F32" s="1">
+      <c r="F41" s="2">
         <v>1.0409999999999999</v>
       </c>
-      <c r="G32" s="1">
+      <c r="G41" s="2">
         <v>1.0549999999999999</v>
       </c>
-      <c r="H32" s="1">
+      <c r="H41" s="2">
         <v>1.069</v>
       </c>
-      <c r="I32" s="1">
+      <c r="I41" s="2">
         <v>0.17899999999999999</v>
       </c>
-      <c r="J32" s="1">
+      <c r="J41" s="2">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="K32" s="1">
+      <c r="K41" s="2">
         <v>1.01</v>
       </c>
-      <c r="L32" s="1">
+      <c r="L41" s="2">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="M32" s="1">
+      <c r="M41" s="2">
         <v>-1.046</v>
       </c>
-      <c r="N32" s="1">
+      <c r="N41" s="2">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="O32" s="1">
+      <c r="O41" s="2">
         <v>0.36399999999999999</v>
       </c>
-      <c r="P32" s="1">
+      <c r="P41" s="2">
         <v>1.6E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
-        <v>6380</v>
-      </c>
-      <c r="B33" s="1">
-        <v>4.3099999999999996</v>
-      </c>
-      <c r="C33" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E33" s="1" t="s">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>6380</v>
+      </c>
+      <c r="B42" s="2">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="C42" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E42" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F33" s="1">
+      <c r="F42" s="2">
         <v>1.069</v>
       </c>
-      <c r="G33" s="1">
+      <c r="G42" s="2">
         <v>1.083</v>
       </c>
-      <c r="H33" s="1">
+      <c r="H42" s="2">
         <v>1.0980000000000001</v>
       </c>
-      <c r="I33" s="1">
+      <c r="I42" s="2">
         <v>0.252</v>
       </c>
-      <c r="J33" s="1">
+      <c r="J42" s="2">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="K33" s="1">
+      <c r="K42" s="2">
         <v>0.83899999999999997</v>
       </c>
-      <c r="L33" s="1">
+      <c r="L42" s="2">
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="M33" s="1">
+      <c r="M42" s="2">
         <v>-0.89400000000000002</v>
       </c>
-      <c r="N33" s="1">
+      <c r="N42" s="2">
         <v>0.05</v>
       </c>
-      <c r="O33" s="1">
+      <c r="O42" s="2">
         <v>0.30299999999999999</v>
       </c>
-      <c r="P33" s="1">
+      <c r="P42" s="2">
         <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
-        <v>6380</v>
-      </c>
-      <c r="B34" s="1">
-        <v>4.3099999999999996</v>
-      </c>
-      <c r="C34" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E34" s="1" t="s">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <v>6380</v>
+      </c>
+      <c r="B43" s="2">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="C43" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E43" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F34" s="1">
+      <c r="F43" s="2">
         <v>1.0980000000000001</v>
       </c>
-      <c r="G34" s="1">
+      <c r="G43" s="2">
         <v>1.1120000000000001</v>
       </c>
-      <c r="H34" s="1">
+      <c r="H43" s="2">
         <v>1.127</v>
       </c>
-      <c r="I34" s="1">
+      <c r="I43" s="2">
         <v>0.22700000000000001</v>
       </c>
-      <c r="J34" s="1">
+      <c r="J43" s="2">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="K34" s="1">
+      <c r="K43" s="2">
         <v>0.91500000000000004</v>
       </c>
-      <c r="L34" s="1">
+      <c r="L43" s="2">
         <v>5.1999999999999998E-2</v>
       </c>
-      <c r="M34" s="1">
+      <c r="M43" s="2">
         <v>-0.98399999999999999</v>
       </c>
-      <c r="N34" s="1">
+      <c r="N43" s="2">
         <v>5.1999999999999998E-2</v>
       </c>
-      <c r="O34" s="1">
+      <c r="O43" s="2">
         <v>0.34499999999999997</v>
       </c>
-      <c r="P34" s="1">
+      <c r="P43" s="2">
         <v>1.9E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
-        <v>6380</v>
-      </c>
-      <c r="B35" s="1">
-        <v>4.3099999999999996</v>
-      </c>
-      <c r="C35" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E35" s="1" t="s">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <v>6380</v>
+      </c>
+      <c r="B44" s="2">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="C44" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E44" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F35" s="1">
+      <c r="F44" s="2">
         <v>1.1279999999999999</v>
       </c>
-      <c r="G35" s="1">
+      <c r="G44" s="2">
         <v>1.143</v>
       </c>
-      <c r="H35" s="1">
+      <c r="H44" s="2">
         <v>1.1579999999999999</v>
       </c>
-      <c r="I35" s="1">
+      <c r="I44" s="2">
         <v>0.252</v>
       </c>
-      <c r="J35" s="1">
+      <c r="J44" s="2">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="K35" s="1">
+      <c r="K44" s="2">
         <v>0.85099999999999998</v>
       </c>
-      <c r="L35" s="1">
+      <c r="L44" s="2">
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="M35" s="1">
+      <c r="M44" s="2">
         <v>-0.93400000000000005</v>
       </c>
-      <c r="N35" s="1">
+      <c r="N44" s="2">
         <v>0.05</v>
       </c>
-      <c r="O35" s="1">
+      <c r="O44" s="2">
         <v>0.33200000000000002</v>
       </c>
-      <c r="P35" s="1">
+      <c r="P44" s="2">
         <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
-        <v>6380</v>
-      </c>
-      <c r="B36" s="1">
-        <v>4.3099999999999996</v>
-      </c>
-      <c r="C36" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E36" s="1" t="s">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
+        <v>6380</v>
+      </c>
+      <c r="B45" s="2">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="C45" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E45" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F36" s="1">
+      <c r="F45" s="2">
         <v>1.1579999999999999</v>
       </c>
-      <c r="G36" s="1">
+      <c r="G45" s="2">
         <v>1.1739999999999999</v>
       </c>
-      <c r="H36" s="1">
+      <c r="H45" s="2">
         <v>1.1890000000000001</v>
       </c>
-      <c r="I36" s="1">
+      <c r="I45" s="2">
         <v>0.28899999999999998</v>
       </c>
-      <c r="J36" s="1">
+      <c r="J45" s="2">
         <v>2.3E-2</v>
       </c>
-      <c r="K36" s="1">
+      <c r="K45" s="2">
         <v>0.77800000000000002</v>
       </c>
-      <c r="L36" s="1">
+      <c r="L45" s="2">
         <v>5.5E-2</v>
       </c>
-      <c r="M36" s="1">
+      <c r="M45" s="2">
         <v>-0.88400000000000001</v>
       </c>
-      <c r="N36" s="1">
+      <c r="N45" s="2">
         <v>5.5E-2</v>
       </c>
-      <c r="O36" s="1">
+      <c r="O45" s="2">
         <v>0.318</v>
       </c>
-      <c r="P36" s="1">
+      <c r="P45" s="2">
         <v>0.02</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
-        <v>6380</v>
-      </c>
-      <c r="B37" s="1">
-        <v>4.3099999999999996</v>
-      </c>
-      <c r="C37" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E37" s="1" t="s">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
+        <v>6380</v>
+      </c>
+      <c r="B46" s="2">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="C46" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E46" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F37" s="1">
+      <c r="F46" s="2">
         <v>1.1890000000000001</v>
       </c>
-      <c r="G37" s="1">
+      <c r="G46" s="2">
         <v>1.2050000000000001</v>
       </c>
-      <c r="H37" s="1">
+      <c r="H46" s="2">
         <v>1.222</v>
       </c>
-      <c r="I37" s="1">
+      <c r="I46" s="2">
         <v>0.31</v>
       </c>
-      <c r="J37" s="1">
+      <c r="J46" s="2">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="K37" s="1">
+      <c r="K46" s="2">
         <v>0.76300000000000001</v>
       </c>
-      <c r="L37" s="1">
+      <c r="L46" s="2">
         <v>6.2E-2</v>
       </c>
-      <c r="M37" s="1">
+      <c r="M46" s="2">
         <v>-0.89900000000000002</v>
       </c>
-      <c r="N37" s="1">
+      <c r="N46" s="2">
         <v>6.3E-2</v>
       </c>
-      <c r="O37" s="1">
+      <c r="O46" s="2">
         <v>0.33100000000000002</v>
       </c>
-      <c r="P37" s="1">
+      <c r="P46" s="2">
         <v>2.3E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A38" s="1">
-        <v>6380</v>
-      </c>
-      <c r="B38" s="1">
-        <v>4.3099999999999996</v>
-      </c>
-      <c r="C38" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E38" s="1" t="s">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
+        <v>6380</v>
+      </c>
+      <c r="B47" s="2">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="C47" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E47" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F38" s="1">
+      <c r="F47" s="2">
         <v>1.222</v>
       </c>
-      <c r="G38" s="1">
+      <c r="G47" s="2">
         <v>1.2370000000000001</v>
       </c>
-      <c r="H38" s="1">
+      <c r="H47" s="2">
         <v>1.254</v>
       </c>
-      <c r="I38" s="1">
+      <c r="I47" s="2">
         <v>0.36299999999999999</v>
       </c>
-      <c r="J38" s="1">
+      <c r="J47" s="2">
         <v>2.7E-2</v>
       </c>
-      <c r="K38" s="1">
+      <c r="K47" s="2">
         <v>0.65900000000000003</v>
       </c>
-      <c r="L38" s="1">
+      <c r="L47" s="2">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="M38" s="1">
+      <c r="M47" s="2">
         <v>-0.82199999999999995</v>
       </c>
-      <c r="N38" s="1">
+      <c r="N47" s="2">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="O38" s="1">
+      <c r="O47" s="2">
         <v>0.309</v>
       </c>
-      <c r="P38" s="1">
+      <c r="P47" s="2">
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
-        <v>6380</v>
-      </c>
-      <c r="B39" s="1">
-        <v>4.3099999999999996</v>
-      </c>
-      <c r="C39" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E39" s="1" t="s">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
+        <v>6380</v>
+      </c>
+      <c r="B48" s="2">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="C48" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E48" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F39" s="1">
+      <c r="F48" s="2">
         <v>1.254</v>
       </c>
-      <c r="G39" s="1">
+      <c r="G48" s="2">
         <v>1.2709999999999999</v>
       </c>
-      <c r="H39" s="1">
+      <c r="H48" s="2">
         <v>1.288</v>
       </c>
-      <c r="I39" s="1">
+      <c r="I48" s="2">
         <v>0.47099999999999997</v>
       </c>
-      <c r="J39" s="1">
+      <c r="J48" s="2">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="K39" s="1">
+      <c r="K48" s="2">
         <v>0.438</v>
       </c>
-      <c r="L39" s="1">
+      <c r="L48" s="2">
         <v>6.0999999999999999E-2</v>
       </c>
-      <c r="M39" s="1">
+      <c r="M48" s="2">
         <v>-0.63600000000000001</v>
       </c>
-      <c r="N39" s="1">
+      <c r="N48" s="2">
         <v>6.0999999999999999E-2</v>
       </c>
-      <c r="O39" s="1">
+      <c r="O48" s="2">
         <v>0.24099999999999999</v>
       </c>
-      <c r="P39" s="1">
+      <c r="P48" s="2">
         <v>2.1999999999999999E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
-        <v>6380</v>
-      </c>
-      <c r="B40" s="1">
-        <v>4.3099999999999996</v>
-      </c>
-      <c r="C40" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E40" s="1" t="s">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A49" s="2">
+        <v>6380</v>
+      </c>
+      <c r="B49" s="2">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="C49" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E49" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F40" s="1">
+      <c r="F49" s="2">
         <v>1.288</v>
       </c>
-      <c r="G40" s="1">
+      <c r="G49" s="2">
         <v>1.306</v>
       </c>
-      <c r="H40" s="1">
+      <c r="H49" s="2">
         <v>1.323</v>
       </c>
-      <c r="I40" s="1">
+      <c r="I49" s="2">
         <v>0.495</v>
       </c>
-      <c r="J40" s="1">
+      <c r="J49" s="2">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="K40" s="1">
+      <c r="K49" s="2">
         <v>0.377</v>
       </c>
-      <c r="L40" s="1">
+      <c r="L49" s="2">
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="M40" s="1">
+      <c r="M49" s="2">
         <v>-0.57999999999999996</v>
       </c>
-      <c r="N40" s="1">
+      <c r="N49" s="2">
         <v>0.05</v>
       </c>
-      <c r="O40" s="1">
+      <c r="O49" s="2">
         <v>0.22700000000000001</v>
       </c>
-      <c r="P40" s="1">
+      <c r="P49" s="2">
         <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
-        <v>6380</v>
-      </c>
-      <c r="B41" s="1">
-        <v>4.3099999999999996</v>
-      </c>
-      <c r="C41" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E41" s="1" t="s">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A50" s="2">
+        <v>6380</v>
+      </c>
+      <c r="B50" s="2">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="C50" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E50" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F41" s="1">
+      <c r="F50" s="2">
         <v>1.323</v>
       </c>
-      <c r="G41" s="1">
+      <c r="G50" s="2">
         <v>1.341</v>
       </c>
-      <c r="H41" s="1">
+      <c r="H50" s="2">
         <v>1.3580000000000001</v>
       </c>
-      <c r="I41" s="1">
+      <c r="I50" s="2">
         <v>0.53600000000000003</v>
       </c>
-      <c r="J41" s="1">
+      <c r="J50" s="2">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="K41" s="1">
+      <c r="K50" s="2">
         <v>0.308</v>
       </c>
-      <c r="L41" s="1">
+      <c r="L50" s="2">
         <v>6.2E-2</v>
       </c>
-      <c r="M41" s="1">
+      <c r="M50" s="2">
         <v>-0.55300000000000005</v>
       </c>
-      <c r="N41" s="1">
+      <c r="N50" s="2">
         <v>6.3E-2</v>
       </c>
-      <c r="O41" s="1">
+      <c r="O50" s="2">
         <v>0.23</v>
       </c>
-      <c r="P41" s="1">
+      <c r="P50" s="2">
         <v>2.3E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A42" s="1">
-        <v>6380</v>
-      </c>
-      <c r="B42" s="1">
-        <v>4.3099999999999996</v>
-      </c>
-      <c r="C42" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E42" s="1" t="s">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A51" s="2">
+        <v>6380</v>
+      </c>
+      <c r="B51" s="2">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="C51" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E51" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F42" s="1">
+      <c r="F51" s="2">
         <v>1.3580000000000001</v>
       </c>
-      <c r="G42" s="1">
+      <c r="G51" s="2">
         <v>1.377</v>
       </c>
-      <c r="H42" s="1">
+      <c r="H51" s="2">
         <v>1.3955</v>
       </c>
-      <c r="I42" s="1">
+      <c r="I51" s="2">
         <v>0.59699999999999998</v>
       </c>
-      <c r="J42" s="1">
+      <c r="J51" s="2">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="K42" s="1">
+      <c r="K51" s="2">
         <v>0.184</v>
       </c>
-      <c r="L42" s="1">
+      <c r="L51" s="2">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="M42" s="1">
+      <c r="M51" s="2">
         <v>-0.45900000000000002</v>
       </c>
-      <c r="N42" s="1">
+      <c r="N51" s="2">
         <v>0.06</v>
       </c>
-      <c r="O42" s="1">
+      <c r="O51" s="2">
         <v>0.20300000000000001</v>
       </c>
-      <c r="P42" s="1">
+      <c r="P51" s="2">
         <v>2.1999999999999999E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A43" s="1">
-        <v>6380</v>
-      </c>
-      <c r="B43" s="1">
-        <v>4.3099999999999996</v>
-      </c>
-      <c r="C43" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E43" s="1" t="s">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A52" s="2">
+        <v>6380</v>
+      </c>
+      <c r="B52" s="2">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="C52" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E52" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F43" s="1">
+      <c r="F52" s="2">
         <v>1.3955</v>
       </c>
-      <c r="G43" s="1">
+      <c r="G52" s="2">
         <v>1.4139999999999999</v>
       </c>
-      <c r="H43" s="1">
+      <c r="H52" s="2">
         <v>1.4339999999999999</v>
       </c>
-      <c r="I43" s="1">
+      <c r="I52" s="2">
         <v>0.68200000000000005</v>
       </c>
-      <c r="J43" s="1">
+      <c r="J52" s="2">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="K43" s="1">
+      <c r="K52" s="2">
         <v>-1.2E-2</v>
       </c>
-      <c r="L43" s="1">
+      <c r="L52" s="2">
         <v>6.0999999999999999E-2</v>
       </c>
-      <c r="M43" s="1">
+      <c r="M52" s="2">
         <v>-0.28999999999999998</v>
       </c>
-      <c r="N43" s="1">
+      <c r="N52" s="2">
         <v>6.0999999999999999E-2</v>
       </c>
-      <c r="O43" s="1">
+      <c r="O52" s="2">
         <v>0.14799999999999999</v>
       </c>
-      <c r="P43" s="1">
+      <c r="P52" s="2">
         <v>2.1999999999999999E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A44" s="1">
-        <v>6380</v>
-      </c>
-      <c r="B44" s="1">
-        <v>4.3099999999999996</v>
-      </c>
-      <c r="C44" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E44" s="1" t="s">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A53" s="2">
+        <v>6380</v>
+      </c>
+      <c r="B53" s="2">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="C53" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E53" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F44" s="1">
+      <c r="F53" s="2">
         <v>1.4339999999999999</v>
       </c>
-      <c r="G44" s="1">
+      <c r="G53" s="2">
         <v>1.452</v>
       </c>
-      <c r="H44" s="1">
+      <c r="H53" s="2">
         <v>1.472</v>
       </c>
-      <c r="I44" s="1">
+      <c r="I53" s="2">
         <v>0.78600000000000003</v>
       </c>
-      <c r="J44" s="1">
+      <c r="J53" s="2">
         <v>1.9E-2</v>
       </c>
-      <c r="K44" s="1">
+      <c r="K53" s="2">
         <v>-0.24</v>
       </c>
-      <c r="L44" s="1">
+      <c r="L53" s="2">
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="M44" s="1">
+      <c r="M53" s="2">
         <v>-8.6999999999999994E-2</v>
       </c>
-      <c r="N44" s="1">
+      <c r="N53" s="2">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="O44" s="1">
+      <c r="O53" s="2">
         <v>0.08</v>
       </c>
-      <c r="P44" s="1">
+      <c r="P53" s="2">
         <v>1.6E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A45" s="1">
-        <v>6380</v>
-      </c>
-      <c r="B45" s="1">
-        <v>4.3099999999999996</v>
-      </c>
-      <c r="C45" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E45" s="1" t="s">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A54" s="2">
+        <v>6380</v>
+      </c>
+      <c r="B54" s="2">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="C54" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E54" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F45" s="1">
+      <c r="F54" s="2">
         <v>1.472</v>
       </c>
-      <c r="G45" s="1">
+      <c r="G54" s="2">
         <v>1.492</v>
       </c>
-      <c r="H45" s="1">
+      <c r="H54" s="2">
         <v>1.512</v>
       </c>
-      <c r="I45" s="1">
+      <c r="I54" s="2">
         <v>0.89</v>
       </c>
-      <c r="J45" s="1">
+      <c r="J54" s="2">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="K45" s="1">
+      <c r="K54" s="2">
         <v>-0.52</v>
       </c>
-      <c r="L45" s="1">
+      <c r="L54" s="2">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="M45" s="1">
+      <c r="M54" s="2">
         <v>0.19600000000000001</v>
       </c>
-      <c r="N45" s="1">
+      <c r="N54" s="2">
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="O45" s="1">
+      <c r="O54" s="2">
         <v>-2.5000000000000001E-2</v>
       </c>
-      <c r="P45" s="1">
+      <c r="P54" s="2">
         <v>1.6E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A46" s="1">
-        <v>6380</v>
-      </c>
-      <c r="B46" s="1">
-        <v>4.3099999999999996</v>
-      </c>
-      <c r="C46" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E46" s="1" t="s">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A55" s="2">
+        <v>6380</v>
+      </c>
+      <c r="B55" s="2">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="C55" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E55" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F46" s="1">
+      <c r="F55" s="2">
         <v>1.512</v>
       </c>
-      <c r="G46" s="1">
+      <c r="G55" s="2">
         <v>1.532</v>
       </c>
-      <c r="H46" s="1">
+      <c r="H55" s="2">
         <v>1.5529999999999999</v>
       </c>
-      <c r="I46" s="1">
+      <c r="I55" s="2">
         <v>0.96399999999999997</v>
       </c>
-      <c r="J46" s="1">
+      <c r="J55" s="2">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="K46" s="1">
+      <c r="K55" s="2">
         <v>-0.69799999999999995</v>
       </c>
-      <c r="L46" s="1">
+      <c r="L55" s="2">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="M46" s="1">
+      <c r="M55" s="2">
         <v>0.34899999999999998</v>
       </c>
-      <c r="N46" s="1">
+      <c r="N55" s="2">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="O46" s="1">
+      <c r="O55" s="2">
         <v>-7.1999999999999995E-2</v>
       </c>
-      <c r="P46" s="1">
+      <c r="P55" s="2">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A47" s="1">
-        <v>6380</v>
-      </c>
-      <c r="B47" s="1">
-        <v>4.3099999999999996</v>
-      </c>
-      <c r="C47" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E47" s="1" t="s">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A56" s="2">
+        <v>6380</v>
+      </c>
+      <c r="B56" s="2">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="C56" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E56" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F47" s="1">
+      <c r="F56" s="2">
         <v>1.5529999999999999</v>
       </c>
-      <c r="G47" s="1">
+      <c r="G56" s="2">
         <v>1.573</v>
       </c>
-      <c r="H47" s="1">
+      <c r="H56" s="2">
         <v>1.595</v>
       </c>
-      <c r="I47" s="1">
+      <c r="I56" s="2">
         <v>0.99</v>
       </c>
-      <c r="J47" s="1">
+      <c r="J56" s="2">
         <v>0.01</v>
       </c>
-      <c r="K47" s="1">
+      <c r="K56" s="2">
         <v>-0.77200000000000002</v>
       </c>
-      <c r="L47" s="1">
+      <c r="L56" s="2">
         <v>2.4E-2</v>
       </c>
-      <c r="M47" s="1">
+      <c r="M56" s="2">
         <v>0.40300000000000002</v>
       </c>
-      <c r="N47" s="1">
+      <c r="N56" s="2">
         <v>2.4E-2</v>
       </c>
-      <c r="O47" s="1">
+      <c r="O56" s="2">
         <v>-8.5999999999999993E-2</v>
       </c>
-      <c r="P47" s="1">
+      <c r="P56" s="2">
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A48" s="1">
-        <v>6380</v>
-      </c>
-      <c r="B48" s="1">
-        <v>4.3099999999999996</v>
-      </c>
-      <c r="C48" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E48" s="1" t="s">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A57" s="2">
+        <v>6380</v>
+      </c>
+      <c r="B57" s="2">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="C57" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E57" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F48" s="1">
+      <c r="F57" s="2">
         <v>1.595</v>
       </c>
-      <c r="G48" s="1">
+      <c r="G57" s="2">
         <v>1.6160000000000001</v>
       </c>
-      <c r="H48" s="1">
+      <c r="H57" s="2">
         <v>1.6379999999999999</v>
       </c>
-      <c r="I48" s="1">
+      <c r="I57" s="2">
         <v>1.0149999999999999</v>
       </c>
-      <c r="J48" s="1">
+      <c r="J57" s="2">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="K48" s="1">
+      <c r="K57" s="2">
         <v>-0.84899999999999998</v>
       </c>
-      <c r="L48" s="1">
+      <c r="L57" s="2">
         <v>0.02</v>
       </c>
-      <c r="M48" s="1">
+      <c r="M57" s="2">
         <v>0.46300000000000002</v>
       </c>
-      <c r="N48" s="1">
+      <c r="N57" s="2">
         <v>0.02</v>
       </c>
-      <c r="O48" s="1">
+      <c r="O57" s="2">
         <v>-0.104</v>
       </c>
-      <c r="P48" s="1">
+      <c r="P57" s="2">
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A49" s="1">
-        <v>6380</v>
-      </c>
-      <c r="B49" s="1">
-        <v>4.3099999999999996</v>
-      </c>
-      <c r="C49" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E49" s="1" t="s">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A58" s="2">
+        <v>6380</v>
+      </c>
+      <c r="B58" s="2">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="C58" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E58" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F49" s="1">
+      <c r="F58" s="2">
         <v>1.6379999999999999</v>
       </c>
-      <c r="G49" s="1">
+      <c r="G58" s="2">
         <v>1.659</v>
       </c>
-      <c r="H49" s="1">
+      <c r="H58" s="2">
         <v>1.6819999999999999</v>
       </c>
-      <c r="I49" s="1">
+      <c r="I58" s="2">
         <v>1.0229999999999999</v>
       </c>
-      <c r="J49" s="1">
+      <c r="J58" s="2">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="K49" s="1">
+      <c r="K58" s="2">
         <v>-0.872</v>
       </c>
-      <c r="L49" s="1">
+      <c r="L58" s="2">
         <v>1.4E-2</v>
       </c>
-      <c r="M49" s="1">
+      <c r="M58" s="2">
         <v>0.495</v>
       </c>
-      <c r="N49" s="1">
+      <c r="N58" s="2">
         <v>1.4E-2</v>
       </c>
-      <c r="O49" s="1">
+      <c r="O58" s="2">
         <v>-0.11899999999999999</v>
       </c>
-      <c r="P49" s="1">
+      <c r="P58" s="2">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A50" s="1">
-        <v>6380</v>
-      </c>
-      <c r="B50" s="1">
-        <v>4.3099999999999996</v>
-      </c>
-      <c r="C50" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E50" s="1" t="s">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A59" s="2">
+        <v>6380</v>
+      </c>
+      <c r="B59" s="2">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="C59" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E59" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F50" s="1">
+      <c r="F59" s="2">
         <v>1.6819999999999999</v>
       </c>
-      <c r="G50" s="1">
+      <c r="G59" s="2">
         <v>1.704</v>
       </c>
-      <c r="H50" s="1">
+      <c r="H59" s="2">
         <v>1.728</v>
       </c>
-      <c r="I50" s="1">
+      <c r="I59" s="2">
         <v>0.96</v>
       </c>
-      <c r="J50" s="1">
+      <c r="J59" s="2">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="K50" s="1">
+      <c r="K59" s="2">
         <v>-0.77</v>
       </c>
-      <c r="L50" s="1">
+      <c r="L59" s="2">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="M50" s="1">
+      <c r="M59" s="2">
         <v>0.39600000000000002</v>
       </c>
-      <c r="N50" s="1">
+      <c r="N59" s="2">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="O50" s="1">
+      <c r="O59" s="2">
         <v>-8.3000000000000004E-2</v>
       </c>
-      <c r="P50" s="1">
+      <c r="P59" s="2">
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A51" s="1">
-        <v>6380</v>
-      </c>
-      <c r="B51" s="1">
-        <v>4.3099999999999996</v>
-      </c>
-      <c r="C51" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E51" s="1" t="s">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A60" s="2">
+        <v>6380</v>
+      </c>
+      <c r="B60" s="2">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="C60" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E60" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F51" s="1">
+      <c r="F60" s="2">
         <v>1.728</v>
       </c>
-      <c r="G51" s="1">
+      <c r="G60" s="2">
         <v>1.7509999999999999</v>
       </c>
-      <c r="H51" s="1">
+      <c r="H60" s="2">
         <v>1.7729999999999999</v>
       </c>
-      <c r="I51" s="1">
+      <c r="I60" s="2">
         <v>0.90600000000000003</v>
       </c>
-      <c r="J51" s="1">
+      <c r="J60" s="2">
         <v>1.4E-2</v>
       </c>
-      <c r="K51" s="1">
+      <c r="K60" s="2">
         <v>-0.68</v>
       </c>
-      <c r="L51" s="1">
+      <c r="L60" s="2">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="M51" s="1">
+      <c r="M60" s="2">
         <v>0.31</v>
       </c>
-      <c r="N51" s="1">
+      <c r="N60" s="2">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="O51" s="1">
+      <c r="O60" s="2">
         <v>-5.2999999999999999E-2</v>
       </c>
-      <c r="P51" s="1">
+      <c r="P60" s="2">
         <v>1.2E-2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Gráficos para o paper
</commit_message>
<xml_diff>
--- a/ExoCTK_results.xlsx
+++ b/ExoCTK_results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Meu Drive\StarsAndExoplanets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meu Drive\StarsAndExoplanets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE6B0B6A-195E-4EE2-9AC9-DBC01E529048}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EE7D566-2526-4CDD-9E7C-BA66D6BC4E28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{FD485E45-5400-4809-8075-6517CC8BF8A4}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{FD485E45-5400-4809-8075-6517CC8BF8A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -168,7 +168,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -467,15 +467,15 @@
   <dimension ref="A1:P60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="20.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -525,7 +525,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
@@ -575,7 +575,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>6380</v>
       </c>
@@ -625,7 +625,7 @@
         <v>1.2E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>6380</v>
       </c>
@@ -675,7 +675,7 @@
         <v>1.2E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>6380</v>
       </c>
@@ -725,7 +725,7 @@
         <v>2.1000000000000001E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>6380</v>
       </c>
@@ -775,7 +775,7 @@
         <v>1.7000000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>6380</v>
       </c>
@@ -825,7 +825,7 @@
         <v>2.1000000000000001E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>6380</v>
       </c>
@@ -875,7 +875,7 @@
         <v>2.3E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>6380</v>
       </c>
@@ -925,7 +925,7 @@
         <v>1.2E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>6380</v>
       </c>
@@ -975,7 +975,7 @@
         <v>2.3E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>6380</v>
       </c>
@@ -1025,7 +1025,7 @@
         <v>3.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>6380</v>
       </c>
@@ -1075,7 +1075,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>6380</v>
       </c>
@@ -1125,7 +1125,7 @@
         <v>2.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>6380</v>
       </c>
@@ -1175,7 +1175,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>6380</v>
       </c>
@@ -1225,7 +1225,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>6380</v>
       </c>
@@ -1275,7 +1275,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>6380</v>
       </c>
@@ -1325,7 +1325,7 @@
         <v>4.1000000000000002E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>6380</v>
       </c>
@@ -1375,7 +1375,7 @@
         <v>4.2999999999999997E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>6380</v>
       </c>
@@ -1425,7 +1425,7 @@
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>6380</v>
       </c>
@@ -1475,7 +1475,7 @@
         <v>4.1000000000000002E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>6380</v>
       </c>
@@ -1525,7 +1525,7 @@
         <v>3.9E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>6380</v>
       </c>
@@ -1575,7 +1575,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>6380</v>
       </c>
@@ -1625,7 +1625,7 @@
         <v>3.2000000000000001E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>6380</v>
       </c>
@@ -1675,7 +1675,7 @@
         <v>2.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>6380</v>
       </c>
@@ -1725,7 +1725,7 @@
         <v>2.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>6380</v>
       </c>
@@ -1775,7 +1775,7 @@
         <v>2.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>6380</v>
       </c>
@@ -1825,7 +1825,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>6380</v>
       </c>
@@ -1875,7 +1875,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>6380</v>
       </c>
@@ -1925,7 +1925,7 @@
         <v>1.7000000000000001E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>6380</v>
       </c>
@@ -1975,7 +1975,7 @@
         <v>1.6E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>6380</v>
       </c>
@@ -2025,7 +2025,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>6380</v>
       </c>
@@ -2075,7 +2075,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>6380</v>
       </c>
@@ -2125,7 +2125,7 @@
         <v>2.1000000000000001E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>6380</v>
       </c>
@@ -2175,7 +2175,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>6380</v>
       </c>
@@ -2225,7 +2225,7 @@
         <v>1.9E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>6380</v>
       </c>
@@ -2275,7 +2275,7 @@
         <v>1.6E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>6380</v>
       </c>
@@ -2325,7 +2325,7 @@
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>6380</v>
       </c>
@@ -2375,7 +2375,7 @@
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>6380</v>
       </c>
@@ -2425,7 +2425,7 @@
         <v>1.6E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>6380</v>
       </c>
@@ -2475,7 +2475,7 @@
         <v>1.6E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>6380</v>
       </c>
@@ -2525,7 +2525,7 @@
         <v>1.6E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>6380</v>
       </c>
@@ -2575,7 +2575,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>6380</v>
       </c>
@@ -2625,7 +2625,7 @@
         <v>1.9E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>6380</v>
       </c>
@@ -2675,7 +2675,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>6380</v>
       </c>
@@ -2725,7 +2725,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>6380</v>
       </c>
@@ -2775,7 +2775,7 @@
         <v>2.3E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>6380</v>
       </c>
@@ -2825,7 +2825,7 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>6380</v>
       </c>
@@ -2875,7 +2875,7 @@
         <v>2.1999999999999999E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>6380</v>
       </c>
@@ -2925,7 +2925,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
         <v>6380</v>
       </c>
@@ -2975,7 +2975,7 @@
         <v>2.3E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
         <v>6380</v>
       </c>
@@ -3025,7 +3025,7 @@
         <v>2.1999999999999999E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
         <v>6380</v>
       </c>
@@ -3075,7 +3075,7 @@
         <v>2.1999999999999999E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
         <v>6380</v>
       </c>
@@ -3125,7 +3125,7 @@
         <v>1.6E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
         <v>6380</v>
       </c>
@@ -3175,7 +3175,7 @@
         <v>1.6E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
         <v>6380</v>
       </c>
@@ -3225,7 +3225,7 @@
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
         <v>6380</v>
       </c>
@@ -3275,7 +3275,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
         <v>6380</v>
       </c>
@@ -3325,7 +3325,7 @@
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
         <v>6380</v>
       </c>
@@ -3375,7 +3375,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
         <v>6380</v>
       </c>
@@ -3425,7 +3425,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
         <v>6380</v>
       </c>

</xml_diff>

<commit_message>
Simulações para GJ 9827 d
</commit_message>
<xml_diff>
--- a/ExoCTK_results.xlsx
+++ b/ExoCTK_results.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Meu Drive\StarsAndExoplanets\Exoplanets\GJ9827d\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Meu Drive\StarsAndExoplanets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E46F3774-C416-49A6-A7CE-7CE3E9E29D1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B628FA7-F4E4-449C-9874-2DC77259083E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{FD485E45-5400-4809-8075-6517CC8BF8A4}"/>
   </bookViews>
@@ -149,10 +149,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -471,7 +470,7 @@
   <dimension ref="A1:P66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K70" sqref="K70"/>
+      <selection activeCell="Y15" sqref="Y15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3477,302 +3476,302 @@
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A61" s="2">
-        <v>4340</v>
-      </c>
-      <c r="B61" s="2">
-        <v>4.66</v>
-      </c>
-      <c r="C61" s="2">
-        <v>-0.26</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E61" s="2" t="s">
+      <c r="A61" s="1">
+        <v>4340</v>
+      </c>
+      <c r="B61" s="1">
+        <v>4.66</v>
+      </c>
+      <c r="C61" s="1">
+        <v>-0.26</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E61" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F61" s="2">
+      <c r="F61" s="1">
         <v>1.9610000000000001</v>
       </c>
-      <c r="G61" s="2">
+      <c r="G61" s="1">
         <v>2.0979999999999999</v>
       </c>
-      <c r="H61" s="2">
+      <c r="H61" s="1">
         <v>2.2320000000000002</v>
       </c>
-      <c r="I61" s="2">
+      <c r="I61" s="1">
         <v>0.7</v>
       </c>
-      <c r="J61" s="2">
+      <c r="J61" s="1">
         <v>0.04</v>
       </c>
-      <c r="K61" s="2">
+      <c r="K61" s="1">
         <v>-5.8999999999999997E-2</v>
       </c>
-      <c r="L61" s="2">
+      <c r="L61" s="1">
         <v>9.4E-2</v>
       </c>
-      <c r="M61" s="2">
+      <c r="M61" s="1">
         <v>-0.20300000000000001</v>
       </c>
-      <c r="N61" s="2">
+      <c r="N61" s="1">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="O61" s="2">
+      <c r="O61" s="1">
         <v>0.104</v>
       </c>
-      <c r="P61" s="2">
+      <c r="P61" s="1">
         <v>3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A62" s="2">
-        <v>4340</v>
-      </c>
-      <c r="B62" s="2">
-        <v>4.66</v>
-      </c>
-      <c r="C62" s="2">
-        <v>-0.26</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E62" s="2" t="s">
+      <c r="A62" s="1">
+        <v>4340</v>
+      </c>
+      <c r="B62" s="1">
+        <v>4.66</v>
+      </c>
+      <c r="C62" s="1">
+        <v>-0.26</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E62" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F62" s="2">
+      <c r="F62" s="1">
         <v>2.879</v>
       </c>
-      <c r="G62" s="2">
+      <c r="G62" s="1">
         <v>2.9380000000000002</v>
       </c>
-      <c r="H62" s="2">
+      <c r="H62" s="1">
         <v>2.9980000000000002</v>
       </c>
-      <c r="I62" s="2">
+      <c r="I62" s="1">
         <v>0.51300000000000001</v>
       </c>
-      <c r="J62" s="2">
+      <c r="J62" s="1">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="K62" s="2">
+      <c r="K62" s="1">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="L62" s="2">
+      <c r="L62" s="1">
         <v>9.7000000000000003E-2</v>
       </c>
-      <c r="M62" s="2">
+      <c r="M62" s="1">
         <v>-0.18099999999999999</v>
       </c>
-      <c r="N62" s="2">
+      <c r="N62" s="1">
         <v>9.7000000000000003E-2</v>
       </c>
-      <c r="O62" s="2">
+      <c r="O62" s="1">
         <v>8.7999999999999995E-2</v>
       </c>
-      <c r="P62" s="2">
+      <c r="P62" s="1">
         <v>3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A63" s="2">
-        <v>4340</v>
-      </c>
-      <c r="B63" s="2">
-        <v>4.66</v>
-      </c>
-      <c r="C63" s="2">
-        <v>-0.26</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E63" s="2" t="s">
+      <c r="A63" s="1">
+        <v>4340</v>
+      </c>
+      <c r="B63" s="1">
+        <v>4.66</v>
+      </c>
+      <c r="C63" s="1">
+        <v>-0.26</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E63" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F63" s="2">
+      <c r="F63" s="1">
         <v>3.0019999999999998</v>
       </c>
-      <c r="G63" s="2">
+      <c r="G63" s="1">
         <v>3.06</v>
       </c>
-      <c r="H63" s="2">
+      <c r="H63" s="1">
         <v>3.121</v>
       </c>
-      <c r="I63" s="2">
+      <c r="I63" s="1">
         <v>0.48299999999999998</v>
       </c>
-      <c r="J63" s="2">
+      <c r="J63" s="1">
         <v>4.7E-2</v>
       </c>
-      <c r="K63" s="2">
+      <c r="K63" s="1">
         <v>4.5999999999999999E-2</v>
       </c>
-      <c r="L63" s="2">
+      <c r="L63" s="1">
         <v>0.111</v>
       </c>
-      <c r="M63" s="2">
+      <c r="M63" s="1">
         <v>-0.222</v>
       </c>
-      <c r="N63" s="2">
+      <c r="N63" s="1">
         <v>0.112</v>
       </c>
-      <c r="O63" s="2">
+      <c r="O63" s="1">
         <v>0.105</v>
       </c>
-      <c r="P63" s="2">
+      <c r="P63" s="1">
         <v>4.1000000000000002E-2</v>
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A64" s="2">
-        <v>4340</v>
-      </c>
-      <c r="B64" s="2">
-        <v>4.66</v>
-      </c>
-      <c r="C64" s="2">
-        <v>-0.26</v>
-      </c>
-      <c r="D64" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E64" s="2" t="s">
+      <c r="A64" s="1">
+        <v>4340</v>
+      </c>
+      <c r="B64" s="1">
+        <v>4.66</v>
+      </c>
+      <c r="C64" s="1">
+        <v>-0.26</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E64" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F64" s="2">
+      <c r="F64" s="1">
         <v>3.125</v>
       </c>
-      <c r="G64" s="2">
+      <c r="G64" s="1">
         <v>3.1840000000000002</v>
       </c>
-      <c r="H64" s="2">
+      <c r="H64" s="1">
         <v>3.2440000000000002</v>
       </c>
-      <c r="I64" s="2">
+      <c r="I64" s="1">
         <v>0.47199999999999998</v>
       </c>
-      <c r="J64" s="2">
+      <c r="J64" s="1">
         <v>4.5999999999999999E-2</v>
       </c>
-      <c r="K64" s="2">
+      <c r="K64" s="1">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="L64" s="2">
+      <c r="L64" s="1">
         <v>0.109</v>
       </c>
-      <c r="M64" s="2">
+      <c r="M64" s="1">
         <v>-0.20200000000000001</v>
       </c>
-      <c r="N64" s="2">
+      <c r="N64" s="1">
         <v>0.11</v>
       </c>
-      <c r="O64" s="2">
+      <c r="O64" s="1">
         <v>9.7000000000000003E-2</v>
       </c>
-      <c r="P64" s="2">
+      <c r="P64" s="1">
         <v>0.04</v>
       </c>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A65" s="2">
-        <v>4340</v>
-      </c>
-      <c r="B65" s="2">
-        <v>4.66</v>
-      </c>
-      <c r="C65" s="2">
-        <v>-0.26</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E65" s="2" t="s">
+      <c r="A65" s="1">
+        <v>4340</v>
+      </c>
+      <c r="B65" s="1">
+        <v>4.66</v>
+      </c>
+      <c r="C65" s="1">
+        <v>-0.26</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E65" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F65" s="2">
+      <c r="F65" s="1">
         <v>3.2480000000000002</v>
       </c>
-      <c r="G65" s="2">
+      <c r="G65" s="1">
         <v>3.3069999999999999</v>
       </c>
-      <c r="H65" s="2">
+      <c r="H65" s="1">
         <v>3.367</v>
       </c>
-      <c r="I65" s="2">
+      <c r="I65" s="1">
         <v>0.47</v>
       </c>
-      <c r="J65" s="2">
+      <c r="J65" s="1">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="K65" s="2">
+      <c r="K65" s="1">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="L65" s="2">
+      <c r="L65" s="1">
         <v>0.10100000000000001</v>
       </c>
-      <c r="M65" s="2">
+      <c r="M65" s="1">
         <v>-0.16800000000000001</v>
       </c>
-      <c r="N65" s="2">
+      <c r="N65" s="1">
         <v>0.10199999999999999</v>
       </c>
-      <c r="O65" s="2">
+      <c r="O65" s="1">
         <v>8.4000000000000005E-2</v>
       </c>
-      <c r="P65" s="2">
+      <c r="P65" s="1">
         <v>3.6999999999999998E-2</v>
       </c>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A66" s="2">
-        <v>4340</v>
-      </c>
-      <c r="B66" s="2">
-        <v>4.66</v>
-      </c>
-      <c r="C66" s="2">
-        <v>-0.26</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E66" s="2" t="s">
+      <c r="A66" s="1">
+        <v>4340</v>
+      </c>
+      <c r="B66" s="1">
+        <v>4.66</v>
+      </c>
+      <c r="C66" s="1">
+        <v>-0.26</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E66" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F66" s="2">
+      <c r="F66" s="1">
         <v>3.371</v>
       </c>
-      <c r="G66" s="2">
+      <c r="G66" s="1">
         <v>3.43</v>
       </c>
-      <c r="H66" s="2">
+      <c r="H66" s="1">
         <v>3.49</v>
       </c>
-      <c r="I66" s="2">
+      <c r="I66" s="1">
         <v>0.442</v>
       </c>
-      <c r="J66" s="2">
+      <c r="J66" s="1">
         <v>4.5999999999999999E-2</v>
       </c>
-      <c r="K66" s="2">
+      <c r="K66" s="1">
         <v>0.04</v>
       </c>
-      <c r="L66" s="2">
+      <c r="L66" s="1">
         <v>0.11</v>
       </c>
-      <c r="M66" s="2">
+      <c r="M66" s="1">
         <v>-0.20100000000000001</v>
       </c>
-      <c r="N66" s="2">
+      <c r="N66" s="1">
         <v>0.11</v>
       </c>
-      <c r="O66" s="2">
+      <c r="O66" s="1">
         <v>9.7000000000000003E-2</v>
       </c>
-      <c r="P66" s="2">
+      <c r="P66" s="1">
         <v>0.04</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Simulações para WASP-74 b
</commit_message>
<xml_diff>
--- a/ExoCTK_results.xlsx
+++ b/ExoCTK_results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Meu Drive\StarsAndExoplanets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03A2E36A-E149-49C1-8C11-E49F8F011F05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E271667-0C85-4A1B-A01C-B5564B004FEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{FD485E45-5400-4809-8075-6517CC8BF8A4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="26">
   <si>
     <t>Teff</t>
   </si>
@@ -93,13 +93,13 @@
     <t>4-parameter</t>
   </si>
   <si>
+    <t>HST/WFC3_IR.G141</t>
+  </si>
+  <si>
     <t>----------</t>
   </si>
   <si>
     <t>STIS.G430L</t>
-  </si>
-  <si>
-    <t>HST/WFC3_IR.G141</t>
   </si>
   <si>
     <t>STIS.G750L</t>
@@ -461,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E7459B0-01F0-423D-9E42-EFF86DA61453}">
-  <dimension ref="A1:P66"/>
+  <dimension ref="A1:P42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V12" sqref="V12"/>
+      <selection activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,7 +533,7 @@
         <v>18</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>19</v>
@@ -545,25 +545,25 @@
         <v>19</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>20</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>20</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>20</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>20</v>
@@ -571,263 +571,263 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>5172</v>
+        <v>5990</v>
       </c>
       <c r="B3" s="1">
-        <v>4.43</v>
+        <v>4.3899999999999997</v>
       </c>
       <c r="C3" s="1">
-        <v>0.35</v>
+        <v>0.39</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F3" s="1">
-        <v>0.40039999999999998</v>
+        <v>0.47</v>
       </c>
       <c r="G3" s="1">
-        <v>0.41770000000000002</v>
+        <v>0.48699999999999999</v>
       </c>
       <c r="H3" s="1">
-        <v>0.43480000000000002</v>
+        <v>0.504</v>
       </c>
       <c r="I3" s="1">
-        <v>0.60399999999999998</v>
+        <v>-0.12</v>
       </c>
       <c r="J3" s="1">
-        <v>2.1000000000000001E-2</v>
+        <v>1.4E-2</v>
       </c>
       <c r="K3" s="1">
-        <v>-0.88200000000000001</v>
+        <v>1.621</v>
       </c>
       <c r="L3" s="1">
-        <v>0.05</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="M3" s="1">
-        <v>1.8069999999999999</v>
+        <v>-0.96899999999999997</v>
       </c>
       <c r="N3" s="1">
-        <v>5.0999999999999997E-2</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="O3" s="1">
-        <v>-0.59699999999999998</v>
+        <v>0.24199999999999999</v>
       </c>
       <c r="P3" s="1">
-        <v>1.9E-2</v>
+        <v>1.2E-2</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>5172</v>
+        <v>5990</v>
       </c>
       <c r="B4" s="1">
-        <v>4.43</v>
+        <v>4.3899999999999997</v>
       </c>
       <c r="C4" s="1">
-        <v>0.35</v>
+        <v>0.39</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F4" s="1">
-        <v>0.435</v>
+        <v>0.505</v>
       </c>
       <c r="G4" s="1">
-        <v>0.4521</v>
+        <v>0.52149999999999996</v>
       </c>
       <c r="H4" s="1">
-        <v>0.46920000000000001</v>
+        <v>0.53900000000000003</v>
       </c>
       <c r="I4" s="1">
-        <v>0.309</v>
+        <v>-5.6000000000000001E-2</v>
       </c>
       <c r="J4" s="1">
-        <v>3.7999999999999999E-2</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="K4" s="1">
-        <v>-2.1000000000000001E-2</v>
+        <v>1.44</v>
       </c>
       <c r="L4" s="1">
-        <v>0.09</v>
+        <v>3.1E-2</v>
       </c>
       <c r="M4" s="1">
-        <v>1.008</v>
+        <v>-0.84899999999999998</v>
       </c>
       <c r="N4" s="1">
-        <v>9.0999999999999998E-2</v>
+        <v>3.1E-2</v>
       </c>
       <c r="O4" s="1">
-        <v>-0.40899999999999997</v>
+        <v>0.21099999999999999</v>
       </c>
       <c r="P4" s="1">
-        <v>3.3000000000000002E-2</v>
+        <v>1.0999999999999999E-2</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>5172</v>
+        <v>5990</v>
       </c>
       <c r="B5" s="1">
-        <v>4.43</v>
+        <v>4.3899999999999997</v>
       </c>
       <c r="C5" s="1">
-        <v>0.35</v>
+        <v>0.39</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F5" s="1">
-        <v>0.46970000000000001</v>
+        <v>0.53900000000000003</v>
       </c>
       <c r="G5" s="1">
-        <v>0.48680000000000001</v>
+        <v>0.55600000000000005</v>
       </c>
       <c r="H5" s="1">
-        <v>0.504</v>
+        <v>0.57299999999999995</v>
       </c>
       <c r="I5" s="1">
-        <v>0.23899999999999999</v>
+        <v>-6.5000000000000002E-2</v>
       </c>
       <c r="J5" s="1">
-        <v>4.2000000000000003E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="K5" s="1">
-        <v>0.23499999999999999</v>
+        <v>1.544</v>
       </c>
       <c r="L5" s="1">
-        <v>9.9000000000000005E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="M5" s="1">
-        <v>0.73199999999999998</v>
+        <v>-1.032</v>
       </c>
       <c r="N5" s="1">
-        <v>0.1</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="O5" s="1">
-        <v>-0.34899999999999998</v>
+        <v>0.27700000000000002</v>
       </c>
       <c r="P5" s="1">
-        <v>3.6999999999999998E-2</v>
+        <v>1.2999999999999999E-2</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>5172</v>
+        <v>5990</v>
       </c>
       <c r="B6" s="1">
-        <v>4.43</v>
+        <v>4.3899999999999997</v>
       </c>
       <c r="C6" s="1">
-        <v>0.35</v>
+        <v>0.39</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F6" s="1">
-        <v>0.504</v>
+        <v>0.55100000000000005</v>
       </c>
       <c r="G6" s="1">
-        <v>0.52149999999999996</v>
+        <v>0.5635</v>
       </c>
       <c r="H6" s="1">
-        <v>0.53859999999999997</v>
+        <v>0.57599999999999996</v>
       </c>
       <c r="I6" s="1">
-        <v>0.40400000000000003</v>
+        <v>-6.0999999999999999E-2</v>
       </c>
       <c r="J6" s="1">
-        <v>3.5999999999999997E-2</v>
+        <v>1.2E-2</v>
       </c>
       <c r="K6" s="1">
-        <v>-8.7999999999999995E-2</v>
+        <v>1.544</v>
       </c>
       <c r="L6" s="1">
-        <v>8.5000000000000006E-2</v>
+        <v>2.9000000000000001E-2</v>
       </c>
       <c r="M6" s="1">
-        <v>0.90200000000000002</v>
+        <v>-1.046</v>
       </c>
       <c r="N6" s="1">
-        <v>8.5999999999999993E-2</v>
+        <v>2.9000000000000001E-2</v>
       </c>
       <c r="O6" s="1">
-        <v>-0.378</v>
+        <v>0.28199999999999997</v>
       </c>
       <c r="P6" s="1">
-        <v>3.1E-2</v>
+        <v>1.0999999999999999E-2</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>5172</v>
+        <v>5990</v>
       </c>
       <c r="B7" s="1">
-        <v>4.43</v>
+        <v>4.3899999999999997</v>
       </c>
       <c r="C7" s="1">
-        <v>0.35</v>
+        <v>0.39</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F7" s="1">
-        <v>0.53900000000000003</v>
+        <v>0.57599999999999996</v>
       </c>
       <c r="G7" s="1">
-        <v>0.55600000000000005</v>
+        <v>0.58840000000000003</v>
       </c>
       <c r="H7" s="1">
-        <v>0.57299999999999995</v>
+        <v>0.60099999999999998</v>
       </c>
       <c r="I7" s="1">
-        <v>0.318</v>
+        <v>-0.08</v>
       </c>
       <c r="J7" s="1">
-        <v>3.9E-2</v>
+        <v>1.4E-2</v>
       </c>
       <c r="K7" s="1">
-        <v>0.24199999999999999</v>
+        <v>1.623</v>
       </c>
       <c r="L7" s="1">
-        <v>9.2999999999999999E-2</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="M7" s="1">
-        <v>0.53200000000000003</v>
+        <v>-1.165</v>
       </c>
       <c r="N7" s="1">
-        <v>9.2999999999999999E-2</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="O7" s="1">
-        <v>-0.27400000000000002</v>
+        <v>0.32500000000000001</v>
       </c>
       <c r="P7" s="1">
-        <v>3.4000000000000002E-2</v>
+        <v>1.2E-2</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>5172</v>
+        <v>5990</v>
       </c>
       <c r="B8" s="1">
-        <v>4.43</v>
+        <v>4.3899999999999997</v>
       </c>
       <c r="C8" s="1">
-        <v>0.35</v>
+        <v>0.39</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>21</v>
@@ -836,48 +836,48 @@
         <v>25</v>
       </c>
       <c r="F8" s="1">
-        <v>0.55100000000000005</v>
+        <v>0.60160000000000002</v>
       </c>
       <c r="G8" s="1">
-        <v>0.5635</v>
+        <v>0.61399999999999999</v>
       </c>
       <c r="H8" s="1">
-        <v>0.57599999999999996</v>
+        <v>0.626</v>
       </c>
       <c r="I8" s="1">
-        <v>0.318</v>
+        <v>-3.7999999999999999E-2</v>
       </c>
       <c r="J8" s="1">
-        <v>3.9E-2</v>
+        <v>1.4E-2</v>
       </c>
       <c r="K8" s="1">
-        <v>0.26</v>
+        <v>1.512</v>
       </c>
       <c r="L8" s="1">
-        <v>9.1999999999999998E-2</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="M8" s="1">
-        <v>0.503</v>
+        <v>-1.0860000000000001</v>
       </c>
       <c r="N8" s="1">
-        <v>9.2999999999999999E-2</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="O8" s="1">
-        <v>-0.26800000000000002</v>
+        <v>0.29899999999999999</v>
       </c>
       <c r="P8" s="1">
-        <v>3.4000000000000002E-2</v>
+        <v>1.2E-2</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>5172</v>
+        <v>5990</v>
       </c>
       <c r="B9" s="1">
-        <v>4.43</v>
+        <v>4.3899999999999997</v>
       </c>
       <c r="C9" s="1">
-        <v>0.35</v>
+        <v>0.39</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>21</v>
@@ -886,48 +886,48 @@
         <v>25</v>
       </c>
       <c r="F9" s="1">
-        <v>0.57599999999999996</v>
+        <v>0.627</v>
       </c>
       <c r="G9" s="1">
-        <v>0.58840000000000003</v>
+        <v>0.63900000000000001</v>
       </c>
       <c r="H9" s="1">
-        <v>0.60099999999999998</v>
+        <v>0.65139999999999998</v>
       </c>
       <c r="I9" s="1">
-        <v>0.29399999999999998</v>
+        <v>-2.1000000000000001E-2</v>
       </c>
       <c r="J9" s="1">
-        <v>3.4000000000000002E-2</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="K9" s="1">
-        <v>0.35099999999999998</v>
+        <v>1.472</v>
       </c>
       <c r="L9" s="1">
-        <v>8.2000000000000003E-2</v>
+        <v>0.04</v>
       </c>
       <c r="M9" s="1">
-        <v>0.38300000000000001</v>
+        <v>-1.0720000000000001</v>
       </c>
       <c r="N9" s="1">
-        <v>8.2000000000000003E-2</v>
+        <v>4.1000000000000002E-2</v>
       </c>
       <c r="O9" s="1">
-        <v>-0.23</v>
+        <v>0.29299999999999998</v>
       </c>
       <c r="P9" s="1">
-        <v>0.03</v>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>5172</v>
+        <v>5990</v>
       </c>
       <c r="B10" s="1">
-        <v>4.43</v>
+        <v>4.3899999999999997</v>
       </c>
       <c r="C10" s="1">
-        <v>0.35</v>
+        <v>0.39</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>21</v>
@@ -936,48 +936,48 @@
         <v>25</v>
       </c>
       <c r="F10" s="1">
-        <v>0.60160000000000002</v>
+        <v>0.65200000000000002</v>
       </c>
       <c r="G10" s="1">
-        <v>0.61399999999999999</v>
+        <v>0.66459999999999997</v>
       </c>
       <c r="H10" s="1">
-        <v>0.626</v>
+        <v>0.67700000000000005</v>
       </c>
       <c r="I10" s="1">
-        <v>0.33400000000000002</v>
+        <v>-8.0000000000000002E-3</v>
       </c>
       <c r="J10" s="1">
-        <v>3.4000000000000002E-2</v>
+        <v>1.9E-2</v>
       </c>
       <c r="K10" s="1">
-        <v>0.29499999999999998</v>
+        <v>1.466</v>
       </c>
       <c r="L10" s="1">
-        <v>0.08</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="M10" s="1">
-        <v>0.379</v>
+        <v>-1.107</v>
       </c>
       <c r="N10" s="1">
-        <v>0.08</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="O10" s="1">
-        <v>-0.223</v>
+        <v>0.30299999999999999</v>
       </c>
       <c r="P10" s="1">
-        <v>2.9000000000000001E-2</v>
+        <v>1.6E-2</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>5172</v>
+        <v>5990</v>
       </c>
       <c r="B11" s="1">
-        <v>4.43</v>
+        <v>4.3899999999999997</v>
       </c>
       <c r="C11" s="1">
-        <v>0.35</v>
+        <v>0.39</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>21</v>
@@ -986,48 +986,48 @@
         <v>25</v>
       </c>
       <c r="F11" s="1">
-        <v>0.627</v>
+        <v>0.67700000000000005</v>
       </c>
       <c r="G11" s="1">
-        <v>0.63900000000000001</v>
+        <v>0.6895</v>
       </c>
       <c r="H11" s="1">
-        <v>0.65139999999999998</v>
+        <v>0.70199999999999996</v>
       </c>
       <c r="I11" s="1">
-        <v>0.35299999999999998</v>
+        <v>-3.0000000000000001E-3</v>
       </c>
       <c r="J11" s="1">
-        <v>3.5000000000000003E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="K11" s="1">
-        <v>0.25700000000000001</v>
+        <v>1.405</v>
       </c>
       <c r="L11" s="1">
-        <v>8.3000000000000004E-2</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="M11" s="1">
-        <v>0.38</v>
+        <v>-1.052</v>
       </c>
       <c r="N11" s="1">
-        <v>8.4000000000000005E-2</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="O11" s="1">
-        <v>-0.221</v>
+        <v>0.29299999999999998</v>
       </c>
       <c r="P11" s="1">
-        <v>3.1E-2</v>
+        <v>1.9E-2</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>5172</v>
+        <v>5990</v>
       </c>
       <c r="B12" s="1">
-        <v>4.43</v>
+        <v>4.3899999999999997</v>
       </c>
       <c r="C12" s="1">
-        <v>0.35</v>
+        <v>0.39</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>21</v>
@@ -1036,48 +1036,48 @@
         <v>25</v>
       </c>
       <c r="F12" s="1">
-        <v>0.65200000000000002</v>
+        <v>0.7026</v>
       </c>
       <c r="G12" s="1">
-        <v>0.66459999999999997</v>
+        <v>0.71499999999999997</v>
       </c>
       <c r="H12" s="1">
-        <v>0.67700000000000005</v>
+        <v>0.72699999999999998</v>
       </c>
       <c r="I12" s="1">
-        <v>0.35199999999999998</v>
+        <v>3.9E-2</v>
       </c>
       <c r="J12" s="1">
-        <v>3.3000000000000002E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="K12" s="1">
-        <v>0.28799999999999998</v>
+        <v>1.286</v>
       </c>
       <c r="L12" s="1">
-        <v>7.6999999999999999E-2</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="M12" s="1">
-        <v>0.315</v>
+        <v>-0.95299999999999996</v>
       </c>
       <c r="N12" s="1">
-        <v>7.8E-2</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="O12" s="1">
-        <v>-0.20300000000000001</v>
+        <v>0.26</v>
       </c>
       <c r="P12" s="1">
-        <v>2.8000000000000001E-2</v>
+        <v>1.9E-2</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>5172</v>
+        <v>5990</v>
       </c>
       <c r="B13" s="1">
-        <v>4.43</v>
+        <v>4.3899999999999997</v>
       </c>
       <c r="C13" s="1">
-        <v>0.35</v>
+        <v>0.39</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>21</v>
@@ -1086,48 +1086,48 @@
         <v>25</v>
       </c>
       <c r="F13" s="1">
-        <v>0.67700000000000005</v>
+        <v>0.72799999999999998</v>
       </c>
       <c r="G13" s="1">
-        <v>0.6895</v>
+        <v>0.74</v>
       </c>
       <c r="H13" s="1">
-        <v>0.70199999999999996</v>
+        <v>0.75239999999999996</v>
       </c>
       <c r="I13" s="1">
-        <v>0.39400000000000002</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="J13" s="1">
-        <v>2.8000000000000001E-2</v>
+        <v>0.02</v>
       </c>
       <c r="K13" s="1">
-        <v>0.193</v>
+        <v>1.208</v>
       </c>
       <c r="L13" s="1">
-        <v>6.7000000000000004E-2</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="M13" s="1">
-        <v>0.36499999999999999</v>
+        <v>-0.9</v>
       </c>
       <c r="N13" s="1">
-        <v>6.8000000000000005E-2</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="O13" s="1">
-        <v>-0.20799999999999999</v>
+        <v>0.24299999999999999</v>
       </c>
       <c r="P13" s="1">
-        <v>2.5000000000000001E-2</v>
+        <v>1.7000000000000001E-2</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>5172</v>
+        <v>5990</v>
       </c>
       <c r="B14" s="1">
-        <v>4.43</v>
+        <v>4.3899999999999997</v>
       </c>
       <c r="C14" s="1">
-        <v>0.35</v>
+        <v>0.39</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>21</v>
@@ -1136,48 +1136,48 @@
         <v>25</v>
       </c>
       <c r="F14" s="1">
-        <v>0.7026</v>
+        <v>0.753</v>
       </c>
       <c r="G14" s="1">
-        <v>0.71499999999999997</v>
+        <v>0.76500000000000001</v>
       </c>
       <c r="H14" s="1">
-        <v>0.72699999999999998</v>
+        <v>0.77800000000000002</v>
       </c>
       <c r="I14" s="1">
-        <v>0.42</v>
+        <v>5.8999999999999997E-2</v>
       </c>
       <c r="J14" s="1">
-        <v>0.03</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="K14" s="1">
-        <v>0.13300000000000001</v>
+        <v>1.23</v>
       </c>
       <c r="L14" s="1">
-        <v>7.0999999999999994E-2</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="M14" s="1">
-        <v>0.38600000000000001</v>
+        <v>-0.94499999999999995</v>
       </c>
       <c r="N14" s="1">
-        <v>7.1999999999999995E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
       <c r="O14" s="1">
-        <v>-0.21</v>
+        <v>0.26300000000000001</v>
       </c>
       <c r="P14" s="1">
-        <v>2.5999999999999999E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>5172</v>
+        <v>5990</v>
       </c>
       <c r="B15" s="1">
-        <v>4.43</v>
+        <v>4.3899999999999997</v>
       </c>
       <c r="C15" s="1">
-        <v>0.35</v>
+        <v>0.39</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>21</v>
@@ -1186,48 +1186,48 @@
         <v>25</v>
       </c>
       <c r="F15" s="1">
-        <v>0.72799999999999998</v>
+        <v>0.77800000000000002</v>
       </c>
       <c r="G15" s="1">
-        <v>0.74</v>
+        <v>0.79049999999999998</v>
       </c>
       <c r="H15" s="1">
-        <v>0.75239999999999996</v>
+        <v>0.80300000000000005</v>
       </c>
       <c r="I15" s="1">
-        <v>0.43099999999999999</v>
+        <v>7.1999999999999995E-2</v>
       </c>
       <c r="J15" s="1">
-        <v>2.7E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="K15" s="1">
-        <v>0.115</v>
+        <v>1.1890000000000001</v>
       </c>
       <c r="L15" s="1">
-        <v>6.4000000000000001E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
       <c r="M15" s="1">
-        <v>0.373</v>
+        <v>-0.91800000000000004</v>
       </c>
       <c r="N15" s="1">
-        <v>6.5000000000000002E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
       <c r="O15" s="1">
-        <v>-0.20300000000000001</v>
+        <v>0.254</v>
       </c>
       <c r="P15" s="1">
-        <v>2.4E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>5172</v>
+        <v>5990</v>
       </c>
       <c r="B16" s="1">
-        <v>4.43</v>
+        <v>4.3899999999999997</v>
       </c>
       <c r="C16" s="1">
-        <v>0.35</v>
+        <v>0.39</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>21</v>
@@ -1236,48 +1236,48 @@
         <v>25</v>
       </c>
       <c r="F16" s="1">
-        <v>0.753</v>
+        <v>0.80369999999999997</v>
       </c>
       <c r="G16" s="1">
-        <v>0.76500000000000001</v>
+        <v>0.81599999999999995</v>
       </c>
       <c r="H16" s="1">
-        <v>0.77800000000000002</v>
+        <v>0.82799999999999996</v>
       </c>
       <c r="I16" s="1">
-        <v>0.41899999999999998</v>
+        <v>9.4E-2</v>
       </c>
       <c r="J16" s="1">
-        <v>2.5999999999999999E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="K16" s="1">
-        <v>0.16200000000000001</v>
+        <v>1.119</v>
       </c>
       <c r="L16" s="1">
-        <v>6.2E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="M16" s="1">
-        <v>0.29199999999999998</v>
+        <v>-0.85699999999999998</v>
       </c>
       <c r="N16" s="1">
-        <v>6.3E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="O16" s="1">
-        <v>-0.17100000000000001</v>
+        <v>0.23300000000000001</v>
       </c>
       <c r="P16" s="1">
-        <v>2.3E-2</v>
+        <v>1.7999999999999999E-2</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>5172</v>
+        <v>5990</v>
       </c>
       <c r="B17" s="1">
-        <v>4.43</v>
+        <v>4.3899999999999997</v>
       </c>
       <c r="C17" s="1">
-        <v>0.35</v>
+        <v>0.39</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>21</v>
@@ -1286,48 +1286,48 @@
         <v>25</v>
       </c>
       <c r="F17" s="1">
-        <v>0.77800000000000002</v>
+        <v>0.82899999999999996</v>
       </c>
       <c r="G17" s="1">
-        <v>0.79049999999999998</v>
+        <v>0.84130000000000005</v>
       </c>
       <c r="H17" s="1">
-        <v>0.80300000000000005</v>
+        <v>0.85350000000000004</v>
       </c>
       <c r="I17" s="1">
-        <v>0.42399999999999999</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="J17" s="1">
-        <v>2.8000000000000001E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="K17" s="1">
-        <v>0.13800000000000001</v>
+        <v>0.99299999999999999</v>
       </c>
       <c r="L17" s="1">
-        <v>6.5000000000000002E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="M17" s="1">
-        <v>0.29899999999999999</v>
+        <v>-0.751</v>
       </c>
       <c r="N17" s="1">
-        <v>6.6000000000000003E-2</v>
+        <v>0.05</v>
       </c>
       <c r="O17" s="1">
-        <v>-0.17100000000000001</v>
+        <v>0.19800000000000001</v>
       </c>
       <c r="P17" s="1">
-        <v>2.4E-2</v>
+        <v>1.7999999999999999E-2</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>5172</v>
+        <v>5990</v>
       </c>
       <c r="B18" s="1">
-        <v>4.43</v>
+        <v>4.3899999999999997</v>
       </c>
       <c r="C18" s="1">
-        <v>0.35</v>
+        <v>0.39</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>21</v>
@@ -1336,48 +1336,48 @@
         <v>25</v>
       </c>
       <c r="F18" s="1">
-        <v>0.80369999999999997</v>
+        <v>0.85399999999999998</v>
       </c>
       <c r="G18" s="1">
-        <v>0.81599999999999995</v>
+        <v>0.86599999999999999</v>
       </c>
       <c r="H18" s="1">
-        <v>0.82799999999999996</v>
+        <v>0.879</v>
       </c>
       <c r="I18" s="1">
-        <v>0.44600000000000001</v>
+        <v>0.151</v>
       </c>
       <c r="J18" s="1">
-        <v>2.9000000000000001E-2</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="K18" s="1">
-        <v>7.0999999999999994E-2</v>
+        <v>0.95199999999999996</v>
       </c>
       <c r="L18" s="1">
-        <v>6.7000000000000004E-2</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="M18" s="1">
-        <v>0.34399999999999997</v>
+        <v>-0.72299999999999998</v>
       </c>
       <c r="N18" s="1">
-        <v>6.8000000000000005E-2</v>
+        <v>4.2999999999999997E-2</v>
       </c>
       <c r="O18" s="1">
-        <v>-0.183</v>
+        <v>0.187</v>
       </c>
       <c r="P18" s="1">
-        <v>2.5000000000000001E-2</v>
+        <v>1.6E-2</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>5172</v>
+        <v>5990</v>
       </c>
       <c r="B19" s="1">
-        <v>4.43</v>
+        <v>4.3899999999999997</v>
       </c>
       <c r="C19" s="1">
-        <v>0.35</v>
+        <v>0.39</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>21</v>
@@ -1386,48 +1386,48 @@
         <v>25</v>
       </c>
       <c r="F19" s="1">
-        <v>0.82899999999999996</v>
+        <v>0.879</v>
       </c>
       <c r="G19" s="1">
-        <v>0.84130000000000005</v>
+        <v>0.89159999999999995</v>
       </c>
       <c r="H19" s="1">
-        <v>0.85350000000000004</v>
+        <v>0.90400000000000003</v>
       </c>
       <c r="I19" s="1">
-        <v>0.46600000000000003</v>
+        <v>0.154</v>
       </c>
       <c r="J19" s="1">
-        <v>2.7E-2</v>
+        <v>1.9E-2</v>
       </c>
       <c r="K19" s="1">
-        <v>3.9E-2</v>
+        <v>0.96</v>
       </c>
       <c r="L19" s="1">
-        <v>6.3E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="M19" s="1">
-        <v>0.34499999999999997</v>
+        <v>-0.76</v>
       </c>
       <c r="N19" s="1">
-        <v>6.3E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="O19" s="1">
-        <v>-0.182</v>
+        <v>0.20599999999999999</v>
       </c>
       <c r="P19" s="1">
-        <v>2.3E-2</v>
+        <v>1.6E-2</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>5172</v>
+        <v>5990</v>
       </c>
       <c r="B20" s="1">
-        <v>4.43</v>
+        <v>4.3899999999999997</v>
       </c>
       <c r="C20" s="1">
-        <v>0.35</v>
+        <v>0.39</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>21</v>
@@ -1436,48 +1436,48 @@
         <v>25</v>
       </c>
       <c r="F20" s="1">
-        <v>0.85399999999999998</v>
+        <v>0.90429999999999999</v>
       </c>
       <c r="G20" s="1">
-        <v>0.86599999999999999</v>
+        <v>0.91700000000000004</v>
       </c>
       <c r="H20" s="1">
-        <v>0.879</v>
+        <v>0.92900000000000005</v>
       </c>
       <c r="I20" s="1">
-        <v>0.46200000000000002</v>
+        <v>0.14599999999999999</v>
       </c>
       <c r="J20" s="1">
-        <v>2.5999999999999999E-2</v>
+        <v>1.9E-2</v>
       </c>
       <c r="K20" s="1">
-        <v>6.5000000000000002E-2</v>
+        <v>0.96499999999999997</v>
       </c>
       <c r="L20" s="1">
-        <v>6.0999999999999999E-2</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="M20" s="1">
-        <v>0.28499999999999998</v>
+        <v>-0.77</v>
       </c>
       <c r="N20" s="1">
-        <v>6.0999999999999999E-2</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="O20" s="1">
-        <v>-0.157</v>
+        <v>0.21299999999999999</v>
       </c>
       <c r="P20" s="1">
-        <v>2.1999999999999999E-2</v>
+        <v>1.7000000000000001E-2</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>5172</v>
+        <v>5990</v>
       </c>
       <c r="B21" s="1">
-        <v>4.43</v>
+        <v>4.3899999999999997</v>
       </c>
       <c r="C21" s="1">
-        <v>0.35</v>
+        <v>0.39</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>21</v>
@@ -1486,48 +1486,48 @@
         <v>25</v>
       </c>
       <c r="F21" s="1">
-        <v>0.879</v>
+        <v>0.93</v>
       </c>
       <c r="G21" s="1">
-        <v>0.89159999999999995</v>
+        <v>0.94240000000000002</v>
       </c>
       <c r="H21" s="1">
-        <v>0.90400000000000003</v>
+        <v>0.9546</v>
       </c>
       <c r="I21" s="1">
-        <v>0.438</v>
+        <v>0.13400000000000001</v>
       </c>
       <c r="J21" s="1">
-        <v>2.8000000000000001E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="K21" s="1">
-        <v>0.13</v>
+        <v>0.98599999999999999</v>
       </c>
       <c r="L21" s="1">
-        <v>6.7000000000000004E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="M21" s="1">
-        <v>0.21099999999999999</v>
+        <v>-0.80600000000000005</v>
       </c>
       <c r="N21" s="1">
-        <v>6.7000000000000004E-2</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="O21" s="1">
-        <v>-0.13400000000000001</v>
+        <v>0.23200000000000001</v>
       </c>
       <c r="P21" s="1">
-        <v>2.5000000000000001E-2</v>
+        <v>1.9E-2</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>5172</v>
+        <v>5990</v>
       </c>
       <c r="B22" s="1">
-        <v>4.43</v>
+        <v>4.3899999999999997</v>
       </c>
       <c r="C22" s="1">
-        <v>0.35</v>
+        <v>0.39</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>21</v>
@@ -1536,48 +1536,48 @@
         <v>25</v>
       </c>
       <c r="F22" s="1">
-        <v>0.90429999999999999</v>
+        <v>0.95499999999999996</v>
       </c>
       <c r="G22" s="1">
-        <v>0.91700000000000004</v>
+        <v>0.96730000000000005</v>
       </c>
       <c r="H22" s="1">
-        <v>0.92900000000000005</v>
+        <v>0.98</v>
       </c>
       <c r="I22" s="1">
-        <v>0.40699999999999997</v>
+        <v>0.13400000000000001</v>
       </c>
       <c r="J22" s="1">
-        <v>0.03</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="K22" s="1">
-        <v>0.221</v>
+        <v>0.998</v>
       </c>
       <c r="L22" s="1">
-        <v>7.0999999999999994E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="M22" s="1">
-        <v>9.5000000000000001E-2</v>
+        <v>-0.84199999999999997</v>
       </c>
       <c r="N22" s="1">
-        <v>7.1999999999999995E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="O22" s="1">
-        <v>-8.7999999999999995E-2</v>
+        <v>0.248</v>
       </c>
       <c r="P22" s="1">
-        <v>2.5999999999999999E-2</v>
+        <v>1.7999999999999999E-2</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>5172</v>
+        <v>5990</v>
       </c>
       <c r="B23" s="1">
-        <v>4.43</v>
+        <v>4.3899999999999997</v>
       </c>
       <c r="C23" s="1">
-        <v>0.35</v>
+        <v>0.39</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>21</v>
@@ -1586,48 +1586,48 @@
         <v>25</v>
       </c>
       <c r="F23" s="1">
-        <v>0.93</v>
+        <v>0.98</v>
       </c>
       <c r="G23" s="1">
-        <v>0.94240000000000002</v>
+        <v>0.99270000000000003</v>
       </c>
       <c r="H23" s="1">
-        <v>0.9546</v>
+        <v>1.0049999999999999</v>
       </c>
       <c r="I23" s="1">
-        <v>0.39300000000000002</v>
+        <v>0.105</v>
       </c>
       <c r="J23" s="1">
-        <v>3.4000000000000002E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="K23" s="1">
-        <v>0.252</v>
+        <v>1.0609999999999999</v>
       </c>
       <c r="L23" s="1">
-        <v>8.1000000000000003E-2</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="M23" s="1">
-        <v>4.9000000000000002E-2</v>
+        <v>-0.90300000000000002</v>
       </c>
       <c r="N23" s="1">
-        <v>8.2000000000000003E-2</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="O23" s="1">
-        <v>-6.8000000000000005E-2</v>
+        <v>0.27100000000000002</v>
       </c>
       <c r="P23" s="1">
-        <v>0.03</v>
+        <v>1.9E-2</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>5172</v>
+        <v>5990</v>
       </c>
       <c r="B24" s="1">
-        <v>4.43</v>
+        <v>4.3899999999999997</v>
       </c>
       <c r="C24" s="1">
-        <v>0.35</v>
+        <v>0.39</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>21</v>
@@ -1636,888 +1636,824 @@
         <v>25</v>
       </c>
       <c r="F24" s="1">
-        <v>0.95499999999999996</v>
+        <v>1.006</v>
       </c>
       <c r="G24" s="1">
-        <v>0.96730000000000005</v>
+        <v>1.018</v>
       </c>
       <c r="H24" s="1">
-        <v>0.98</v>
+        <v>1.03</v>
       </c>
       <c r="I24" s="1">
-        <v>0.39500000000000002</v>
+        <v>0.13200000000000001</v>
       </c>
       <c r="J24" s="1">
-        <v>3.5999999999999997E-2</v>
+        <v>1.9E-2</v>
       </c>
       <c r="K24" s="1">
-        <v>0.252</v>
+        <v>1.0049999999999999</v>
       </c>
       <c r="L24" s="1">
-        <v>8.4000000000000005E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="M24" s="1">
-        <v>4.3999999999999997E-2</v>
+        <v>-0.86299999999999999</v>
       </c>
       <c r="N24" s="1">
-        <v>8.5000000000000006E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="O24" s="1">
-        <v>-7.0999999999999994E-2</v>
+        <v>0.255</v>
       </c>
       <c r="P24" s="1">
-        <v>3.1E-2</v>
+        <v>1.6E-2</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>5172</v>
+        <v>5990</v>
       </c>
       <c r="B25" s="1">
-        <v>4.43</v>
+        <v>4.3899999999999997</v>
       </c>
       <c r="C25" s="1">
-        <v>0.35</v>
+        <v>0.39</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F25" s="1">
-        <v>0.98</v>
+        <v>1.0409999999999999</v>
       </c>
       <c r="G25" s="1">
-        <v>0.99270000000000003</v>
+        <v>1.06</v>
       </c>
       <c r="H25" s="1">
-        <v>1.0049999999999999</v>
+        <v>1.0780000000000001</v>
       </c>
       <c r="I25" s="1">
-        <v>0.35199999999999998</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="J25" s="1">
-        <v>4.2000000000000003E-2</v>
+        <v>1.4E-2</v>
       </c>
       <c r="K25" s="1">
-        <v>0.35299999999999998</v>
+        <v>0.97899999999999998</v>
       </c>
       <c r="L25" s="1">
-        <v>0.1</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="M25" s="1">
-        <v>-6.8000000000000005E-2</v>
+        <v>-0.86</v>
       </c>
       <c r="N25" s="1">
-        <v>0.10100000000000001</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="O25" s="1">
-        <v>-2.5999999999999999E-2</v>
+        <v>0.26200000000000001</v>
       </c>
       <c r="P25" s="1">
-        <v>3.6999999999999998E-2</v>
+        <v>1.2E-2</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>5172</v>
+        <v>5990</v>
       </c>
       <c r="B26" s="1">
-        <v>4.43</v>
+        <v>4.3899999999999997</v>
       </c>
       <c r="C26" s="1">
-        <v>0.35</v>
+        <v>0.39</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F26" s="1">
-        <v>1.006</v>
+        <v>1.0780000000000001</v>
       </c>
       <c r="G26" s="1">
-        <v>1.018</v>
+        <v>1.0980000000000001</v>
       </c>
       <c r="H26" s="1">
-        <v>1.03</v>
+        <v>1.117</v>
       </c>
       <c r="I26" s="1">
-        <v>0.35899999999999999</v>
+        <v>0.17100000000000001</v>
       </c>
       <c r="J26" s="1">
-        <v>3.6999999999999998E-2</v>
+        <v>1.2E-2</v>
       </c>
       <c r="K26" s="1">
-        <v>0.33900000000000002</v>
+        <v>0.92300000000000004</v>
       </c>
       <c r="L26" s="1">
-        <v>8.7999999999999995E-2</v>
+        <v>2.9000000000000001E-2</v>
       </c>
       <c r="M26" s="1">
-        <v>-6.3E-2</v>
+        <v>-0.82799999999999996</v>
       </c>
       <c r="N26" s="1">
-        <v>8.8999999999999996E-2</v>
+        <v>2.9000000000000001E-2</v>
       </c>
       <c r="O26" s="1">
-        <v>-0.03</v>
+        <v>0.249</v>
       </c>
       <c r="P26" s="1">
-        <v>3.2000000000000001E-2</v>
+        <v>1.0999999999999999E-2</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>5172</v>
+        <v>5990</v>
       </c>
       <c r="B27" s="1">
-        <v>4.43</v>
+        <v>4.3899999999999997</v>
       </c>
       <c r="C27" s="1">
-        <v>0.35</v>
+        <v>0.39</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F27" s="1">
-        <v>1.0409999999999999</v>
+        <v>1.117</v>
       </c>
       <c r="G27" s="1">
-        <v>1.06</v>
+        <v>1.1379999999999999</v>
       </c>
       <c r="H27" s="1">
-        <v>1.0780000000000001</v>
+        <v>1.1579999999999999</v>
       </c>
       <c r="I27" s="1">
-        <v>0.37</v>
+        <v>0.156</v>
       </c>
       <c r="J27" s="1">
-        <v>3.3000000000000002E-2</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="K27" s="1">
-        <v>0.31</v>
+        <v>0.96599999999999997</v>
       </c>
       <c r="L27" s="1">
-        <v>7.8E-2</v>
+        <v>0.03</v>
       </c>
       <c r="M27" s="1">
-        <v>-5.7000000000000002E-2</v>
+        <v>-0.89400000000000002</v>
       </c>
       <c r="N27" s="1">
-        <v>7.8E-2</v>
+        <v>0.03</v>
       </c>
       <c r="O27" s="1">
-        <v>-3.1E-2</v>
+        <v>0.28199999999999997</v>
       </c>
       <c r="P27" s="1">
-        <v>2.9000000000000001E-2</v>
+        <v>1.0999999999999999E-2</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>5172</v>
+        <v>5990</v>
       </c>
       <c r="B28" s="1">
-        <v>4.43</v>
+        <v>4.3899999999999997</v>
       </c>
       <c r="C28" s="1">
-        <v>0.35</v>
+        <v>0.39</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F28" s="1">
-        <v>1.0780000000000001</v>
+        <v>1.1579999999999999</v>
       </c>
       <c r="G28" s="1">
-        <v>1.0980000000000001</v>
+        <v>1.179</v>
       </c>
       <c r="H28" s="1">
-        <v>1.117</v>
+        <v>1.2</v>
       </c>
       <c r="I28" s="1">
-        <v>0.36399999999999999</v>
+        <v>0.17699999999999999</v>
       </c>
       <c r="J28" s="1">
-        <v>2.9000000000000001E-2</v>
+        <v>1.4E-2</v>
       </c>
       <c r="K28" s="1">
-        <v>0.32900000000000001</v>
+        <v>0.94899999999999995</v>
       </c>
       <c r="L28" s="1">
-        <v>6.9000000000000006E-2</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="M28" s="1">
-        <v>-0.08</v>
+        <v>-0.91</v>
       </c>
       <c r="N28" s="1">
-        <v>6.9000000000000006E-2</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="O28" s="1">
-        <v>-2.8000000000000001E-2</v>
+        <v>0.29299999999999998</v>
       </c>
       <c r="P28" s="1">
-        <v>2.5000000000000001E-2</v>
+        <v>1.2E-2</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>5172</v>
+        <v>5990</v>
       </c>
       <c r="B29" s="1">
-        <v>4.43</v>
+        <v>4.3899999999999997</v>
       </c>
       <c r="C29" s="1">
-        <v>0.35</v>
+        <v>0.39</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F29" s="1">
-        <v>1.117</v>
+        <v>1.2</v>
       </c>
       <c r="G29" s="1">
-        <v>1.1379999999999999</v>
+        <v>1.222</v>
       </c>
       <c r="H29" s="1">
-        <v>1.1579999999999999</v>
+        <v>1.2430000000000001</v>
       </c>
       <c r="I29" s="1">
-        <v>0.316</v>
+        <v>0.16700000000000001</v>
       </c>
       <c r="J29" s="1">
-        <v>3.5000000000000003E-2</v>
+        <v>1.9E-2</v>
       </c>
       <c r="K29" s="1">
-        <v>0.45700000000000002</v>
+        <v>1.0189999999999999</v>
       </c>
       <c r="L29" s="1">
-        <v>8.3000000000000004E-2</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="M29" s="1">
-        <v>-0.223</v>
+        <v>-1.02</v>
       </c>
       <c r="N29" s="1">
-        <v>8.3000000000000004E-2</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="O29" s="1">
-        <v>2.5999999999999999E-2</v>
+        <v>0.34100000000000003</v>
       </c>
       <c r="P29" s="1">
-        <v>0.03</v>
+        <v>1.7000000000000001E-2</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>5172</v>
+        <v>5990</v>
       </c>
       <c r="B30" s="1">
-        <v>4.43</v>
+        <v>4.3899999999999997</v>
       </c>
       <c r="C30" s="1">
-        <v>0.35</v>
+        <v>0.39</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F30" s="1">
-        <v>1.1579999999999999</v>
+        <v>1.2430000000000001</v>
       </c>
       <c r="G30" s="1">
-        <v>1.179</v>
+        <v>1.266</v>
       </c>
       <c r="H30" s="1">
-        <v>1.2</v>
+        <v>1.288</v>
       </c>
       <c r="I30" s="1">
-        <v>0.28499999999999998</v>
+        <v>0.249</v>
       </c>
       <c r="J30" s="1">
-        <v>3.6999999999999998E-2</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="K30" s="1">
-        <v>0.55100000000000005</v>
+        <v>0.878</v>
       </c>
       <c r="L30" s="1">
-        <v>8.6999999999999994E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="M30" s="1">
-        <v>-0.33500000000000002</v>
+        <v>-0.92200000000000004</v>
       </c>
       <c r="N30" s="1">
-        <v>8.7999999999999995E-2</v>
+        <v>2.3E-2</v>
       </c>
       <c r="O30" s="1">
-        <v>6.6000000000000003E-2</v>
+        <v>0.308</v>
       </c>
       <c r="P30" s="1">
-        <v>3.2000000000000001E-2</v>
+        <v>8.0000000000000002E-3</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>5172</v>
+        <v>5990</v>
       </c>
       <c r="B31" s="1">
-        <v>4.43</v>
+        <v>4.3899999999999997</v>
       </c>
       <c r="C31" s="1">
-        <v>0.35</v>
+        <v>0.39</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F31" s="1">
-        <v>1.2</v>
+        <v>1.288</v>
       </c>
       <c r="G31" s="1">
-        <v>1.222</v>
+        <v>1.3120000000000001</v>
       </c>
       <c r="H31" s="1">
-        <v>1.2430000000000001</v>
+        <v>1.335</v>
       </c>
       <c r="I31" s="1">
-        <v>0.25800000000000001</v>
+        <v>0.307</v>
       </c>
       <c r="J31" s="1">
-        <v>3.5000000000000003E-2</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="K31" s="1">
-        <v>0.64500000000000002</v>
+        <v>0.755</v>
       </c>
       <c r="L31" s="1">
-        <v>8.3000000000000004E-2</v>
+        <v>4.2999999999999997E-2</v>
       </c>
       <c r="M31" s="1">
-        <v>-0.44500000000000001</v>
+        <v>-0.82199999999999995</v>
       </c>
       <c r="N31" s="1">
-        <v>8.3000000000000004E-2</v>
+        <v>4.2999999999999997E-2</v>
       </c>
       <c r="O31" s="1">
-        <v>0.104</v>
+        <v>0.27900000000000003</v>
       </c>
       <c r="P31" s="1">
-        <v>0.03</v>
+        <v>1.6E-2</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>5172</v>
+        <v>5990</v>
       </c>
       <c r="B32" s="1">
-        <v>4.43</v>
+        <v>4.3899999999999997</v>
       </c>
       <c r="C32" s="1">
-        <v>0.35</v>
+        <v>0.39</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F32" s="1">
-        <v>1.2430000000000001</v>
+        <v>1.335</v>
       </c>
       <c r="G32" s="1">
-        <v>1.266</v>
+        <v>1.3580000000000001</v>
       </c>
       <c r="H32" s="1">
-        <v>1.288</v>
+        <v>1.383</v>
       </c>
       <c r="I32" s="1">
-        <v>0.254</v>
+        <v>0.35299999999999998</v>
       </c>
       <c r="J32" s="1">
-        <v>2.8000000000000001E-2</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="K32" s="1">
-        <v>0.69899999999999995</v>
+        <v>0.71399999999999997</v>
       </c>
       <c r="L32" s="1">
-        <v>6.7000000000000004E-2</v>
+        <v>4.3999999999999997E-2</v>
       </c>
       <c r="M32" s="1">
-        <v>-0.51900000000000002</v>
+        <v>-0.85</v>
       </c>
       <c r="N32" s="1">
-        <v>6.8000000000000005E-2</v>
+        <v>4.3999999999999997E-2</v>
       </c>
       <c r="O32" s="1">
-        <v>0.127</v>
+        <v>0.30499999999999999</v>
       </c>
       <c r="P32" s="1">
-        <v>2.5000000000000001E-2</v>
+        <v>1.6E-2</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>5172</v>
+        <v>5990</v>
       </c>
       <c r="B33" s="1">
-        <v>4.43</v>
+        <v>4.3899999999999997</v>
       </c>
       <c r="C33" s="1">
-        <v>0.35</v>
+        <v>0.39</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F33" s="1">
-        <v>1.288</v>
+        <v>1.383</v>
       </c>
       <c r="G33" s="1">
-        <v>1.3120000000000001</v>
+        <v>1.4079999999999999</v>
       </c>
       <c r="H33" s="1">
-        <v>1.335</v>
+        <v>1.4339999999999999</v>
       </c>
       <c r="I33" s="1">
-        <v>0.252</v>
+        <v>0.47099999999999997</v>
       </c>
       <c r="J33" s="1">
-        <v>2.5999999999999999E-2</v>
+        <v>1.9E-2</v>
       </c>
       <c r="K33" s="1">
-        <v>0.73799999999999999</v>
+        <v>0.48099999999999998</v>
       </c>
       <c r="L33" s="1">
-        <v>6.2E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="M33" s="1">
-        <v>-0.58799999999999997</v>
+        <v>-0.67100000000000004</v>
       </c>
       <c r="N33" s="1">
-        <v>6.3E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="O33" s="1">
-        <v>0.157</v>
+        <v>0.253</v>
       </c>
       <c r="P33" s="1">
-        <v>2.3E-2</v>
+        <v>1.6E-2</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>5172</v>
+        <v>5990</v>
       </c>
       <c r="B34" s="1">
-        <v>4.43</v>
+        <v>4.3899999999999997</v>
       </c>
       <c r="C34" s="1">
-        <v>0.35</v>
+        <v>0.39</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F34" s="1">
-        <v>1.335</v>
+        <v>1.4339999999999999</v>
       </c>
       <c r="G34" s="1">
-        <v>1.3580000000000001</v>
+        <v>1.4590000000000001</v>
       </c>
       <c r="H34" s="1">
-        <v>1.383</v>
+        <v>1.4850000000000001</v>
       </c>
       <c r="I34" s="1">
-        <v>0.248</v>
+        <v>0.61399999999999999</v>
       </c>
       <c r="J34" s="1">
-        <v>2.9000000000000001E-2</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="K34" s="1">
-        <v>0.84199999999999997</v>
+        <v>0.17899999999999999</v>
       </c>
       <c r="L34" s="1">
-        <v>7.0000000000000007E-2</v>
+        <v>4.3999999999999997E-2</v>
       </c>
       <c r="M34" s="1">
-        <v>-0.751</v>
+        <v>-0.41399999999999998</v>
       </c>
       <c r="N34" s="1">
-        <v>7.0000000000000007E-2</v>
+        <v>4.3999999999999997E-2</v>
       </c>
       <c r="O34" s="1">
-        <v>0.223</v>
+        <v>0.16800000000000001</v>
       </c>
       <c r="P34" s="1">
-        <v>2.5999999999999999E-2</v>
+        <v>1.6E-2</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>5172</v>
+        <v>5990</v>
       </c>
       <c r="B35" s="1">
-        <v>4.43</v>
+        <v>4.3899999999999997</v>
       </c>
       <c r="C35" s="1">
-        <v>0.35</v>
+        <v>0.39</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F35" s="1">
-        <v>1.383</v>
+        <v>1.4850000000000001</v>
       </c>
       <c r="G35" s="1">
-        <v>1.4079999999999999</v>
+        <v>1.512</v>
       </c>
       <c r="H35" s="1">
-        <v>1.4339999999999999</v>
+        <v>1.5389999999999999</v>
       </c>
       <c r="I35" s="1">
-        <v>0.30499999999999999</v>
+        <v>0.75</v>
       </c>
       <c r="J35" s="1">
-        <v>1.2999999999999999E-2</v>
+        <v>0.03</v>
       </c>
       <c r="K35" s="1">
-        <v>0.78100000000000003</v>
+        <v>-0.13200000000000001</v>
       </c>
       <c r="L35" s="1">
-        <v>3.2000000000000001E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="M35" s="1">
-        <v>-0.751</v>
+        <v>-0.14699999999999999</v>
       </c>
       <c r="N35" s="1">
-        <v>3.2000000000000001E-2</v>
+        <v>7.0999999999999994E-2</v>
       </c>
       <c r="O35" s="1">
-        <v>0.23</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="P35" s="1">
-        <v>1.2E-2</v>
+        <v>2.5999999999999999E-2</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>5172</v>
+        <v>5990</v>
       </c>
       <c r="B36" s="1">
-        <v>4.43</v>
+        <v>4.3899999999999997</v>
       </c>
       <c r="C36" s="1">
-        <v>0.35</v>
+        <v>0.39</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F36" s="1">
-        <v>1.4339999999999999</v>
+        <v>1.5389999999999999</v>
       </c>
       <c r="G36" s="1">
-        <v>1.4590000000000001</v>
+        <v>1.5660000000000001</v>
       </c>
       <c r="H36" s="1">
-        <v>1.4850000000000001</v>
+        <v>1.595</v>
       </c>
       <c r="I36" s="1">
-        <v>0.40300000000000002</v>
+        <v>0.85899999999999999</v>
       </c>
       <c r="J36" s="1">
-        <v>5.0000000000000001E-3</v>
+        <v>0.02</v>
       </c>
       <c r="K36" s="1">
-        <v>0.64200000000000002</v>
+        <v>-0.373</v>
       </c>
       <c r="L36" s="1">
-        <v>1.0999999999999999E-2</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="M36" s="1">
-        <v>-0.68600000000000005</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="N36" s="1">
-        <v>1.0999999999999999E-2</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="O36" s="1">
-        <v>0.219</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="P36" s="1">
-        <v>4.0000000000000001E-3</v>
+        <v>1.7999999999999999E-2</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>5172</v>
+        <v>5990</v>
       </c>
       <c r="B37" s="1">
-        <v>4.43</v>
+        <v>4.3899999999999997</v>
       </c>
       <c r="C37" s="1">
-        <v>0.35</v>
+        <v>0.39</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F37" s="1">
-        <v>1.4850000000000001</v>
+        <v>1.595</v>
       </c>
       <c r="G37" s="1">
-        <v>1.512</v>
+        <v>1.623</v>
       </c>
       <c r="H37" s="1">
-        <v>1.5389999999999999</v>
+        <v>1.6519999999999999</v>
       </c>
       <c r="I37" s="1">
-        <v>0.54500000000000004</v>
+        <v>0.91800000000000004</v>
       </c>
       <c r="J37" s="1">
-        <v>1.4E-2</v>
+        <v>0.02</v>
       </c>
       <c r="K37" s="1">
-        <v>0.39200000000000002</v>
+        <v>-0.51900000000000002</v>
       </c>
       <c r="L37" s="1">
-        <v>3.4000000000000002E-2</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="M37" s="1">
-        <v>-0.52700000000000002</v>
+        <v>0.159</v>
       </c>
       <c r="N37" s="1">
-        <v>3.4000000000000002E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="O37" s="1">
-        <v>0.18</v>
+        <v>-8.0000000000000002E-3</v>
       </c>
       <c r="P37" s="1">
-        <v>1.2E-2</v>
+        <v>1.7999999999999999E-2</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>5172</v>
+        <v>5990</v>
       </c>
       <c r="B38" s="1">
-        <v>4.43</v>
+        <v>4.3899999999999997</v>
       </c>
       <c r="C38" s="1">
-        <v>0.35</v>
+        <v>0.39</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F38" s="1">
-        <v>1.5389999999999999</v>
+        <v>1.6519999999999999</v>
       </c>
       <c r="G38" s="1">
-        <v>1.5660000000000001</v>
+        <v>1.6819999999999999</v>
       </c>
       <c r="H38" s="1">
-        <v>1.595</v>
+        <v>1.712</v>
       </c>
       <c r="I38" s="1">
-        <v>0.69099999999999995</v>
+        <v>0.91400000000000003</v>
       </c>
       <c r="J38" s="1">
-        <v>1.2E-2</v>
+        <v>0.02</v>
       </c>
       <c r="K38" s="1">
-        <v>0.128</v>
+        <v>-0.52</v>
       </c>
       <c r="L38" s="1">
-        <v>2.9000000000000001E-2</v>
+        <v>4.7E-2</v>
       </c>
       <c r="M38" s="1">
-        <v>-0.35599999999999998</v>
+        <v>0.16800000000000001</v>
       </c>
       <c r="N38" s="1">
-        <v>2.9000000000000001E-2</v>
+        <v>4.7E-2</v>
       </c>
       <c r="O38" s="1">
-        <v>0.13800000000000001</v>
+        <v>-1.2999999999999999E-2</v>
       </c>
       <c r="P38" s="1">
-        <v>0.01</v>
+        <v>1.7000000000000001E-2</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>5172</v>
+        <v>5990</v>
       </c>
       <c r="B39" s="1">
-        <v>4.43</v>
+        <v>4.3899999999999997</v>
       </c>
       <c r="C39" s="1">
-        <v>0.35</v>
+        <v>0.39</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F39" s="1">
-        <v>1.595</v>
+        <v>1.712</v>
       </c>
       <c r="G39" s="1">
-        <v>1.623</v>
+        <v>1.7430000000000001</v>
       </c>
       <c r="H39" s="1">
-        <v>1.6519999999999999</v>
+        <v>1.7729999999999999</v>
       </c>
       <c r="I39" s="1">
-        <v>0.79500000000000004</v>
+        <v>0.85</v>
       </c>
       <c r="J39" s="1">
-        <v>0.01</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="K39" s="1">
-        <v>-8.7999999999999995E-2</v>
+        <v>-0.434</v>
       </c>
       <c r="L39" s="1">
-        <v>2.5000000000000001E-2</v>
+        <v>4.1000000000000002E-2</v>
       </c>
       <c r="M39" s="1">
-        <v>-0.20499999999999999</v>
+        <v>8.7999999999999995E-2</v>
       </c>
       <c r="N39" s="1">
-        <v>2.5000000000000001E-2</v>
+        <v>4.1000000000000002E-2</v>
       </c>
       <c r="O39" s="1">
-        <v>9.9000000000000005E-2</v>
+        <v>1.4E-2</v>
       </c>
       <c r="P39" s="1">
-        <v>8.9999999999999993E-3</v>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
-        <v>5172</v>
-      </c>
-      <c r="B40" s="1">
-        <v>4.43</v>
-      </c>
-      <c r="C40" s="1">
-        <v>0.35</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F40" s="1">
-        <v>1.6519999999999999</v>
-      </c>
-      <c r="G40" s="1">
-        <v>1.6819999999999999</v>
-      </c>
-      <c r="H40" s="1">
-        <v>1.712</v>
-      </c>
-      <c r="I40" s="1">
-        <v>0.81599999999999995</v>
-      </c>
-      <c r="J40" s="1">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="K40" s="1">
-        <v>-0.14099999999999999</v>
-      </c>
-      <c r="L40" s="1">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="M40" s="1">
-        <v>-0.161</v>
-      </c>
-      <c r="N40" s="1">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="O40" s="1">
-        <v>8.5999999999999993E-2</v>
-      </c>
-      <c r="P40" s="1">
-        <v>8.9999999999999993E-3</v>
-      </c>
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+      <c r="K40" s="1"/>
+      <c r="L40" s="1"/>
+      <c r="M40" s="1"/>
+      <c r="N40" s="1"/>
+      <c r="O40" s="1"/>
+      <c r="P40" s="1"/>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
-        <v>5172</v>
-      </c>
-      <c r="B41" s="1">
-        <v>4.43</v>
-      </c>
-      <c r="C41" s="1">
-        <v>0.35</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F41" s="1">
-        <v>1.712</v>
-      </c>
-      <c r="G41" s="1">
-        <v>1.7430000000000001</v>
-      </c>
-      <c r="H41" s="1">
-        <v>1.7729999999999999</v>
-      </c>
-      <c r="I41" s="1">
-        <v>0.78</v>
-      </c>
-      <c r="J41" s="1">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="K41" s="1">
-        <v>-0.108</v>
-      </c>
-      <c r="L41" s="1">
-        <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="M41" s="1">
-        <v>-0.193</v>
-      </c>
-      <c r="N41" s="1">
-        <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="O41" s="1">
-        <v>9.8000000000000004E-2</v>
-      </c>
-      <c r="P41" s="1">
-        <v>0.01</v>
-      </c>
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+      <c r="L41" s="1"/>
+      <c r="M41" s="1"/>
+      <c r="N41" s="1"/>
+      <c r="O41" s="1"/>
+      <c r="P41" s="1"/>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
@@ -2537,438 +2473,6 @@
       <c r="O42" s="1"/>
       <c r="P42" s="1"/>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
-      <c r="I43" s="1"/>
-      <c r="J43" s="1"/>
-      <c r="K43" s="1"/>
-      <c r="L43" s="1"/>
-      <c r="M43" s="1"/>
-      <c r="N43" s="1"/>
-      <c r="O43" s="1"/>
-      <c r="P43" s="1"/>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
-      <c r="I44" s="1"/>
-      <c r="J44" s="1"/>
-      <c r="K44" s="1"/>
-      <c r="L44" s="1"/>
-      <c r="M44" s="1"/>
-      <c r="N44" s="1"/>
-      <c r="O44" s="1"/>
-      <c r="P44" s="1"/>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
-      <c r="H45" s="1"/>
-      <c r="I45" s="1"/>
-      <c r="J45" s="1"/>
-      <c r="K45" s="1"/>
-      <c r="L45" s="1"/>
-      <c r="M45" s="1"/>
-      <c r="N45" s="1"/>
-      <c r="O45" s="1"/>
-      <c r="P45" s="1"/>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
-      <c r="H46" s="1"/>
-      <c r="I46" s="1"/>
-      <c r="J46" s="1"/>
-      <c r="K46" s="1"/>
-      <c r="L46" s="1"/>
-      <c r="M46" s="1"/>
-      <c r="N46" s="1"/>
-      <c r="O46" s="1"/>
-      <c r="P46" s="1"/>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A47" s="1"/>
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
-      <c r="H47" s="1"/>
-      <c r="I47" s="1"/>
-      <c r="J47" s="1"/>
-      <c r="K47" s="1"/>
-      <c r="L47" s="1"/>
-      <c r="M47" s="1"/>
-      <c r="N47" s="1"/>
-      <c r="O47" s="1"/>
-      <c r="P47" s="1"/>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A48" s="1"/>
-      <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
-      <c r="H48" s="1"/>
-      <c r="I48" s="1"/>
-      <c r="J48" s="1"/>
-      <c r="K48" s="1"/>
-      <c r="L48" s="1"/>
-      <c r="M48" s="1"/>
-      <c r="N48" s="1"/>
-      <c r="O48" s="1"/>
-      <c r="P48" s="1"/>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
-      <c r="H49" s="1"/>
-      <c r="I49" s="1"/>
-      <c r="J49" s="1"/>
-      <c r="K49" s="1"/>
-      <c r="L49" s="1"/>
-      <c r="M49" s="1"/>
-      <c r="N49" s="1"/>
-      <c r="O49" s="1"/>
-      <c r="P49" s="1"/>
-    </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A50" s="1"/>
-      <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
-      <c r="G50" s="1"/>
-      <c r="H50" s="1"/>
-      <c r="I50" s="1"/>
-      <c r="J50" s="1"/>
-      <c r="K50" s="1"/>
-      <c r="L50" s="1"/>
-      <c r="M50" s="1"/>
-      <c r="N50" s="1"/>
-      <c r="O50" s="1"/>
-      <c r="P50" s="1"/>
-    </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A51" s="1"/>
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
-      <c r="F51" s="1"/>
-      <c r="G51" s="1"/>
-      <c r="H51" s="1"/>
-      <c r="I51" s="1"/>
-      <c r="J51" s="1"/>
-      <c r="K51" s="1"/>
-      <c r="L51" s="1"/>
-      <c r="M51" s="1"/>
-      <c r="N51" s="1"/>
-      <c r="O51" s="1"/>
-      <c r="P51" s="1"/>
-    </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A52" s="1"/>
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
-      <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
-      <c r="H52" s="1"/>
-      <c r="I52" s="1"/>
-      <c r="J52" s="1"/>
-      <c r="K52" s="1"/>
-      <c r="L52" s="1"/>
-      <c r="M52" s="1"/>
-      <c r="N52" s="1"/>
-      <c r="O52" s="1"/>
-      <c r="P52" s="1"/>
-    </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A53" s="1"/>
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
-      <c r="H53" s="1"/>
-      <c r="I53" s="1"/>
-      <c r="J53" s="1"/>
-      <c r="K53" s="1"/>
-      <c r="L53" s="1"/>
-      <c r="M53" s="1"/>
-      <c r="N53" s="1"/>
-      <c r="O53" s="1"/>
-      <c r="P53" s="1"/>
-    </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A54" s="1"/>
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
-      <c r="H54" s="1"/>
-      <c r="I54" s="1"/>
-      <c r="J54" s="1"/>
-      <c r="K54" s="1"/>
-      <c r="L54" s="1"/>
-      <c r="M54" s="1"/>
-      <c r="N54" s="1"/>
-      <c r="O54" s="1"/>
-      <c r="P54" s="1"/>
-    </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A55" s="1"/>
-      <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
-      <c r="E55" s="1"/>
-      <c r="F55" s="1"/>
-      <c r="G55" s="1"/>
-      <c r="H55" s="1"/>
-      <c r="I55" s="1"/>
-      <c r="J55" s="1"/>
-      <c r="K55" s="1"/>
-      <c r="L55" s="1"/>
-      <c r="M55" s="1"/>
-      <c r="N55" s="1"/>
-      <c r="O55" s="1"/>
-      <c r="P55" s="1"/>
-    </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A56" s="1"/>
-      <c r="B56" s="1"/>
-      <c r="C56" s="1"/>
-      <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
-      <c r="F56" s="1"/>
-      <c r="G56" s="1"/>
-      <c r="H56" s="1"/>
-      <c r="I56" s="1"/>
-      <c r="J56" s="1"/>
-      <c r="K56" s="1"/>
-      <c r="L56" s="1"/>
-      <c r="M56" s="1"/>
-      <c r="N56" s="1"/>
-      <c r="O56" s="1"/>
-      <c r="P56" s="1"/>
-    </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A57" s="1"/>
-      <c r="B57" s="1"/>
-      <c r="C57" s="1"/>
-      <c r="D57" s="1"/>
-      <c r="E57" s="1"/>
-      <c r="F57" s="1"/>
-      <c r="G57" s="1"/>
-      <c r="H57" s="1"/>
-      <c r="I57" s="1"/>
-      <c r="J57" s="1"/>
-      <c r="K57" s="1"/>
-      <c r="L57" s="1"/>
-      <c r="M57" s="1"/>
-      <c r="N57" s="1"/>
-      <c r="O57" s="1"/>
-      <c r="P57" s="1"/>
-    </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A58" s="1"/>
-      <c r="B58" s="1"/>
-      <c r="C58" s="1"/>
-      <c r="D58" s="1"/>
-      <c r="E58" s="1"/>
-      <c r="F58" s="1"/>
-      <c r="G58" s="1"/>
-      <c r="H58" s="1"/>
-      <c r="I58" s="1"/>
-      <c r="J58" s="1"/>
-      <c r="K58" s="1"/>
-      <c r="L58" s="1"/>
-      <c r="M58" s="1"/>
-      <c r="N58" s="1"/>
-      <c r="O58" s="1"/>
-      <c r="P58" s="1"/>
-    </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A59" s="1"/>
-      <c r="B59" s="1"/>
-      <c r="C59" s="1"/>
-      <c r="D59" s="1"/>
-      <c r="E59" s="1"/>
-      <c r="F59" s="1"/>
-      <c r="G59" s="1"/>
-      <c r="H59" s="1"/>
-      <c r="I59" s="1"/>
-      <c r="J59" s="1"/>
-      <c r="K59" s="1"/>
-      <c r="L59" s="1"/>
-      <c r="M59" s="1"/>
-      <c r="N59" s="1"/>
-      <c r="O59" s="1"/>
-      <c r="P59" s="1"/>
-    </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A60" s="1"/>
-      <c r="B60" s="1"/>
-      <c r="C60" s="1"/>
-      <c r="D60" s="1"/>
-      <c r="E60" s="1"/>
-      <c r="F60" s="1"/>
-      <c r="G60" s="1"/>
-      <c r="H60" s="1"/>
-      <c r="I60" s="1"/>
-      <c r="J60" s="1"/>
-      <c r="K60" s="1"/>
-      <c r="L60" s="1"/>
-      <c r="M60" s="1"/>
-      <c r="N60" s="1"/>
-      <c r="O60" s="1"/>
-      <c r="P60" s="1"/>
-    </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A61" s="1"/>
-      <c r="B61" s="1"/>
-      <c r="C61" s="1"/>
-      <c r="D61" s="1"/>
-      <c r="E61" s="1"/>
-      <c r="F61" s="1"/>
-      <c r="G61" s="1"/>
-      <c r="H61" s="1"/>
-      <c r="I61" s="1"/>
-      <c r="J61" s="1"/>
-      <c r="K61" s="1"/>
-      <c r="L61" s="1"/>
-      <c r="M61" s="1"/>
-      <c r="N61" s="1"/>
-      <c r="O61" s="1"/>
-      <c r="P61" s="1"/>
-    </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A62" s="1"/>
-      <c r="B62" s="1"/>
-      <c r="C62" s="1"/>
-      <c r="D62" s="1"/>
-      <c r="E62" s="1"/>
-      <c r="F62" s="1"/>
-      <c r="G62" s="1"/>
-      <c r="H62" s="1"/>
-      <c r="I62" s="1"/>
-      <c r="J62" s="1"/>
-      <c r="K62" s="1"/>
-      <c r="L62" s="1"/>
-      <c r="M62" s="1"/>
-      <c r="N62" s="1"/>
-      <c r="O62" s="1"/>
-      <c r="P62" s="1"/>
-    </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A63" s="1"/>
-      <c r="B63" s="1"/>
-      <c r="C63" s="1"/>
-      <c r="D63" s="1"/>
-      <c r="E63" s="1"/>
-      <c r="F63" s="1"/>
-      <c r="G63" s="1"/>
-      <c r="H63" s="1"/>
-      <c r="I63" s="1"/>
-      <c r="J63" s="1"/>
-      <c r="K63" s="1"/>
-      <c r="L63" s="1"/>
-      <c r="M63" s="1"/>
-      <c r="N63" s="1"/>
-      <c r="O63" s="1"/>
-      <c r="P63" s="1"/>
-    </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A64" s="1"/>
-      <c r="B64" s="1"/>
-      <c r="C64" s="1"/>
-      <c r="D64" s="1"/>
-      <c r="E64" s="1"/>
-      <c r="F64" s="1"/>
-      <c r="G64" s="1"/>
-      <c r="H64" s="1"/>
-      <c r="I64" s="1"/>
-      <c r="J64" s="1"/>
-      <c r="K64" s="1"/>
-      <c r="L64" s="1"/>
-      <c r="M64" s="1"/>
-      <c r="N64" s="1"/>
-      <c r="O64" s="1"/>
-      <c r="P64" s="1"/>
-    </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A65" s="1"/>
-      <c r="B65" s="1"/>
-      <c r="C65" s="1"/>
-      <c r="D65" s="1"/>
-      <c r="E65" s="1"/>
-      <c r="F65" s="1"/>
-      <c r="G65" s="1"/>
-      <c r="H65" s="1"/>
-      <c r="I65" s="1"/>
-      <c r="J65" s="1"/>
-      <c r="K65" s="1"/>
-      <c r="L65" s="1"/>
-      <c r="M65" s="1"/>
-      <c r="N65" s="1"/>
-      <c r="O65" s="1"/>
-      <c r="P65" s="1"/>
-    </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A66" s="1"/>
-      <c r="B66" s="1"/>
-      <c r="C66" s="1"/>
-      <c r="D66" s="1"/>
-      <c r="E66" s="1"/>
-      <c r="F66" s="1"/>
-      <c r="G66" s="1"/>
-      <c r="H66" s="1"/>
-      <c r="I66" s="1"/>
-      <c r="J66" s="1"/>
-      <c r="K66" s="1"/>
-      <c r="L66" s="1"/>
-      <c r="M66" s="1"/>
-      <c r="N66" s="1"/>
-      <c r="O66" s="1"/>
-      <c r="P66" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Simulações variando a Temperatura
</commit_message>
<xml_diff>
--- a/ExoCTK_results.xlsx
+++ b/ExoCTK_results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Meu Drive\StarsAndExoplanets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Meu Drive\StarsAndExoplanets\Exoplanets\GJ9827d\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D077C0A0-F24C-425A-ACCE-BC43B3AB015A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E46F3774-C416-49A6-A7CE-7CE3E9E29D1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{FD485E45-5400-4809-8075-6517CC8BF8A4}"/>
   </bookViews>
@@ -149,9 +149,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -470,7 +471,7 @@
   <dimension ref="A1:P66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W6" sqref="W6"/>
+      <selection activeCell="K70" sqref="K70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3476,302 +3477,302 @@
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A61" s="1">
-        <v>4340</v>
-      </c>
-      <c r="B61" s="1">
-        <v>4.66</v>
-      </c>
-      <c r="C61" s="1">
-        <v>-0.26</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E61" s="1" t="s">
+      <c r="A61" s="2">
+        <v>4340</v>
+      </c>
+      <c r="B61" s="2">
+        <v>4.66</v>
+      </c>
+      <c r="C61" s="2">
+        <v>-0.26</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E61" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F61" s="1">
+      <c r="F61" s="2">
         <v>1.9610000000000001</v>
       </c>
-      <c r="G61" s="1">
+      <c r="G61" s="2">
         <v>2.0979999999999999</v>
       </c>
-      <c r="H61" s="1">
+      <c r="H61" s="2">
         <v>2.2320000000000002</v>
       </c>
-      <c r="I61" s="1">
+      <c r="I61" s="2">
         <v>0.7</v>
       </c>
-      <c r="J61" s="1">
+      <c r="J61" s="2">
         <v>0.04</v>
       </c>
-      <c r="K61" s="1">
+      <c r="K61" s="2">
         <v>-5.8999999999999997E-2</v>
       </c>
-      <c r="L61" s="1">
+      <c r="L61" s="2">
         <v>9.4E-2</v>
       </c>
-      <c r="M61" s="1">
+      <c r="M61" s="2">
         <v>-0.20300000000000001</v>
       </c>
-      <c r="N61" s="1">
+      <c r="N61" s="2">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="O61" s="1">
+      <c r="O61" s="2">
         <v>0.104</v>
       </c>
-      <c r="P61" s="1">
+      <c r="P61" s="2">
         <v>3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A62" s="1">
-        <v>4340</v>
-      </c>
-      <c r="B62" s="1">
-        <v>4.66</v>
-      </c>
-      <c r="C62" s="1">
-        <v>-0.26</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E62" s="1" t="s">
+      <c r="A62" s="2">
+        <v>4340</v>
+      </c>
+      <c r="B62" s="2">
+        <v>4.66</v>
+      </c>
+      <c r="C62" s="2">
+        <v>-0.26</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E62" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F62" s="1">
+      <c r="F62" s="2">
         <v>2.879</v>
       </c>
-      <c r="G62" s="1">
+      <c r="G62" s="2">
         <v>2.9380000000000002</v>
       </c>
-      <c r="H62" s="1">
+      <c r="H62" s="2">
         <v>2.9980000000000002</v>
       </c>
-      <c r="I62" s="1">
+      <c r="I62" s="2">
         <v>0.51300000000000001</v>
       </c>
-      <c r="J62" s="1">
+      <c r="J62" s="2">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="K62" s="1">
+      <c r="K62" s="2">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="L62" s="1">
+      <c r="L62" s="2">
         <v>9.7000000000000003E-2</v>
       </c>
-      <c r="M62" s="1">
+      <c r="M62" s="2">
         <v>-0.18099999999999999</v>
       </c>
-      <c r="N62" s="1">
+      <c r="N62" s="2">
         <v>9.7000000000000003E-2</v>
       </c>
-      <c r="O62" s="1">
+      <c r="O62" s="2">
         <v>8.7999999999999995E-2</v>
       </c>
-      <c r="P62" s="1">
+      <c r="P62" s="2">
         <v>3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A63" s="1">
-        <v>4340</v>
-      </c>
-      <c r="B63" s="1">
-        <v>4.66</v>
-      </c>
-      <c r="C63" s="1">
-        <v>-0.26</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E63" s="1" t="s">
+      <c r="A63" s="2">
+        <v>4340</v>
+      </c>
+      <c r="B63" s="2">
+        <v>4.66</v>
+      </c>
+      <c r="C63" s="2">
+        <v>-0.26</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E63" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F63" s="1">
+      <c r="F63" s="2">
         <v>3.0019999999999998</v>
       </c>
-      <c r="G63" s="1">
+      <c r="G63" s="2">
         <v>3.06</v>
       </c>
-      <c r="H63" s="1">
+      <c r="H63" s="2">
         <v>3.121</v>
       </c>
-      <c r="I63" s="1">
+      <c r="I63" s="2">
         <v>0.48299999999999998</v>
       </c>
-      <c r="J63" s="1">
+      <c r="J63" s="2">
         <v>4.7E-2</v>
       </c>
-      <c r="K63" s="1">
+      <c r="K63" s="2">
         <v>4.5999999999999999E-2</v>
       </c>
-      <c r="L63" s="1">
+      <c r="L63" s="2">
         <v>0.111</v>
       </c>
-      <c r="M63" s="1">
+      <c r="M63" s="2">
         <v>-0.222</v>
       </c>
-      <c r="N63" s="1">
+      <c r="N63" s="2">
         <v>0.112</v>
       </c>
-      <c r="O63" s="1">
+      <c r="O63" s="2">
         <v>0.105</v>
       </c>
-      <c r="P63" s="1">
+      <c r="P63" s="2">
         <v>4.1000000000000002E-2</v>
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A64" s="1">
-        <v>4340</v>
-      </c>
-      <c r="B64" s="1">
-        <v>4.66</v>
-      </c>
-      <c r="C64" s="1">
-        <v>-0.26</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E64" s="1" t="s">
+      <c r="A64" s="2">
+        <v>4340</v>
+      </c>
+      <c r="B64" s="2">
+        <v>4.66</v>
+      </c>
+      <c r="C64" s="2">
+        <v>-0.26</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E64" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F64" s="1">
+      <c r="F64" s="2">
         <v>3.125</v>
       </c>
-      <c r="G64" s="1">
+      <c r="G64" s="2">
         <v>3.1840000000000002</v>
       </c>
-      <c r="H64" s="1">
+      <c r="H64" s="2">
         <v>3.2440000000000002</v>
       </c>
-      <c r="I64" s="1">
+      <c r="I64" s="2">
         <v>0.47199999999999998</v>
       </c>
-      <c r="J64" s="1">
+      <c r="J64" s="2">
         <v>4.5999999999999999E-2</v>
       </c>
-      <c r="K64" s="1">
+      <c r="K64" s="2">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="L64" s="1">
+      <c r="L64" s="2">
         <v>0.109</v>
       </c>
-      <c r="M64" s="1">
+      <c r="M64" s="2">
         <v>-0.20200000000000001</v>
       </c>
-      <c r="N64" s="1">
+      <c r="N64" s="2">
         <v>0.11</v>
       </c>
-      <c r="O64" s="1">
+      <c r="O64" s="2">
         <v>9.7000000000000003E-2</v>
       </c>
-      <c r="P64" s="1">
+      <c r="P64" s="2">
         <v>0.04</v>
       </c>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A65" s="1">
-        <v>4340</v>
-      </c>
-      <c r="B65" s="1">
-        <v>4.66</v>
-      </c>
-      <c r="C65" s="1">
-        <v>-0.26</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E65" s="1" t="s">
+      <c r="A65" s="2">
+        <v>4340</v>
+      </c>
+      <c r="B65" s="2">
+        <v>4.66</v>
+      </c>
+      <c r="C65" s="2">
+        <v>-0.26</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E65" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F65" s="1">
+      <c r="F65" s="2">
         <v>3.2480000000000002</v>
       </c>
-      <c r="G65" s="1">
+      <c r="G65" s="2">
         <v>3.3069999999999999</v>
       </c>
-      <c r="H65" s="1">
+      <c r="H65" s="2">
         <v>3.367</v>
       </c>
-      <c r="I65" s="1">
+      <c r="I65" s="2">
         <v>0.47</v>
       </c>
-      <c r="J65" s="1">
+      <c r="J65" s="2">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="K65" s="1">
+      <c r="K65" s="2">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="L65" s="1">
+      <c r="L65" s="2">
         <v>0.10100000000000001</v>
       </c>
-      <c r="M65" s="1">
+      <c r="M65" s="2">
         <v>-0.16800000000000001</v>
       </c>
-      <c r="N65" s="1">
+      <c r="N65" s="2">
         <v>0.10199999999999999</v>
       </c>
-      <c r="O65" s="1">
+      <c r="O65" s="2">
         <v>8.4000000000000005E-2</v>
       </c>
-      <c r="P65" s="1">
+      <c r="P65" s="2">
         <v>3.6999999999999998E-2</v>
       </c>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A66" s="1">
-        <v>4340</v>
-      </c>
-      <c r="B66" s="1">
-        <v>4.66</v>
-      </c>
-      <c r="C66" s="1">
-        <v>-0.26</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E66" s="1" t="s">
+      <c r="A66" s="2">
+        <v>4340</v>
+      </c>
+      <c r="B66" s="2">
+        <v>4.66</v>
+      </c>
+      <c r="C66" s="2">
+        <v>-0.26</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E66" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F66" s="1">
+      <c r="F66" s="2">
         <v>3.371</v>
       </c>
-      <c r="G66" s="1">
+      <c r="G66" s="2">
         <v>3.43</v>
       </c>
-      <c r="H66" s="1">
+      <c r="H66" s="2">
         <v>3.49</v>
       </c>
-      <c r="I66" s="1">
+      <c r="I66" s="2">
         <v>0.442</v>
       </c>
-      <c r="J66" s="1">
+      <c r="J66" s="2">
         <v>4.5999999999999999E-2</v>
       </c>
-      <c r="K66" s="1">
+      <c r="K66" s="2">
         <v>0.04</v>
       </c>
-      <c r="L66" s="1">
+      <c r="L66" s="2">
         <v>0.11</v>
       </c>
-      <c r="M66" s="1">
+      <c r="M66" s="2">
         <v>-0.20100000000000001</v>
       </c>
-      <c r="N66" s="1">
+      <c r="N66" s="2">
         <v>0.11</v>
       </c>
-      <c r="O66" s="1">
+      <c r="O66" s="2">
         <v>9.7000000000000003E-2</v>
       </c>
-      <c r="P66" s="1">
+      <c r="P66" s="2">
         <v>0.04</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Simulações para epsilon Rackham
</commit_message>
<xml_diff>
--- a/ExoCTK_results.xlsx
+++ b/ExoCTK_results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\StarsAndExoplanets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Meu Drive\StarsAndExoplanets\Exoplanets\GJ9827d\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49BB163D-D51A-4804-9B0D-DC7B52B87F3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E46F3774-C416-49A6-A7CE-7CE3E9E29D1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FD485E45-5400-4809-8075-6517CC8BF8A4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{FD485E45-5400-4809-8075-6517CC8BF8A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,17 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -160,9 +149,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,12 +471,12 @@
   <dimension ref="A1:P66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q4" sqref="A4:Q66"/>
+      <selection activeCell="K70" sqref="K70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -536,7 +526,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
@@ -586,7 +576,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>4340</v>
       </c>
@@ -636,7 +626,7 @@
         <v>2.3E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>4340</v>
       </c>
@@ -686,7 +676,7 @@
         <v>5.3999999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4340</v>
       </c>
@@ -736,7 +726,7 @@
         <v>4.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4340</v>
       </c>
@@ -786,7 +776,7 @@
         <v>3.1E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4340</v>
       </c>
@@ -836,7 +826,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>4340</v>
       </c>
@@ -886,7 +876,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>4340</v>
       </c>
@@ -936,7 +926,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>4340</v>
       </c>
@@ -986,7 +976,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>4340</v>
       </c>
@@ -1036,7 +1026,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>4340</v>
       </c>
@@ -1086,7 +1076,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>4340</v>
       </c>
@@ -1136,7 +1126,7 @@
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>4340</v>
       </c>
@@ -1186,7 +1176,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>4340</v>
       </c>
@@ -1236,7 +1226,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>4340</v>
       </c>
@@ -1286,7 +1276,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>4340</v>
       </c>
@@ -1336,7 +1326,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>4340</v>
       </c>
@@ -1386,7 +1376,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>4340</v>
       </c>
@@ -1436,7 +1426,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>4340</v>
       </c>
@@ -1486,7 +1476,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>4340</v>
       </c>
@@ -1536,7 +1526,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>4340</v>
       </c>
@@ -1586,7 +1576,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>4340</v>
       </c>
@@ -1636,7 +1626,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>4340</v>
       </c>
@@ -1686,7 +1676,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>4340</v>
       </c>
@@ -1736,7 +1726,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>4340</v>
       </c>
@@ -1786,7 +1776,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>4340</v>
       </c>
@@ -1836,7 +1826,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>4340</v>
       </c>
@@ -1886,7 +1876,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>4340</v>
       </c>
@@ -1936,7 +1926,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>4340</v>
       </c>
@@ -1986,7 +1976,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>4340</v>
       </c>
@@ -2036,7 +2026,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>4340</v>
       </c>
@@ -2086,7 +2076,7 @@
         <v>1.9E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>4340</v>
       </c>
@@ -2136,7 +2126,7 @@
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>4340</v>
       </c>
@@ -2186,7 +2176,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>4340</v>
       </c>
@@ -2236,7 +2226,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>4340</v>
       </c>
@@ -2286,7 +2276,7 @@
         <v>3.2000000000000001E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>4340</v>
       </c>
@@ -2336,7 +2326,7 @@
         <v>2.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>4340</v>
       </c>
@@ -2386,7 +2376,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>4340</v>
       </c>
@@ -2436,7 +2426,7 @@
         <v>4.3999999999999997E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>4340</v>
       </c>
@@ -2486,7 +2476,7 @@
         <v>4.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>4340</v>
       </c>
@@ -2536,7 +2526,7 @@
         <v>3.6999999999999998E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>4340</v>
       </c>
@@ -2586,7 +2576,7 @@
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>4340</v>
       </c>
@@ -2636,7 +2626,7 @@
         <v>4.1000000000000002E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>4340</v>
       </c>
@@ -2686,7 +2676,7 @@
         <v>3.2000000000000001E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>4340</v>
       </c>
@@ -2736,7 +2726,7 @@
         <v>3.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>4340</v>
       </c>
@@ -2786,7 +2776,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>4340</v>
       </c>
@@ -2836,7 +2826,7 @@
         <v>4.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>4340</v>
       </c>
@@ -2886,7 +2876,7 @@
         <v>4.3999999999999997E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>4340</v>
       </c>
@@ -2936,7 +2926,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>4340</v>
       </c>
@@ -2986,7 +2976,7 @@
         <v>4.1000000000000002E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>4340</v>
       </c>
@@ -3036,7 +3026,7 @@
         <v>3.4000000000000002E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>4340</v>
       </c>
@@ -3086,7 +3076,7 @@
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>4340</v>
       </c>
@@ -3136,7 +3126,7 @@
         <v>2.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>4340</v>
       </c>
@@ -3186,7 +3176,7 @@
         <v>1.9E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>4340</v>
       </c>
@@ -3236,7 +3226,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>4340</v>
       </c>
@@ -3286,7 +3276,7 @@
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>4340</v>
       </c>
@@ -3336,7 +3326,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>4340</v>
       </c>
@@ -3386,7 +3376,7 @@
         <v>2.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>4340</v>
       </c>
@@ -3436,7 +3426,7 @@
         <v>2.1000000000000001E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>4340</v>
       </c>
@@ -3486,303 +3476,303 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A61" s="1">
-        <v>4340</v>
-      </c>
-      <c r="B61" s="1">
-        <v>4.66</v>
-      </c>
-      <c r="C61" s="1">
-        <v>-0.26</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E61" s="1" t="s">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A61" s="2">
+        <v>4340</v>
+      </c>
+      <c r="B61" s="2">
+        <v>4.66</v>
+      </c>
+      <c r="C61" s="2">
+        <v>-0.26</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E61" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F61" s="1">
+      <c r="F61" s="2">
         <v>1.9610000000000001</v>
       </c>
-      <c r="G61" s="1">
+      <c r="G61" s="2">
         <v>2.0979999999999999</v>
       </c>
-      <c r="H61" s="1">
+      <c r="H61" s="2">
         <v>2.2320000000000002</v>
       </c>
-      <c r="I61" s="1">
+      <c r="I61" s="2">
         <v>0.7</v>
       </c>
-      <c r="J61" s="1">
+      <c r="J61" s="2">
         <v>0.04</v>
       </c>
-      <c r="K61" s="1">
+      <c r="K61" s="2">
         <v>-5.8999999999999997E-2</v>
       </c>
-      <c r="L61" s="1">
+      <c r="L61" s="2">
         <v>9.4E-2</v>
       </c>
-      <c r="M61" s="1">
+      <c r="M61" s="2">
         <v>-0.20300000000000001</v>
       </c>
-      <c r="N61" s="1">
+      <c r="N61" s="2">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="O61" s="1">
+      <c r="O61" s="2">
         <v>0.104</v>
       </c>
-      <c r="P61" s="1">
+      <c r="P61" s="2">
         <v>3.5000000000000003E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A62" s="1">
-        <v>4340</v>
-      </c>
-      <c r="B62" s="1">
-        <v>4.66</v>
-      </c>
-      <c r="C62" s="1">
-        <v>-0.26</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E62" s="1" t="s">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A62" s="2">
+        <v>4340</v>
+      </c>
+      <c r="B62" s="2">
+        <v>4.66</v>
+      </c>
+      <c r="C62" s="2">
+        <v>-0.26</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E62" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F62" s="1">
+      <c r="F62" s="2">
         <v>2.879</v>
       </c>
-      <c r="G62" s="1">
+      <c r="G62" s="2">
         <v>2.9380000000000002</v>
       </c>
-      <c r="H62" s="1">
+      <c r="H62" s="2">
         <v>2.9980000000000002</v>
       </c>
-      <c r="I62" s="1">
+      <c r="I62" s="2">
         <v>0.51300000000000001</v>
       </c>
-      <c r="J62" s="1">
+      <c r="J62" s="2">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="K62" s="1">
+      <c r="K62" s="2">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="L62" s="1">
+      <c r="L62" s="2">
         <v>9.7000000000000003E-2</v>
       </c>
-      <c r="M62" s="1">
+      <c r="M62" s="2">
         <v>-0.18099999999999999</v>
       </c>
-      <c r="N62" s="1">
+      <c r="N62" s="2">
         <v>9.7000000000000003E-2</v>
       </c>
-      <c r="O62" s="1">
+      <c r="O62" s="2">
         <v>8.7999999999999995E-2</v>
       </c>
-      <c r="P62" s="1">
+      <c r="P62" s="2">
         <v>3.5000000000000003E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A63" s="1">
-        <v>4340</v>
-      </c>
-      <c r="B63" s="1">
-        <v>4.66</v>
-      </c>
-      <c r="C63" s="1">
-        <v>-0.26</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E63" s="1" t="s">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A63" s="2">
+        <v>4340</v>
+      </c>
+      <c r="B63" s="2">
+        <v>4.66</v>
+      </c>
+      <c r="C63" s="2">
+        <v>-0.26</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E63" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F63" s="1">
+      <c r="F63" s="2">
         <v>3.0019999999999998</v>
       </c>
-      <c r="G63" s="1">
+      <c r="G63" s="2">
         <v>3.06</v>
       </c>
-      <c r="H63" s="1">
+      <c r="H63" s="2">
         <v>3.121</v>
       </c>
-      <c r="I63" s="1">
+      <c r="I63" s="2">
         <v>0.48299999999999998</v>
       </c>
-      <c r="J63" s="1">
+      <c r="J63" s="2">
         <v>4.7E-2</v>
       </c>
-      <c r="K63" s="1">
+      <c r="K63" s="2">
         <v>4.5999999999999999E-2</v>
       </c>
-      <c r="L63" s="1">
+      <c r="L63" s="2">
         <v>0.111</v>
       </c>
-      <c r="M63" s="1">
+      <c r="M63" s="2">
         <v>-0.222</v>
       </c>
-      <c r="N63" s="1">
+      <c r="N63" s="2">
         <v>0.112</v>
       </c>
-      <c r="O63" s="1">
+      <c r="O63" s="2">
         <v>0.105</v>
       </c>
-      <c r="P63" s="1">
+      <c r="P63" s="2">
         <v>4.1000000000000002E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A64" s="1">
-        <v>4340</v>
-      </c>
-      <c r="B64" s="1">
-        <v>4.66</v>
-      </c>
-      <c r="C64" s="1">
-        <v>-0.26</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E64" s="1" t="s">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A64" s="2">
+        <v>4340</v>
+      </c>
+      <c r="B64" s="2">
+        <v>4.66</v>
+      </c>
+      <c r="C64" s="2">
+        <v>-0.26</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E64" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F64" s="1">
+      <c r="F64" s="2">
         <v>3.125</v>
       </c>
-      <c r="G64" s="1">
+      <c r="G64" s="2">
         <v>3.1840000000000002</v>
       </c>
-      <c r="H64" s="1">
+      <c r="H64" s="2">
         <v>3.2440000000000002</v>
       </c>
-      <c r="I64" s="1">
+      <c r="I64" s="2">
         <v>0.47199999999999998</v>
       </c>
-      <c r="J64" s="1">
+      <c r="J64" s="2">
         <v>4.5999999999999999E-2</v>
       </c>
-      <c r="K64" s="1">
+      <c r="K64" s="2">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="L64" s="1">
+      <c r="L64" s="2">
         <v>0.109</v>
       </c>
-      <c r="M64" s="1">
+      <c r="M64" s="2">
         <v>-0.20200000000000001</v>
       </c>
-      <c r="N64" s="1">
+      <c r="N64" s="2">
         <v>0.11</v>
       </c>
-      <c r="O64" s="1">
+      <c r="O64" s="2">
         <v>9.7000000000000003E-2</v>
       </c>
-      <c r="P64" s="1">
+      <c r="P64" s="2">
         <v>0.04</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A65" s="1">
-        <v>4340</v>
-      </c>
-      <c r="B65" s="1">
-        <v>4.66</v>
-      </c>
-      <c r="C65" s="1">
-        <v>-0.26</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E65" s="1" t="s">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A65" s="2">
+        <v>4340</v>
+      </c>
+      <c r="B65" s="2">
+        <v>4.66</v>
+      </c>
+      <c r="C65" s="2">
+        <v>-0.26</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E65" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F65" s="1">
+      <c r="F65" s="2">
         <v>3.2480000000000002</v>
       </c>
-      <c r="G65" s="1">
+      <c r="G65" s="2">
         <v>3.3069999999999999</v>
       </c>
-      <c r="H65" s="1">
+      <c r="H65" s="2">
         <v>3.367</v>
       </c>
-      <c r="I65" s="1">
+      <c r="I65" s="2">
         <v>0.47</v>
       </c>
-      <c r="J65" s="1">
+      <c r="J65" s="2">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="K65" s="1">
+      <c r="K65" s="2">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="L65" s="1">
+      <c r="L65" s="2">
         <v>0.10100000000000001</v>
       </c>
-      <c r="M65" s="1">
+      <c r="M65" s="2">
         <v>-0.16800000000000001</v>
       </c>
-      <c r="N65" s="1">
+      <c r="N65" s="2">
         <v>0.10199999999999999</v>
       </c>
-      <c r="O65" s="1">
+      <c r="O65" s="2">
         <v>8.4000000000000005E-2</v>
       </c>
-      <c r="P65" s="1">
+      <c r="P65" s="2">
         <v>3.6999999999999998E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A66" s="1">
-        <v>4340</v>
-      </c>
-      <c r="B66" s="1">
-        <v>4.66</v>
-      </c>
-      <c r="C66" s="1">
-        <v>-0.26</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E66" s="1" t="s">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A66" s="2">
+        <v>4340</v>
+      </c>
+      <c r="B66" s="2">
+        <v>4.66</v>
+      </c>
+      <c r="C66" s="2">
+        <v>-0.26</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E66" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F66" s="1">
+      <c r="F66" s="2">
         <v>3.371</v>
       </c>
-      <c r="G66" s="1">
+      <c r="G66" s="2">
         <v>3.43</v>
       </c>
-      <c r="H66" s="1">
+      <c r="H66" s="2">
         <v>3.49</v>
       </c>
-      <c r="I66" s="1">
+      <c r="I66" s="2">
         <v>0.442</v>
       </c>
-      <c r="J66" s="1">
+      <c r="J66" s="2">
         <v>4.5999999999999999E-2</v>
       </c>
-      <c r="K66" s="1">
+      <c r="K66" s="2">
         <v>0.04</v>
       </c>
-      <c r="L66" s="1">
+      <c r="L66" s="2">
         <v>0.11</v>
       </c>
-      <c r="M66" s="1">
+      <c r="M66" s="2">
         <v>-0.20100000000000001</v>
       </c>
-      <c r="N66" s="1">
+      <c r="N66" s="2">
         <v>0.11</v>
       </c>
-      <c r="O66" s="1">
+      <c r="O66" s="2">
         <v>9.7000000000000003E-2</v>
       </c>
-      <c r="P66" s="1">
+      <c r="P66" s="2">
         <v>0.04</v>
       </c>
     </row>

</xml_diff>